<commit_message>
extend max row and check if run_meet.time
</commit_message>
<xml_diff>
--- a/Copy of 06-23-24 to 06-29-24 Full Shedule.xlsx
+++ b/Copy of 06-23-24 to 06-29-24 Full Shedule.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y131"/>
+  <dimension ref="A1:Y119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -666,7 +666,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>5:30 AM MEET COLLEGE (SOUTHWEST)</t>
+          <t>M: 5:30 AM MEET COLLEGE (SOUTHWEST)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -674,7 +674,7 @@
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t>6:00 AM START</t>
+          <t>M: 6:00 AM START</t>
         </is>
       </c>
       <c r="K8" t="inlineStr"/>
@@ -682,7 +682,7 @@
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr">
         <is>
-          <t>6:00 AM START</t>
+          <t>IL: 4:15 AM MEET AT OFFICE</t>
         </is>
       </c>
       <c r="O8" t="inlineStr"/>
@@ -690,7 +690,7 @@
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr">
         <is>
-          <t>5:15 AM MEET OFFICE</t>
+          <t>M: 5:15 AM MEET OFFICE</t>
         </is>
       </c>
       <c r="S8" t="inlineStr"/>
@@ -698,7 +698,7 @@
       <c r="U8" t="inlineStr"/>
       <c r="V8" t="inlineStr">
         <is>
-          <t>6:00 AM START</t>
+          <t>IL: 4:15 MEET AT OFFICE</t>
         </is>
       </c>
       <c r="W8" t="inlineStr"/>
@@ -729,7 +729,7 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr">
         <is>
-          <t>DC5-ITEM LEVEL</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="O9" t="inlineStr"/>
@@ -745,7 +745,7 @@
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="W9" t="inlineStr"/>
@@ -776,7 +776,7 @@
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr">
         <is>
-          <t>PICK #348 +RX, OAK CREEK - 27TH ST</t>
+          <t>DC5-ITEM LEVEL</t>
         </is>
       </c>
       <c r="O10" t="inlineStr"/>
@@ -792,7 +792,7 @@
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr">
         <is>
-          <t>GOOD HARVEST MARKET, PEWAUKEE</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="W10" t="inlineStr"/>
@@ -823,7 +823,7 @@
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr">
         <is>
-          <t>6462 S 27TH ST</t>
+          <t>PICK #348 +RX, OAK CREEK - 27TH ST</t>
         </is>
       </c>
       <c r="O11" t="inlineStr"/>
@@ -839,7 +839,7 @@
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr">
         <is>
-          <t>2205 SILVERNAIL RD</t>
+          <t>GOOD HARVEST MARKET, PEWAUKEE</t>
         </is>
       </c>
       <c r="W11" t="inlineStr"/>
@@ -870,7 +870,7 @@
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/Ya5hSzVYqX42</t>
+          <t>6462 S 27TH ST</t>
         </is>
       </c>
       <c r="O12" t="inlineStr"/>
@@ -886,7 +886,7 @@
       <c r="U12" t="inlineStr"/>
       <c r="V12" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/dbog9UtxNWp</t>
+          <t>2205 SILVERNAIL RD</t>
         </is>
       </c>
       <c r="W12" t="inlineStr"/>
@@ -917,7 +917,7 @@
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr">
         <is>
-          <t>SET UP ON REG FAR RIGHT BY OFFICE</t>
+          <t>https://goo.gl/maps/Ya5hSzVYqX42</t>
         </is>
       </c>
       <c r="O13" t="inlineStr"/>
@@ -931,7 +931,11 @@
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/dbog9UtxNWp</t>
+        </is>
+      </c>
       <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
       <c r="Y13" t="inlineStr"/>
@@ -944,7 +948,8 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>SMALL CHANGES-RESET</t>
+          <t>SMALL CHANGES-RESET
+4:45 am meet for Carlie/Trevor at Grafton Park n Ride</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
@@ -956,7 +961,8 @@
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr">
         <is>
-          <t>5:15 am meet for Carlie/Trevor at Grafton Park n Ride</t>
+          <t xml:space="preserve">SET UP ON REG FAR RIGHT BY OFFICE
+5:15 am meet for Carlie/Trevor at Grafton Park n Ride	</t>
         </is>
       </c>
       <c r="O14" t="inlineStr"/>
@@ -969,21 +975,9 @@
       </c>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
-      <c r="V14" t="inlineStr">
-        <is>
-          <t>DJ</t>
-        </is>
-      </c>
-      <c r="W14" t="inlineStr">
-        <is>
-          <t>Equip</t>
-        </is>
-      </c>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
       <c r="X14" t="inlineStr"/>
       <c r="Y14" t="inlineStr"/>
     </row>
@@ -993,11 +987,7 @@
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>4:45 am meet for Carlie/Trevor at Grafton Park n Ride</t>
-        </is>
-      </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
@@ -1026,15 +1016,19 @@
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>1)</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>Aaron</t>
-        </is>
-      </c>
-      <c r="W15" t="inlineStr"/>
+          <t>DJ</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>Equip</t>
+        </is>
+      </c>
       <c r="X15" t="inlineStr"/>
       <c r="Y15" t="inlineStr"/>
     </row>
@@ -1043,9 +1037,22 @@
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Kim</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Driver,
+Red Van, Equip</t>
+        </is>
+      </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
@@ -1098,12 +1105,12 @@
       <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr">
         <is>
-          <t>3)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>Greg</t>
+          <t>Aaron</t>
         </is>
       </c>
       <c r="W16" t="inlineStr"/>
@@ -1117,18 +1124,18 @@
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Carlie</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Driver,
-Red Van, Equip</t>
+          <t>@ Store
+(w/ Trevor)</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
@@ -1184,12 +1191,12 @@
       <c r="T17" t="inlineStr"/>
       <c r="U17" t="inlineStr">
         <is>
-          <t>4)</t>
+          <t>3)</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>Jerry D</t>
+          <t>Greg</t>
         </is>
       </c>
       <c r="W17" t="inlineStr"/>
@@ -1203,20 +1210,15 @@
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>3)</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Carlie</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>@ Store
-(w/ Trevor)</t>
-        </is>
-      </c>
+          <t>Curt</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
         <is>
@@ -1261,12 +1263,12 @@
       <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr">
         <is>
-          <t>5)</t>
+          <t>4)</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>Sonia</t>
+          <t>Jerry D</t>
         </is>
       </c>
       <c r="W18" t="inlineStr"/>
@@ -1280,12 +1282,12 @@
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>3)</t>
+          <t>4)</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Curt</t>
+          <t>Cynthia</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
@@ -1328,19 +1330,15 @@
       <c r="T19" t="inlineStr"/>
       <c r="U19" t="inlineStr">
         <is>
-          <t>6)</t>
+          <t>5)</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>Ashley P</t>
-        </is>
-      </c>
-      <c r="W19" t="inlineStr">
-        <is>
-          <t>@ Store</t>
-        </is>
-      </c>
+          <t>Sonia</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr"/>
       <c r="X19" t="inlineStr"/>
       <c r="Y19" t="inlineStr"/>
     </row>
@@ -1351,12 +1349,12 @@
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
-          <t>4)</t>
+          <t>5)</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Cynthia</t>
+          <t>Greg</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
@@ -1404,17 +1402,18 @@
       <c r="T20" t="inlineStr"/>
       <c r="U20" t="inlineStr">
         <is>
-          <t>7)</t>
+          <t>6)</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>Evelin</t>
+          <t>Ashley P</t>
         </is>
       </c>
       <c r="W20" t="inlineStr">
         <is>
-          <t>@ Store</t>
+          <t>Driver, 1/2
+Silver Van</t>
         </is>
       </c>
       <c r="X20" t="inlineStr"/>
@@ -1427,12 +1426,12 @@
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
-          <t>5)</t>
+          <t>6)</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Greg</t>
+          <t>Robyn</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
@@ -1467,17 +1466,18 @@
       <c r="T21" t="inlineStr"/>
       <c r="U21" t="inlineStr">
         <is>
-          <t>8)</t>
+          <t>7)</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>Qiana</t>
+          <t>Evelin</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
         <is>
-          <t>@ Store</t>
+          <t>Driver, 1/2
+Silver Van</t>
         </is>
       </c>
       <c r="X21" t="inlineStr"/>
@@ -1490,12 +1490,12 @@
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>6)</t>
+          <t>7)</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Robyn</t>
+          <t>Sonia</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
@@ -1528,8 +1528,16 @@
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
-      <c r="U22" t="inlineStr"/>
-      <c r="V22" t="inlineStr"/>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>8)</t>
+        </is>
+      </c>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>Qiana</t>
+        </is>
+      </c>
       <c r="W22" t="inlineStr"/>
       <c r="X22" t="inlineStr"/>
       <c r="Y22" t="inlineStr"/>
@@ -1541,15 +1549,20 @@
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>7)</t>
+          <t>8)</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Sonia</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr"/>
+          <t>Trevor</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>@ Store
+(w/ Carlie)</t>
+        </is>
+      </c>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr">
         <is>
@@ -1578,7 +1591,7 @@
       <c r="Q23" t="inlineStr"/>
       <c r="R23" t="inlineStr">
         <is>
-          <t>5:00 AM MEET OFFICE</t>
+          <t>M: 5:00 AM MEET OFFICE</t>
         </is>
       </c>
       <c r="S23" t="inlineStr"/>
@@ -1594,22 +1607,9 @@
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>8)</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Trevor</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>@ Store
-(w/ Carlie)</t>
-        </is>
-      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr">
         <is>
@@ -1649,11 +1649,7 @@
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
       <c r="U24" t="inlineStr"/>
-      <c r="V24" t="inlineStr">
-        <is>
-          <t>5:30 AM OFFICE LEAVE TIME</t>
-        </is>
-      </c>
+      <c r="V24" t="inlineStr"/>
       <c r="W24" t="inlineStr"/>
       <c r="X24" t="inlineStr"/>
       <c r="Y24" t="inlineStr"/>
@@ -1694,7 +1690,7 @@
       <c r="U25" t="inlineStr"/>
       <c r="V25" t="inlineStr">
         <is>
-          <t>6:00 AM START</t>
+          <t>M: 5:30 AM OFFICE LEAVE TIME</t>
         </is>
       </c>
       <c r="W25" t="inlineStr"/>
@@ -1707,7 +1703,11 @@
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>M: 5:30 AM MEET WATERTOWN PLANK</t>
+        </is>
+      </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr"/>
@@ -1742,7 +1742,7 @@
       <c r="U26" t="inlineStr"/>
       <c r="V26" t="inlineStr">
         <is>
-          <t>DC5-ITEM LEVEL</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="W26" t="inlineStr"/>
@@ -1757,7 +1757,7 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>5:30 AM MEET WATERTOWN PLANK</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
@@ -1765,7 +1765,7 @@
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr">
         <is>
-          <t>6:30 AM MEET SOUTH RACINE COURT (HWY 43 &amp; Y)</t>
+          <t>M: 6:30 AM MEET SOUTH RACINE COURT (HWY 43 &amp; Y)</t>
         </is>
       </c>
       <c r="K27" t="inlineStr"/>
@@ -1782,7 +1782,8 @@
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>@ Store,
+          <t>Driver, 1/2
+Silver Van,
 Rx</t>
         </is>
       </c>
@@ -1798,7 +1799,7 @@
       <c r="U27" t="inlineStr"/>
       <c r="V27" t="inlineStr">
         <is>
-          <t>DHILLON'S MOBIL, COLGATE</t>
+          <t>DC5-ITEM LEVEL</t>
         </is>
       </c>
       <c r="W27" t="inlineStr"/>
@@ -1813,7 +1814,7 @@
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>6:00 AM START</t>
+          <t>EXCEL FINANCIAL</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
@@ -1836,11 +1837,7 @@
           <t>Anisha</t>
         </is>
       </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>@ Store</t>
-        </is>
-      </c>
+      <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
       <c r="R28" t="inlineStr">
@@ -1853,7 +1850,7 @@
       <c r="U28" t="inlineStr"/>
       <c r="V28" t="inlineStr">
         <is>
-          <t>4522 HWY Q</t>
+          <t>DHILLON'S MOBIL, COLGATE</t>
         </is>
       </c>
       <c r="W28" t="inlineStr"/>
@@ -1868,7 +1865,7 @@
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>EXCEL FINANCIAL</t>
+          <t>KOHN'S FILLING STATION, KEWASKUM</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
@@ -1891,11 +1888,7 @@
           <t>Brianna</t>
         </is>
       </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>@ Store</t>
-        </is>
-      </c>
+      <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="inlineStr"/>
@@ -1904,7 +1897,7 @@
       <c r="U29" t="inlineStr"/>
       <c r="V29" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/4Gd7nmyouVsSpUj2A</t>
+          <t>4522 HWY Q</t>
         </is>
       </c>
       <c r="W29" t="inlineStr"/>
@@ -1919,7 +1912,7 @@
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>KOHN'S FILLING STATION, KEWASKUM</t>
+          <t>890 FOND DU LAC AVE</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
@@ -1944,7 +1937,8 @@
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>@ Store</t>
+          <t>Driver, 1/2
+Silver Van</t>
         </is>
       </c>
       <c r="P30" t="inlineStr"/>
@@ -1965,7 +1959,11 @@
       </c>
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr"/>
-      <c r="V30" t="inlineStr"/>
+      <c r="V30" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/4Gd7nmyouVsSpUj2A</t>
+        </is>
+      </c>
       <c r="W30" t="inlineStr"/>
       <c r="X30" t="inlineStr"/>
       <c r="Y30" t="inlineStr"/>
@@ -1978,7 +1976,7 @@
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>890 FOND DU LAC AVE</t>
+          <t>https://goo.gl/maps/CJnRNDyortw</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
@@ -2001,11 +1999,7 @@
           <t>Joseph</t>
         </is>
       </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>@ Store</t>
-        </is>
-      </c>
+      <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr"/>
       <c r="Q31" t="inlineStr">
         <is>
@@ -2019,21 +2013,9 @@
       </c>
       <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr"/>
-      <c r="U31" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
-      <c r="V31" t="inlineStr">
-        <is>
-          <t>Nate</t>
-        </is>
-      </c>
-      <c r="W31" t="inlineStr">
-        <is>
-          <t>@ Store</t>
-        </is>
-      </c>
+      <c r="U31" t="inlineStr"/>
+      <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr"/>
       <c r="X31" t="inlineStr"/>
       <c r="Y31" t="inlineStr"/>
     </row>
@@ -2045,7 +2027,7 @@
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/CJnRNDyortw</t>
+          <t>TO FOLLOW</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
@@ -2068,11 +2050,7 @@
           <t>Justin</t>
         </is>
       </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>@ Store</t>
-        </is>
-      </c>
+      <c r="O32" t="inlineStr"/>
       <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr">
         <is>
@@ -2093,18 +2071,17 @@
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>1)</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Nate</t>
         </is>
       </c>
       <c r="W32" t="inlineStr">
         <is>
-          <t>Sante Fe,
-Until 11:30</t>
+          <t>@ Store</t>
         </is>
       </c>
       <c r="X32" t="inlineStr"/>
@@ -2118,7 +2095,7 @@
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>TO FOLLOW</t>
+          <t>EXCEL FINANCIAL</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
@@ -2143,7 +2120,8 @@
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>@ Store</t>
+          <t>Driver, 1/2
+Gray Van</t>
         </is>
       </c>
       <c r="P33" t="inlineStr"/>
@@ -2157,25 +2135,22 @@
           <t>Lori</t>
         </is>
       </c>
-      <c r="S33" t="inlineStr">
-        <is>
-          <t>@ Store</t>
-        </is>
-      </c>
+      <c r="S33" t="inlineStr"/>
       <c r="T33" t="inlineStr"/>
       <c r="U33" t="inlineStr">
         <is>
-          <t>3)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>Lori</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="W33" t="inlineStr">
         <is>
-          <t>@ Store</t>
+          <t>Sante Fe,
+Until 11:30</t>
         </is>
       </c>
       <c r="X33" t="inlineStr"/>
@@ -2189,7 +2164,7 @@
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>EXCEL FINANCIAL</t>
+          <t>KOHN'S FILLING STATION 259, CAMPBELLSPORT</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
@@ -2210,7 +2185,8 @@
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>@ Store,
+          <t>Driver, 1/2
+Gray Van,
 Supv Rx</t>
         </is>
       </c>
@@ -2219,8 +2195,16 @@
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr"/>
       <c r="T34" t="inlineStr"/>
-      <c r="U34" t="inlineStr"/>
-      <c r="V34" t="inlineStr"/>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>3)</t>
+        </is>
+      </c>
+      <c r="V34" t="inlineStr">
+        <is>
+          <t>Lori</t>
+        </is>
+      </c>
       <c r="W34" t="inlineStr"/>
       <c r="X34" t="inlineStr"/>
       <c r="Y34" t="inlineStr"/>
@@ -2233,7 +2217,7 @@
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>KOHN'S FILLING STATION 259, CAMPBELLSPORT</t>
+          <t>259 N FOND DU LAC AVE</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
@@ -2265,11 +2249,7 @@
           <t>Taylor</t>
         </is>
       </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>@ Store</t>
-        </is>
-      </c>
+      <c r="O35" t="inlineStr"/>
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="inlineStr"/>
@@ -2289,7 +2269,7 @@
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
-          <t>259 N FOND DU LAC AVE</t>
+          <t>https://goo.gl/maps/WCsZpx5SMsA2</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
@@ -2313,17 +2293,13 @@
       <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr">
         <is>
-          <t>5:15 AM MEET OFFICE</t>
+          <t>M: 5:15 AM MEET OFFICE</t>
         </is>
       </c>
       <c r="S36" t="inlineStr"/>
       <c r="T36" t="inlineStr"/>
       <c r="U36" t="inlineStr"/>
-      <c r="V36" t="inlineStr">
-        <is>
-          <t>5:00 AM MEET WATERTOWN PLANK</t>
-        </is>
-      </c>
+      <c r="V36" t="inlineStr"/>
       <c r="W36" t="inlineStr"/>
       <c r="X36" t="inlineStr"/>
       <c r="Y36" t="inlineStr"/>
@@ -2334,11 +2310,7 @@
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>https://goo.gl/maps/WCsZpx5SMsA2</t>
-        </is>
-      </c>
+      <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr">
@@ -2368,7 +2340,7 @@
       <c r="U37" t="inlineStr"/>
       <c r="V37" t="inlineStr">
         <is>
-          <t>6:00 AM START</t>
+          <t>M: 5:00 AM MEET WATERTOWN PLANK</t>
         </is>
       </c>
       <c r="W37" t="inlineStr"/>
@@ -2380,9 +2352,22 @@
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Ian</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Driver,
+Sante Fe, Equip</t>
+        </is>
+      </c>
       <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr"/>
@@ -2407,7 +2392,7 @@
       <c r="U38" t="inlineStr"/>
       <c r="V38" t="inlineStr">
         <is>
-          <t>DC5-ITEM LEVEL</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="W38" t="inlineStr"/>
@@ -2421,20 +2406,15 @@
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr">
         <is>
-          <t>1)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Ian</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>Driver,
-Sante Fe, Equip</t>
-        </is>
-      </c>
+          <t>Paul</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr"/>
@@ -2459,7 +2439,7 @@
       <c r="U39" t="inlineStr"/>
       <c r="V39" t="inlineStr">
         <is>
-          <t>DHILLON'S BP, FOND DU LAC - JOHNSON</t>
+          <t>DC5-ITEM LEVEL</t>
         </is>
       </c>
       <c r="W39" t="inlineStr"/>
@@ -2471,22 +2451,14 @@
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>2)</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>Paul</t>
-        </is>
-      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr">
         <is>
-          <t>6:30 AM MEET OFFICE</t>
+          <t>M: 6:30 AM MEET OFFICE</t>
         </is>
       </c>
       <c r="K40" t="inlineStr"/>
@@ -2510,7 +2482,7 @@
       <c r="U40" t="inlineStr"/>
       <c r="V40" t="inlineStr">
         <is>
-          <t>919 E JOHNSON ST</t>
+          <t>DHILLON'S BP, FOND DU LAC - JOHNSON</t>
         </is>
       </c>
       <c r="W40" t="inlineStr"/>
@@ -2553,7 +2525,7 @@
       <c r="U41" t="inlineStr"/>
       <c r="V41" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/K1uY65NKN1wdvR36A</t>
+          <t>919 E JOHNSON ST</t>
         </is>
       </c>
       <c r="W41" t="inlineStr"/>
@@ -2565,8 +2537,16 @@
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr"/>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>M: 5:00 AM MEET AT THE OFFICE</t>
+        </is>
+      </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr"/>
@@ -2590,7 +2570,11 @@
       <c r="S42" t="inlineStr"/>
       <c r="T42" t="inlineStr"/>
       <c r="U42" t="inlineStr"/>
-      <c r="V42" t="inlineStr"/>
+      <c r="V42" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/K1uY65NKN1wdvR36A</t>
+        </is>
+      </c>
       <c r="W42" t="inlineStr"/>
       <c r="X42" t="inlineStr"/>
       <c r="Y42" t="inlineStr"/>
@@ -2607,7 +2591,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>5:00 AM MEET AT THE OFFICE</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
@@ -2645,22 +2629,9 @@
         </is>
       </c>
       <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
-      <c r="V43" t="inlineStr">
-        <is>
-          <t>Lashaun</t>
-        </is>
-      </c>
-      <c r="W43" t="inlineStr">
-        <is>
-          <t>Driver,
-Gold Camry, Equip</t>
-        </is>
-      </c>
+      <c r="U43" t="inlineStr"/>
+      <c r="V43" t="inlineStr"/>
+      <c r="W43" t="inlineStr"/>
       <c r="X43" t="inlineStr"/>
       <c r="Y43" t="inlineStr"/>
     </row>
@@ -2669,14 +2640,10 @@
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
+      <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
-          <t>6:00 AM START</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
@@ -2711,17 +2678,18 @@
       <c r="T44" t="inlineStr"/>
       <c r="U44" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>1)</t>
         </is>
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>Carlie</t>
+          <t>Lashaun</t>
         </is>
       </c>
       <c r="W44" t="inlineStr">
         <is>
-          <t>@ Store</t>
+          <t>Driver,
+Gold Camry, Equip</t>
         </is>
       </c>
       <c r="X44" t="inlineStr"/>
@@ -2735,7 +2703,7 @@
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>ROTE OIL #03 TWIN LAKES</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
@@ -2770,15 +2738,19 @@
       <c r="T45" t="inlineStr"/>
       <c r="U45" t="inlineStr">
         <is>
-          <t>3)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t>Casey</t>
-        </is>
-      </c>
-      <c r="W45" t="inlineStr"/>
+          <t>Carlie</t>
+        </is>
+      </c>
+      <c r="W45" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
       <c r="X45" t="inlineStr"/>
       <c r="Y45" t="inlineStr"/>
     </row>
@@ -2790,7 +2762,7 @@
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
-          <t>ROTE OIL #03 TWIN LAKES</t>
+          <t>475 N LAKE AVE</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
@@ -2825,12 +2797,12 @@
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr">
         <is>
-          <t>4)</t>
+          <t>3)</t>
         </is>
       </c>
       <c r="V46" t="inlineStr">
         <is>
-          <t>Stephanie</t>
+          <t>Casey</t>
         </is>
       </c>
       <c r="W46" t="inlineStr"/>
@@ -2845,7 +2817,7 @@
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
-          <t>475 N LAKE AVE</t>
+          <t>https://goo.gl/maps/jNgJR8hii6jJGZQP7</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
@@ -2870,8 +2842,16 @@
       <c r="R47" t="inlineStr"/>
       <c r="S47" t="inlineStr"/>
       <c r="T47" t="inlineStr"/>
-      <c r="U47" t="inlineStr"/>
-      <c r="V47" t="inlineStr"/>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>4)</t>
+        </is>
+      </c>
+      <c r="V47" t="inlineStr">
+        <is>
+          <t>Stephanie</t>
+        </is>
+      </c>
       <c r="W47" t="inlineStr"/>
       <c r="X47" t="inlineStr"/>
       <c r="Y47" t="inlineStr"/>
@@ -2884,7 +2864,7 @@
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/jNgJR8hii6jJGZQP7</t>
+          <t xml:space="preserve">TO FOLLOW   </t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
@@ -2923,7 +2903,7 @@
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr">
         <is>
-          <t xml:space="preserve">TO FOLLOW   </t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
@@ -2947,17 +2927,13 @@
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="inlineStr">
         <is>
-          <t>5:00 AM MEET AT OFFICE</t>
+          <t>M: 5:00 AM MEET AT OFFICE</t>
         </is>
       </c>
       <c r="S49" t="inlineStr"/>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr"/>
-      <c r="V49" t="inlineStr">
-        <is>
-          <t>6:00 AM START</t>
-        </is>
-      </c>
+      <c r="V49" t="inlineStr"/>
       <c r="W49" t="inlineStr"/>
       <c r="X49" t="inlineStr"/>
       <c r="Y49" t="inlineStr"/>
@@ -2970,7 +2946,7 @@
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>ROTE OIL #04 GENOA CITY</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
@@ -3002,7 +2978,7 @@
       <c r="U50" t="inlineStr"/>
       <c r="V50" t="inlineStr">
         <is>
-          <t>DC5-ITEM LEVEL</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="W50" t="inlineStr"/>
@@ -3017,7 +2993,7 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>ROTE OIL #04 GENOA CITY</t>
+          <t xml:space="preserve">100 ELIZABETH LANE    </t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
@@ -3045,7 +3021,7 @@
       <c r="U51" t="inlineStr"/>
       <c r="V51" t="inlineStr">
         <is>
-          <t>SERVE YOU PHARMACY, WAUWATOSA</t>
+          <t>DC5-ITEM LEVEL</t>
         </is>
       </c>
       <c r="W51" t="inlineStr"/>
@@ -3060,7 +3036,7 @@
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
-          <t xml:space="preserve">100 ELIZABETH LANE    </t>
+          <t>https://goo.gl/maps/DitGJzEvTVhJPxkJ8</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
@@ -3097,7 +3073,7 @@
       <c r="U52" t="inlineStr"/>
       <c r="V52" t="inlineStr">
         <is>
-          <t>10201 INNOVATION DR, SUIT 100</t>
+          <t>SERVE YOU PHARMACY, WAUWATOSA</t>
         </is>
       </c>
       <c r="W52" t="inlineStr"/>
@@ -3112,7 +3088,7 @@
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/DitGJzEvTVhJPxkJ8</t>
+          <t xml:space="preserve">TO FOLLOW   </t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
@@ -3156,7 +3132,7 @@
       <c r="U53" t="inlineStr"/>
       <c r="V53" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/KoXB6dUABdyxHvCT9</t>
+          <t>10201 INNOVATION DR, SUIT 100</t>
         </is>
       </c>
       <c r="W53" t="inlineStr"/>
@@ -3171,7 +3147,7 @@
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr">
         <is>
-          <t xml:space="preserve">TO FOLLOW   </t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="G54" t="inlineStr"/>
@@ -3201,7 +3177,11 @@
       <c r="S54" t="inlineStr"/>
       <c r="T54" t="inlineStr"/>
       <c r="U54" t="inlineStr"/>
-      <c r="V54" t="inlineStr"/>
+      <c r="V54" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/KoXB6dUABdyxHvCT9</t>
+        </is>
+      </c>
       <c r="W54" t="inlineStr"/>
       <c r="X54" t="inlineStr"/>
       <c r="Y54" t="inlineStr"/>
@@ -3214,7 +3194,7 @@
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>ROTE OIL #05  LAKE GENEVA</t>
         </is>
       </c>
       <c r="G55" t="inlineStr"/>
@@ -3235,21 +3215,9 @@
       </c>
       <c r="S55" t="inlineStr"/>
       <c r="T55" t="inlineStr"/>
-      <c r="U55" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
-      <c r="V55" t="inlineStr">
-        <is>
-          <t>Katherine</t>
-        </is>
-      </c>
-      <c r="W55" t="inlineStr">
-        <is>
-          <t>Optima available, Equip</t>
-        </is>
-      </c>
+      <c r="U55" t="inlineStr"/>
+      <c r="V55" t="inlineStr"/>
+      <c r="W55" t="inlineStr"/>
       <c r="X55" t="inlineStr"/>
       <c r="Y55" t="inlineStr"/>
     </row>
@@ -3261,7 +3229,7 @@
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
-          <t>ROTE OIL #05  LAKE GENEVA</t>
+          <t>300 PELLER RD</t>
         </is>
       </c>
       <c r="G56" t="inlineStr"/>
@@ -3288,15 +3256,19 @@
       <c r="T56" t="inlineStr"/>
       <c r="U56" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>1)</t>
         </is>
       </c>
       <c r="V56" t="inlineStr">
         <is>
-          <t>Cynthia</t>
-        </is>
-      </c>
-      <c r="W56" t="inlineStr"/>
+          <t>Katherine</t>
+        </is>
+      </c>
+      <c r="W56" t="inlineStr">
+        <is>
+          <t>Optima available, Equip</t>
+        </is>
+      </c>
       <c r="X56" t="inlineStr"/>
       <c r="Y56" t="inlineStr"/>
     </row>
@@ -3308,7 +3280,7 @@
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
-          <t>300 PELLER RD</t>
+          <t>https://goo.gl/maps/6fegzT1PbyY5VkDR6</t>
         </is>
       </c>
       <c r="G57" t="inlineStr"/>
@@ -3324,7 +3296,7 @@
       <c r="M57" t="inlineStr"/>
       <c r="N57" t="inlineStr">
         <is>
-          <t>Office</t>
+          <t>IL: 5:45 MEET AT OFFICE</t>
         </is>
       </c>
       <c r="O57" t="inlineStr"/>
@@ -3339,12 +3311,12 @@
       <c r="T57" t="inlineStr"/>
       <c r="U57" t="inlineStr">
         <is>
-          <t>3)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="V57" t="inlineStr">
         <is>
-          <t>Mai</t>
+          <t>Cynthia</t>
         </is>
       </c>
       <c r="W57" t="inlineStr"/>
@@ -3357,11 +3329,7 @@
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr"/>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>https://goo.gl/maps/6fegzT1PbyY5VkDR6</t>
-        </is>
-      </c>
+      <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr"/>
       <c r="I58" t="inlineStr"/>
@@ -3375,7 +3343,7 @@
       <c r="M58" t="inlineStr"/>
       <c r="N58" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>7:00 AM START</t>
         </is>
       </c>
       <c r="O58" t="inlineStr"/>
@@ -3390,12 +3358,12 @@
       <c r="T58" t="inlineStr"/>
       <c r="U58" t="inlineStr">
         <is>
-          <t>4)</t>
+          <t>3)</t>
         </is>
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t>Monica</t>
+          <t>Mai</t>
         </is>
       </c>
       <c r="W58" t="inlineStr"/>
@@ -3407,9 +3375,21 @@
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr"/>
-      <c r="F59" t="inlineStr"/>
-      <c r="G59" t="inlineStr"/>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Katherine</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Equip</t>
+        </is>
+      </c>
       <c r="H59" t="inlineStr"/>
       <c r="I59" t="inlineStr"/>
       <c r="J59" t="inlineStr">
@@ -3422,7 +3402,7 @@
       <c r="M59" t="inlineStr"/>
       <c r="N59" t="inlineStr">
         <is>
-          <t>Lashaun</t>
+          <t>DC5-ITEM LEVEL</t>
         </is>
       </c>
       <c r="O59" t="inlineStr"/>
@@ -3435,8 +3415,16 @@
       </c>
       <c r="S59" t="inlineStr"/>
       <c r="T59" t="inlineStr"/>
-      <c r="U59" t="inlineStr"/>
-      <c r="V59" t="inlineStr"/>
+      <c r="U59" t="inlineStr">
+        <is>
+          <t>4)</t>
+        </is>
+      </c>
+      <c r="V59" t="inlineStr">
+        <is>
+          <t>Monica</t>
+        </is>
+      </c>
       <c r="W59" t="inlineStr"/>
       <c r="X59" t="inlineStr"/>
       <c r="Y59" t="inlineStr"/>
@@ -3448,17 +3436,18 @@
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Katherine</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Equip</t>
+          <t>Driver,
+Optima</t>
         </is>
       </c>
       <c r="H60" t="inlineStr"/>
@@ -3471,7 +3460,11 @@
       <c r="K60" t="inlineStr"/>
       <c r="L60" t="inlineStr"/>
       <c r="M60" t="inlineStr"/>
-      <c r="N60" t="inlineStr"/>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>GROUP HEALTH RX, CAPITOL</t>
+        </is>
+      </c>
       <c r="O60" t="inlineStr"/>
       <c r="P60" t="inlineStr"/>
       <c r="Q60" t="inlineStr"/>
@@ -3489,22 +3482,9 @@
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>2)</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>Sue</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>Driver,
-Optima</t>
-        </is>
-      </c>
+      <c r="E61" t="inlineStr"/>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr"/>
       <c r="I61" t="inlineStr"/>
       <c r="J61" t="inlineStr">
@@ -3515,7 +3495,11 @@
       <c r="K61" t="inlineStr"/>
       <c r="L61" t="inlineStr"/>
       <c r="M61" t="inlineStr"/>
-      <c r="N61" t="inlineStr"/>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>675 W WASHINGTON AVE</t>
+        </is>
+      </c>
       <c r="O61" t="inlineStr"/>
       <c r="P61" t="inlineStr"/>
       <c r="Q61" t="inlineStr">
@@ -3535,11 +3519,7 @@
       </c>
       <c r="T61" t="inlineStr"/>
       <c r="U61" t="inlineStr"/>
-      <c r="V61" t="inlineStr">
-        <is>
-          <t>5:15 AM MEET COLLEGE (SOUTHWEST)</t>
-        </is>
-      </c>
+      <c r="V61" t="inlineStr"/>
       <c r="W61" t="inlineStr"/>
       <c r="X61" t="inlineStr"/>
       <c r="Y61" t="inlineStr"/>
@@ -3564,7 +3544,7 @@
       <c r="M62" t="inlineStr"/>
       <c r="N62" t="inlineStr">
         <is>
-          <t>7:00 AM START</t>
+          <t>https://goo.gl/maps/uSFXx2q34bs</t>
         </is>
       </c>
       <c r="O62" t="inlineStr"/>
@@ -3589,7 +3569,7 @@
       <c r="U62" t="inlineStr"/>
       <c r="V62" t="inlineStr">
         <is>
-          <t>6:00 AM START</t>
+          <t>M: 5:15 AM MEET COLLEGE (SOUTHWEST)</t>
         </is>
       </c>
       <c r="W62" t="inlineStr"/>
@@ -3602,7 +3582,11 @@
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr"/>
-      <c r="F63" t="inlineStr"/>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>M: 6:30 AM MEET OFFICE</t>
+        </is>
+      </c>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr"/>
@@ -3616,7 +3600,7 @@
       <c r="M63" t="inlineStr"/>
       <c r="N63" t="inlineStr">
         <is>
-          <t>DC5-ITEM LEVEL</t>
+          <t xml:space="preserve">TO FOLLOW   </t>
         </is>
       </c>
       <c r="O63" t="inlineStr"/>
@@ -3628,7 +3612,7 @@
       <c r="U63" t="inlineStr"/>
       <c r="V63" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="W63" t="inlineStr"/>
@@ -3643,7 +3627,7 @@
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr">
         <is>
-          <t>6:30 AM MEET OFFICE</t>
+          <t>7:00 AM START</t>
         </is>
       </c>
       <c r="G64" t="inlineStr"/>
@@ -3659,7 +3643,7 @@
       <c r="M64" t="inlineStr"/>
       <c r="N64" t="inlineStr">
         <is>
-          <t>GROUP HEALTH RX, CAPITOL</t>
+          <t>DC5-ITEM LEVEL</t>
         </is>
       </c>
       <c r="O64" t="inlineStr"/>
@@ -3671,7 +3655,7 @@
       <c r="U64" t="inlineStr"/>
       <c r="V64" t="inlineStr">
         <is>
-          <t>ROTE OIL #14 TREVOR (CITGO)</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="W64" t="inlineStr"/>
@@ -3686,7 +3670,7 @@
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr">
         <is>
-          <t>7:00 AM START</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="G65" t="inlineStr"/>
@@ -3702,7 +3686,7 @@
       <c r="M65" t="inlineStr"/>
       <c r="N65" t="inlineStr">
         <is>
-          <t>675 W WASHINGTON AVE</t>
+          <t>GROUP HEALTH RX, SAUK TRAILS</t>
         </is>
       </c>
       <c r="O65" t="inlineStr"/>
@@ -3710,7 +3694,8 @@
       <c r="Q65" t="inlineStr"/>
       <c r="R65" t="inlineStr">
         <is>
-          <t>4:30 AM OFFICE MEET</t>
+          <t>M: 4:30 AM OFFICE MEET
+IL: 4:30 AM MEET AT OFFICE</t>
         </is>
       </c>
       <c r="S65" t="inlineStr"/>
@@ -3718,7 +3703,7 @@
       <c r="U65" t="inlineStr"/>
       <c r="V65" t="inlineStr">
         <is>
-          <t>12617 ANTIOCH RD</t>
+          <t>ROTE OIL #14 TREVOR (CITGO)</t>
         </is>
       </c>
       <c r="W65" t="inlineStr"/>
@@ -3733,7 +3718,7 @@
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>GAUGERT'S BUSS STOP, SULLIVAN</t>
         </is>
       </c>
       <c r="G66" t="inlineStr"/>
@@ -3749,7 +3734,7 @@
       <c r="M66" t="inlineStr"/>
       <c r="N66" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/uSFXx2q34bs</t>
+          <t>8202 EXCELSIOR DR</t>
         </is>
       </c>
       <c r="O66" t="inlineStr"/>
@@ -3765,7 +3750,7 @@
       <c r="U66" t="inlineStr"/>
       <c r="V66" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/xA9YMzPGc6Vhxi5r8</t>
+          <t>12617 ANTIOCH RD</t>
         </is>
       </c>
       <c r="W66" t="inlineStr"/>
@@ -3780,7 +3765,7 @@
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr">
         <is>
-          <t>GAUGERT'S BUSS STOP, SULLIVAN</t>
+          <t>141 MAIN ST</t>
         </is>
       </c>
       <c r="G67" t="inlineStr"/>
@@ -3796,7 +3781,7 @@
       <c r="M67" t="inlineStr"/>
       <c r="N67" t="inlineStr">
         <is>
-          <t xml:space="preserve">TO FOLLOW   </t>
+          <t>https://goo.gl/maps/SvuibWN5b3H2</t>
         </is>
       </c>
       <c r="O67" t="inlineStr"/>
@@ -3812,7 +3797,7 @@
       <c r="U67" t="inlineStr"/>
       <c r="V67" t="inlineStr">
         <is>
-          <t>TO FOLLOW</t>
+          <t>https://goo.gl/maps/xA9YMzPGc6Vhxi5r8</t>
         </is>
       </c>
       <c r="W67" t="inlineStr"/>
@@ -3827,7 +3812,7 @@
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr">
         <is>
-          <t>141 MAIN ST</t>
+          <t>https://goo.gl/maps/TEUfEX2J1AE2</t>
         </is>
       </c>
       <c r="G68" t="inlineStr"/>
@@ -3843,7 +3828,7 @@
       <c r="M68" t="inlineStr"/>
       <c r="N68" t="inlineStr">
         <is>
-          <t>DC5-ITEM LEVEL</t>
+          <t xml:space="preserve">TO FOLLOW   </t>
         </is>
       </c>
       <c r="O68" t="inlineStr"/>
@@ -3859,7 +3844,7 @@
       <c r="U68" t="inlineStr"/>
       <c r="V68" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>TO FOLLOW</t>
         </is>
       </c>
       <c r="W68" t="inlineStr"/>
@@ -3874,7 +3859,7 @@
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/TEUfEX2J1AE2</t>
+          <t>APPROX 9:30/10:30 AM START</t>
         </is>
       </c>
       <c r="G69" t="inlineStr"/>
@@ -3890,7 +3875,7 @@
       <c r="M69" t="inlineStr"/>
       <c r="N69" t="inlineStr">
         <is>
-          <t>GROUP HEALTH RX, SAUK TRAILS</t>
+          <t>DC5-ITEM LEVEL</t>
         </is>
       </c>
       <c r="O69" t="inlineStr"/>
@@ -3906,7 +3891,7 @@
       <c r="U69" t="inlineStr"/>
       <c r="V69" t="inlineStr">
         <is>
-          <t>ROTE OIL #13 TREVOR (BP)</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="W69" t="inlineStr"/>
@@ -3921,7 +3906,7 @@
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr">
         <is>
-          <t>APPROX 9:30/10:30 AM START</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="G70" t="inlineStr"/>
@@ -3937,7 +3922,7 @@
       <c r="M70" t="inlineStr"/>
       <c r="N70" t="inlineStr">
         <is>
-          <t>8202 EXCELSIOR DR</t>
+          <t>GROUP HEALTH RX, HATCHERY HILLS</t>
         </is>
       </c>
       <c r="O70" t="inlineStr"/>
@@ -3953,7 +3938,7 @@
       <c r="U70" t="inlineStr"/>
       <c r="V70" t="inlineStr">
         <is>
-          <t>12511 ANTIOCH RD</t>
+          <t>ROTE OIL #13 TREVOR (BP)</t>
         </is>
       </c>
       <c r="W70" t="inlineStr"/>
@@ -3968,7 +3953,7 @@
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>RON'S MARKET, HELENVILLE</t>
         </is>
       </c>
       <c r="G71" t="inlineStr"/>
@@ -3984,7 +3969,7 @@
       <c r="M71" t="inlineStr"/>
       <c r="N71" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/SvuibWN5b3H2</t>
+          <t>3051 CAHILL MAIN</t>
         </is>
       </c>
       <c r="O71" t="inlineStr"/>
@@ -3996,7 +3981,7 @@
       <c r="U71" t="inlineStr"/>
       <c r="V71" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/iu3xzNwgJ32esP5RA</t>
+          <t>12511 ANTIOCH RD</t>
         </is>
       </c>
       <c r="W71" t="inlineStr"/>
@@ -4011,7 +3996,7 @@
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr">
         <is>
-          <t>RON'S MARKET, HELENVILLE</t>
+          <t>W3094 HWY 18</t>
         </is>
       </c>
       <c r="G72" t="inlineStr"/>
@@ -4027,7 +4012,7 @@
       <c r="M72" t="inlineStr"/>
       <c r="N72" t="inlineStr">
         <is>
-          <t xml:space="preserve">TO FOLLOW   </t>
+          <t>https://goo.gl/maps/BVziRjp8bAS2</t>
         </is>
       </c>
       <c r="O72" t="inlineStr"/>
@@ -4049,7 +4034,11 @@
       </c>
       <c r="T72" t="inlineStr"/>
       <c r="U72" t="inlineStr"/>
-      <c r="V72" t="inlineStr"/>
+      <c r="V72" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/iu3xzNwgJ32esP5RA</t>
+        </is>
+      </c>
       <c r="W72" t="inlineStr"/>
       <c r="X72" t="inlineStr"/>
       <c r="Y72" t="inlineStr"/>
@@ -4062,7 +4051,7 @@
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
-          <t>W3094 HWY 18</t>
+          <t>https://goo.gl/maps/pyYX7wkpwom</t>
         </is>
       </c>
       <c r="G73" t="inlineStr"/>
@@ -4076,11 +4065,7 @@
       <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr"/>
       <c r="M73" t="inlineStr"/>
-      <c r="N73" t="inlineStr">
-        <is>
-          <t>DC5-ITEM LEVEL</t>
-        </is>
-      </c>
+      <c r="N73" t="inlineStr"/>
       <c r="O73" t="inlineStr"/>
       <c r="P73" t="inlineStr"/>
       <c r="Q73" t="inlineStr">
@@ -4095,22 +4080,9 @@
       </c>
       <c r="S73" t="inlineStr"/>
       <c r="T73" t="inlineStr"/>
-      <c r="U73" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
-      <c r="V73" t="inlineStr">
-        <is>
-          <t>Ian</t>
-        </is>
-      </c>
-      <c r="W73" t="inlineStr">
-        <is>
-          <t>Driver,
-Red Van, Equip</t>
-        </is>
-      </c>
+      <c r="U73" t="inlineStr"/>
+      <c r="V73" t="inlineStr"/>
+      <c r="W73" t="inlineStr"/>
       <c r="X73" t="inlineStr"/>
       <c r="Y73" t="inlineStr"/>
     </row>
@@ -4120,11 +4092,7 @@
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr"/>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>https://goo.gl/maps/pyYX7wkpwom</t>
-        </is>
-      </c>
+      <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr"/>
       <c r="I74" t="inlineStr"/>
@@ -4135,13 +4103,22 @@
       </c>
       <c r="K74" t="inlineStr"/>
       <c r="L74" t="inlineStr"/>
-      <c r="M74" t="inlineStr"/>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
       <c r="N74" t="inlineStr">
         <is>
-          <t>GROUP HEALTH RX, HATCHERY HILLS</t>
-        </is>
-      </c>
-      <c r="O74" t="inlineStr"/>
+          <t>Sarah</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>@ Store,
+Equip</t>
+        </is>
+      </c>
       <c r="P74" t="inlineStr"/>
       <c r="Q74" t="inlineStr">
         <is>
@@ -4157,15 +4134,20 @@
       <c r="T74" t="inlineStr"/>
       <c r="U74" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>1)</t>
         </is>
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>Paul</t>
-        </is>
-      </c>
-      <c r="W74" t="inlineStr"/>
+          <t>Ian</t>
+        </is>
+      </c>
+      <c r="W74" t="inlineStr">
+        <is>
+          <t>Driver,
+Red Van, Equip</t>
+        </is>
+      </c>
       <c r="X74" t="inlineStr"/>
       <c r="Y74" t="inlineStr"/>
     </row>
@@ -4174,9 +4156,22 @@
       <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr"/>
-      <c r="F75" t="inlineStr"/>
-      <c r="G75" t="inlineStr"/>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>DJ</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Driver,
+Altima, Equip</t>
+        </is>
+      </c>
       <c r="H75" t="inlineStr"/>
       <c r="I75" t="inlineStr"/>
       <c r="J75" t="inlineStr">
@@ -4186,13 +4181,22 @@
       </c>
       <c r="K75" t="inlineStr"/>
       <c r="L75" t="inlineStr"/>
-      <c r="M75" t="inlineStr"/>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
       <c r="N75" t="inlineStr">
         <is>
-          <t>3051 CAHILL MAIN</t>
-        </is>
-      </c>
-      <c r="O75" t="inlineStr"/>
+          <t>Ashley P</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>Driver,
+Camry 3</t>
+        </is>
+      </c>
       <c r="P75" t="inlineStr"/>
       <c r="Q75" t="inlineStr">
         <is>
@@ -4206,8 +4210,16 @@
       </c>
       <c r="S75" t="inlineStr"/>
       <c r="T75" t="inlineStr"/>
-      <c r="U75" t="inlineStr"/>
-      <c r="V75" t="inlineStr"/>
+      <c r="U75" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="V75" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
       <c r="W75" t="inlineStr"/>
       <c r="X75" t="inlineStr"/>
       <c r="Y75" t="inlineStr"/>
@@ -4219,29 +4231,28 @@
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr">
         <is>
-          <t>1)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>DJ</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>Driver,
-Altima, Equip</t>
-        </is>
-      </c>
+          <t>Mai</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
       <c r="I76" t="inlineStr"/>
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr"/>
       <c r="L76" t="inlineStr"/>
-      <c r="M76" t="inlineStr"/>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>3)</t>
+        </is>
+      </c>
       <c r="N76" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/BVziRjp8bAS2</t>
+          <t>Eva</t>
         </is>
       </c>
       <c r="O76" t="inlineStr"/>
@@ -4274,16 +4285,8 @@
       <c r="B77" t="inlineStr"/>
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>2)</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>Mai</t>
-        </is>
-      </c>
+      <c r="E77" t="inlineStr"/>
+      <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr"/>
       <c r="I77" t="inlineStr">
@@ -4302,13 +4305,21 @@
         </is>
       </c>
       <c r="L77" t="inlineStr"/>
-      <c r="M77" t="inlineStr"/>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>4)</t>
+        </is>
+      </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>*IL Meet is 5:45 am at IL Office</t>
-        </is>
-      </c>
-      <c r="O77" t="inlineStr"/>
+          <t>Lori</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
       <c r="P77" t="inlineStr"/>
       <c r="Q77" t="inlineStr">
         <is>
@@ -4322,16 +4333,13 @@
       </c>
       <c r="S77" t="inlineStr">
         <is>
-          <t>@ Store</t>
+          <t>Driver, 1/2
+Camry 3</t>
         </is>
       </c>
       <c r="T77" t="inlineStr"/>
       <c r="U77" t="inlineStr"/>
-      <c r="V77" t="inlineStr">
-        <is>
-          <t>7:00 AM START</t>
-        </is>
-      </c>
+      <c r="V77" t="inlineStr"/>
       <c r="W77" t="inlineStr"/>
       <c r="X77" t="inlineStr"/>
       <c r="Y77" t="inlineStr"/>
@@ -4341,7 +4349,11 @@
       <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr"/>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="inlineStr"/>
@@ -4380,7 +4392,7 @@
       <c r="U78" t="inlineStr"/>
       <c r="V78" t="inlineStr">
         <is>
-          <t>SALE INVENTORIES</t>
+          <t>7:00 AM START</t>
         </is>
       </c>
       <c r="W78" t="inlineStr"/>
@@ -4392,12 +4404,12 @@
       <c r="B79" t="inlineStr"/>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="inlineStr"/>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr"/>
+      <c r="E79" t="inlineStr"/>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>IL: 4:40 MEET AT JANESVILLE PARK N RIDE</t>
+        </is>
+      </c>
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="inlineStr"/>
       <c r="I79" t="inlineStr">
@@ -4412,22 +4424,9 @@
       </c>
       <c r="K79" t="inlineStr"/>
       <c r="L79" t="inlineStr"/>
-      <c r="M79" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
-      <c r="N79" t="inlineStr">
-        <is>
-          <t>Sarah</t>
-        </is>
-      </c>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>@ Store,
-Equip</t>
-        </is>
-      </c>
+      <c r="M79" t="inlineStr"/>
+      <c r="N79" t="inlineStr"/>
+      <c r="O79" t="inlineStr"/>
       <c r="P79" t="inlineStr"/>
       <c r="Q79" t="inlineStr">
         <is>
@@ -4441,14 +4440,15 @@
       </c>
       <c r="S79" t="inlineStr">
         <is>
-          <t>@ Store</t>
+          <t>Driver, 1/2
+Camry 3</t>
         </is>
       </c>
       <c r="T79" t="inlineStr"/>
       <c r="U79" t="inlineStr"/>
       <c r="V79" t="inlineStr">
         <is>
-          <t>CONTACT IS ROBBY</t>
+          <t>EXCEL FINANCIAL</t>
         </is>
       </c>
       <c r="W79" t="inlineStr"/>
@@ -4465,29 +4465,24 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F80" t="inlineStr"/>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>6:00 AM START</t>
+        </is>
+      </c>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr"/>
       <c r="I80" t="inlineStr"/>
       <c r="J80" t="inlineStr"/>
       <c r="K80" t="inlineStr"/>
       <c r="L80" t="inlineStr"/>
-      <c r="M80" t="inlineStr">
-        <is>
-          <t>2)</t>
-        </is>
-      </c>
+      <c r="M80" t="inlineStr"/>
       <c r="N80" t="inlineStr">
         <is>
-          <t>Ashley P</t>
-        </is>
-      </c>
-      <c r="O80" t="inlineStr">
-        <is>
-          <t>Driver,
-Camry 3</t>
-        </is>
-      </c>
+          <t>Office</t>
+        </is>
+      </c>
+      <c r="O80" t="inlineStr"/>
       <c r="P80" t="inlineStr"/>
       <c r="Q80" t="inlineStr">
         <is>
@@ -4508,7 +4503,7 @@
       <c r="U80" t="inlineStr"/>
       <c r="V80" t="inlineStr">
         <is>
-          <t>EXCEL FINANCIAL</t>
+          <t>AMOCO, MADISON-VERONA RD</t>
         </is>
       </c>
       <c r="W80" t="inlineStr"/>
@@ -4520,26 +4515,22 @@
       <c r="B81" t="inlineStr"/>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr"/>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr"/>
+      <c r="E81" t="inlineStr"/>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>DC5-FINANCIAL</t>
+        </is>
+      </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr"/>
       <c r="I81" t="inlineStr"/>
       <c r="J81" t="inlineStr"/>
       <c r="K81" t="inlineStr"/>
       <c r="L81" t="inlineStr"/>
-      <c r="M81" t="inlineStr">
-        <is>
-          <t>3)</t>
-        </is>
-      </c>
+      <c r="M81" t="inlineStr"/>
       <c r="N81" t="inlineStr">
         <is>
-          <t>Eva</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="O81" t="inlineStr"/>
@@ -4554,16 +4545,12 @@
           <t>Taylor</t>
         </is>
       </c>
-      <c r="S81" t="inlineStr">
-        <is>
-          <t>@ Store</t>
-        </is>
-      </c>
+      <c r="S81" t="inlineStr"/>
       <c r="T81" t="inlineStr"/>
       <c r="U81" t="inlineStr"/>
       <c r="V81" t="inlineStr">
         <is>
-          <t>AMOCO, MADISON-VERONA RD</t>
+          <t>4602 VERONA RD</t>
         </is>
       </c>
       <c r="W81" t="inlineStr"/>
@@ -4575,37 +4562,29 @@
       <c r="B82" t="inlineStr"/>
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="inlineStr"/>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr"/>
+      <c r="E82" t="inlineStr"/>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>BWP LIQUOR EXPO, LAKE DELTON</t>
+        </is>
+      </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr"/>
       <c r="I82" t="inlineStr"/>
       <c r="J82" t="inlineStr">
         <is>
-          <t>6:00 AM START</t>
+          <t>IL: 5:00 AM MEET AT OFFICE</t>
         </is>
       </c>
       <c r="K82" t="inlineStr"/>
       <c r="L82" t="inlineStr"/>
-      <c r="M82" t="inlineStr">
-        <is>
-          <t>4)</t>
-        </is>
-      </c>
+      <c r="M82" t="inlineStr"/>
       <c r="N82" t="inlineStr">
         <is>
-          <t>Lori</t>
-        </is>
-      </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>@ Store</t>
-        </is>
-      </c>
+          <t>Lashaun</t>
+        </is>
+      </c>
+      <c r="O82" t="inlineStr"/>
       <c r="P82" t="inlineStr"/>
       <c r="Q82" t="inlineStr"/>
       <c r="R82" t="inlineStr"/>
@@ -4614,7 +4593,7 @@
       <c r="U82" t="inlineStr"/>
       <c r="V82" t="inlineStr">
         <is>
-          <t>4602 VERONA RD</t>
+          <t>https://maps.app.goo.gl/tdbvCRXWi1zyhZ7WA</t>
         </is>
       </c>
       <c r="W82" t="inlineStr"/>
@@ -4626,14 +4605,10 @@
       <c r="B83" t="inlineStr"/>
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="inlineStr"/>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
+      <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr">
         <is>
-          <t>5:30 AM MEET COLLEGE (SOUTHWEST)</t>
+          <t>21 WISCONSIN DELLS PARKWAY</t>
         </is>
       </c>
       <c r="G83" t="inlineStr"/>
@@ -4641,7 +4616,7 @@
       <c r="I83" t="inlineStr"/>
       <c r="J83" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="K83" t="inlineStr"/>
@@ -4657,7 +4632,7 @@
       <c r="U83" t="inlineStr"/>
       <c r="V83" t="inlineStr">
         <is>
-          <t>https://maps.app.goo.gl/tdbvCRXWi1zyhZ7WA</t>
+          <t>TO FOLLOW</t>
         </is>
       </c>
       <c r="W83" t="inlineStr"/>
@@ -4672,7 +4647,7 @@
       <c r="E84" t="inlineStr"/>
       <c r="F84" t="inlineStr">
         <is>
-          <t>6:00 AM START</t>
+          <t>https://goo.gl/maps/34cUYxex6oP2</t>
         </is>
       </c>
       <c r="G84" t="inlineStr"/>
@@ -4680,7 +4655,7 @@
       <c r="I84" t="inlineStr"/>
       <c r="J84" t="inlineStr">
         <is>
-          <t>SULLIVAN'S FOODS #241, LENA</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="K84" t="inlineStr"/>
@@ -4692,7 +4667,7 @@
       <c r="Q84" t="inlineStr"/>
       <c r="R84" t="inlineStr">
         <is>
-          <t>7:00 AM START</t>
+          <t>IL: 5:00 MEET AT OFFICE</t>
         </is>
       </c>
       <c r="S84" t="inlineStr"/>
@@ -4700,7 +4675,7 @@
       <c r="U84" t="inlineStr"/>
       <c r="V84" t="inlineStr">
         <is>
-          <t>TO FOLLOW</t>
+          <t>BP, MADISON-VERONA RD</t>
         </is>
       </c>
       <c r="W84" t="inlineStr"/>
@@ -4715,7 +4690,7 @@
       <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>TO FOLLOW</t>
         </is>
       </c>
       <c r="G85" t="inlineStr"/>
@@ -4723,7 +4698,7 @@
       <c r="I85" t="inlineStr"/>
       <c r="J85" t="inlineStr">
         <is>
-          <t>201 DODDS DRIVE</t>
+          <t>SULLIVAN'S FOODS #241, LENA</t>
         </is>
       </c>
       <c r="K85" t="inlineStr"/>
@@ -4735,7 +4710,7 @@
       <c r="Q85" t="inlineStr"/>
       <c r="R85" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>7:00 AM START</t>
         </is>
       </c>
       <c r="S85" t="inlineStr"/>
@@ -4743,7 +4718,7 @@
       <c r="U85" t="inlineStr"/>
       <c r="V85" t="inlineStr">
         <is>
-          <t>BP, MADISON-VERONA RD</t>
+          <t>4501 VERONA RD</t>
         </is>
       </c>
       <c r="W85" t="inlineStr"/>
@@ -4758,7 +4733,7 @@
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr">
         <is>
-          <t>PIGGLY WIGGLY #355, RACINE</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="G86" t="inlineStr"/>
@@ -4766,7 +4741,7 @@
       <c r="I86" t="inlineStr"/>
       <c r="J86" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/82qhta5RyXsUSC2u9</t>
+          <t>201 DODDS DRIVE</t>
         </is>
       </c>
       <c r="K86" t="inlineStr"/>
@@ -4778,7 +4753,7 @@
       <c r="Q86" t="inlineStr"/>
       <c r="R86" t="inlineStr">
         <is>
-          <t>MAURER'S MARKET, WISCONSIN DELLS</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="S86" t="inlineStr"/>
@@ -4786,7 +4761,7 @@
       <c r="U86" t="inlineStr"/>
       <c r="V86" t="inlineStr">
         <is>
-          <t>4501 VERONA RD</t>
+          <t>https://maps.app.goo.gl/KVpnPc3rpoZKAen88</t>
         </is>
       </c>
       <c r="W86" t="inlineStr"/>
@@ -4801,7 +4776,7 @@
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr">
         <is>
-          <t>3901 ERIE ST</t>
+          <t>PIERCE'S WEST EXPRESS, BARABOO</t>
         </is>
       </c>
       <c r="G87" t="inlineStr"/>
@@ -4809,7 +4784,7 @@
       <c r="I87" t="inlineStr"/>
       <c r="J87" t="inlineStr">
         <is>
-          <t>*IL Meet is 5:00 am at IL Office</t>
+          <t>https://goo.gl/maps/82qhta5RyXsUSC2u9</t>
         </is>
       </c>
       <c r="K87" t="inlineStr"/>
@@ -4821,7 +4796,7 @@
       <c r="Q87" t="inlineStr"/>
       <c r="R87" t="inlineStr">
         <is>
-          <t>216 WASHINGTON AVE</t>
+          <t>MAURER'S MARKET, WISCONSIN DELLS</t>
         </is>
       </c>
       <c r="S87" t="inlineStr"/>
@@ -4829,7 +4804,7 @@
       <c r="U87" t="inlineStr"/>
       <c r="V87" t="inlineStr">
         <is>
-          <t>https://maps.app.goo.gl/KVpnPc3rpoZKAen88</t>
+          <t>SALE INVENTORIES CONTACT IS ROBBY</t>
         </is>
       </c>
       <c r="W87" t="inlineStr"/>
@@ -4844,7 +4819,7 @@
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/pSDNmBRxXrQ3</t>
+          <t>527 LINN ST</t>
         </is>
       </c>
       <c r="G88" t="inlineStr"/>
@@ -4860,7 +4835,7 @@
       <c r="Q88" t="inlineStr"/>
       <c r="R88" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/CXVPLJR1DyH2</t>
+          <t>216 WASHINGTON AVE</t>
         </is>
       </c>
       <c r="S88" t="inlineStr"/>
@@ -4879,7 +4854,7 @@
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr">
         <is>
-          <t>SMALL CHANGES-RESET</t>
+          <t>https://goo.gl/maps/efhcEzsX18sU7KcN9</t>
         </is>
       </c>
       <c r="G89" t="inlineStr"/>
@@ -4909,7 +4884,7 @@
       <c r="Q89" t="inlineStr"/>
       <c r="R89" t="inlineStr">
         <is>
-          <t>*IL Meet is 5:00 am at IL Office</t>
+          <t>https://goo.gl/maps/CXVPLJR1DyH2</t>
         </is>
       </c>
       <c r="S89" t="inlineStr"/>
@@ -4940,7 +4915,8 @@
       <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr">
         <is>
-          <t>4:45 am meet for Carlie/Trevor at Grafton Park n Ride</t>
+          <t>Janesville park n ride address:
+550 Midland Ct, Janesville</t>
         </is>
       </c>
       <c r="G90" t="inlineStr"/>
@@ -5035,9 +5011,22 @@
       <c r="B92" t="inlineStr"/>
       <c r="C92" t="inlineStr"/>
       <c r="D92" t="inlineStr"/>
-      <c r="E92" t="inlineStr"/>
-      <c r="F92" t="inlineStr"/>
-      <c r="G92" t="inlineStr"/>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Brianna</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Driver,
+Prius</t>
+        </is>
+      </c>
       <c r="H92" t="inlineStr"/>
       <c r="I92" t="inlineStr">
         <is>
@@ -5085,15 +5074,19 @@
       <c r="D93" t="inlineStr"/>
       <c r="E93" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>2)</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>6:00 AM START</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr"/>
+          <t>Josie</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Until Noon</t>
+        </is>
+      </c>
       <c r="H93" t="inlineStr"/>
       <c r="I93" t="inlineStr">
         <is>
@@ -5139,13 +5132,21 @@
       <c r="B94" t="inlineStr"/>
       <c r="C94" t="inlineStr"/>
       <c r="D94" t="inlineStr"/>
-      <c r="E94" t="inlineStr"/>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>3)</t>
+        </is>
+      </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr"/>
+          <t>Lori</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Until Noon</t>
+        </is>
+      </c>
       <c r="H94" t="inlineStr"/>
       <c r="I94" t="inlineStr">
         <is>
@@ -5191,13 +5192,21 @@
       <c r="B95" t="inlineStr"/>
       <c r="C95" t="inlineStr"/>
       <c r="D95" t="inlineStr"/>
-      <c r="E95" t="inlineStr"/>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>4)</t>
+        </is>
+      </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>BWP LIQUOR EXPO, LAKE DELTON</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr"/>
+          <t>Qiana</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Camry 3 to meet</t>
+        </is>
+      </c>
       <c r="H95" t="inlineStr"/>
       <c r="I95" t="inlineStr">
         <is>
@@ -5239,11 +5248,7 @@
       <c r="C96" t="inlineStr"/>
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr"/>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>21 WISCONSIN DELLS PARKWAY</t>
-        </is>
-      </c>
+      <c r="F96" t="inlineStr"/>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr"/>
       <c r="I96" t="inlineStr"/>
@@ -5278,11 +5283,7 @@
       <c r="C97" t="inlineStr"/>
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="inlineStr"/>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>https://goo.gl/maps/34cUYxex6oP2</t>
-        </is>
-      </c>
+      <c r="F97" t="inlineStr"/>
       <c r="G97" t="inlineStr"/>
       <c r="H97" t="inlineStr"/>
       <c r="I97" t="inlineStr"/>
@@ -5317,19 +5318,11 @@
       <c r="C98" t="inlineStr"/>
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr"/>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>TO FOLLOW</t>
-        </is>
-      </c>
+      <c r="F98" t="inlineStr"/>
       <c r="G98" t="inlineStr"/>
       <c r="H98" t="inlineStr"/>
       <c r="I98" t="inlineStr"/>
-      <c r="J98" t="inlineStr">
-        <is>
-          <t>6:00 AM START</t>
-        </is>
-      </c>
+      <c r="J98" t="inlineStr"/>
       <c r="K98" t="inlineStr"/>
       <c r="L98" t="inlineStr"/>
       <c r="M98" t="inlineStr"/>
@@ -5365,17 +5358,14 @@
       <c r="C99" t="inlineStr"/>
       <c r="D99" t="inlineStr"/>
       <c r="E99" t="inlineStr"/>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>DC5-FINANCIAL</t>
-        </is>
-      </c>
+      <c r="F99" t="inlineStr"/>
       <c r="G99" t="inlineStr"/>
       <c r="H99" t="inlineStr"/>
       <c r="I99" t="inlineStr"/>
       <c r="J99" t="inlineStr">
         <is>
-          <t>DC5-ITEM LEVEL</t>
+          <t>IL: 4:00 AM MEET AT OFFICE
+MD: 4:45 MEET HOME DEPOT VERONA RD</t>
         </is>
       </c>
       <c r="K99" t="inlineStr"/>
@@ -5413,17 +5403,13 @@
       <c r="C100" t="inlineStr"/>
       <c r="D100" t="inlineStr"/>
       <c r="E100" t="inlineStr"/>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>PIERCE'S WEST EXPRESS, BARABOO</t>
-        </is>
-      </c>
+      <c r="F100" t="inlineStr"/>
       <c r="G100" t="inlineStr"/>
       <c r="H100" t="inlineStr"/>
       <c r="I100" t="inlineStr"/>
       <c r="J100" t="inlineStr">
         <is>
-          <t>SOUTHWEST HEALTH HOSPITAL-INPATIENT, PLATTEVILLE</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="K100" t="inlineStr"/>
@@ -5450,7 +5436,7 @@
       <c r="E101" t="inlineStr"/>
       <c r="F101" t="inlineStr">
         <is>
-          <t>527 LINN ST</t>
+          <t>IL: 4:15 AM MEET AT OFFICE</t>
         </is>
       </c>
       <c r="G101" t="inlineStr"/>
@@ -5458,7 +5444,7 @@
       <c r="I101" t="inlineStr"/>
       <c r="J101" t="inlineStr">
         <is>
-          <t>1400 EASTSIDE RD</t>
+          <t>DC5-ITEM LEVEL</t>
         </is>
       </c>
       <c r="K101" t="inlineStr"/>
@@ -5485,7 +5471,7 @@
       <c r="E102" t="inlineStr"/>
       <c r="F102" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/efhcEzsX18sU7KcN9</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="G102" t="inlineStr"/>
@@ -5493,7 +5479,7 @@
       <c r="I102" t="inlineStr"/>
       <c r="J102" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/tENERhYm35H2</t>
+          <t>SOUTHWEST HEALTH HOSPITAL-INPATIENT, PLATTEVILLE</t>
         </is>
       </c>
       <c r="K102" t="inlineStr"/>
@@ -5520,7 +5506,7 @@
       <c r="E103" t="inlineStr"/>
       <c r="F103" t="inlineStr">
         <is>
-          <t>*4:00 am IL office leave time</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="G103" t="inlineStr"/>
@@ -5528,7 +5514,7 @@
       <c r="I103" t="inlineStr"/>
       <c r="J103" t="inlineStr">
         <is>
-          <t>TO FOLLOW</t>
+          <t>1400 EASTSIDE RD</t>
         </is>
       </c>
       <c r="K103" t="inlineStr"/>
@@ -5555,7 +5541,7 @@
       <c r="E104" t="inlineStr"/>
       <c r="F104" t="inlineStr">
         <is>
-          <t>*4:40 am meet for Brianna/Qiana at Janesville park n ride</t>
+          <t>PIERCE'S EXPRESS MARKET, BARABOO (GROC + C-STORE)</t>
         </is>
       </c>
       <c r="G104" t="inlineStr"/>
@@ -5563,7 +5549,7 @@
       <c r="I104" t="inlineStr"/>
       <c r="J104" t="inlineStr">
         <is>
-          <t>DC5-ITEM LEVEL</t>
+          <t>https://goo.gl/maps/tENERhYm35H2</t>
         </is>
       </c>
       <c r="K104" t="inlineStr"/>
@@ -5590,8 +5576,7 @@
       <c r="E105" t="inlineStr"/>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Janesville park n ride address:
-550 Midland Ct, Janesville</t>
+          <t>935 8TH ST</t>
         </is>
       </c>
       <c r="G105" t="inlineStr"/>
@@ -5599,7 +5584,7 @@
       <c r="I105" t="inlineStr"/>
       <c r="J105" t="inlineStr">
         <is>
-          <t>SOUTHWEST HEALTH HOSPITAL-OUTPATIENT, PLATTEVILLE</t>
+          <t>TO FOLLOW</t>
         </is>
       </c>
       <c r="K105" t="inlineStr"/>
@@ -5624,13 +5609,17 @@
       <c r="C106" t="inlineStr"/>
       <c r="D106" t="inlineStr"/>
       <c r="E106" t="inlineStr"/>
-      <c r="F106" t="inlineStr"/>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/GhH3B9P8DGn</t>
+        </is>
+      </c>
       <c r="G106" t="inlineStr"/>
       <c r="H106" t="inlineStr"/>
       <c r="I106" t="inlineStr"/>
       <c r="J106" t="inlineStr">
         <is>
-          <t>1400 EASTSIDE RD</t>
+          <t>DC5-ITEM LEVEL</t>
         </is>
       </c>
       <c r="K106" t="inlineStr"/>
@@ -5654,27 +5643,14 @@
       <c r="B107" t="inlineStr"/>
       <c r="C107" t="inlineStr"/>
       <c r="D107" t="inlineStr"/>
-      <c r="E107" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>Brianna</t>
-        </is>
-      </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>Driver,
-Prius</t>
-        </is>
-      </c>
+      <c r="E107" t="inlineStr"/>
+      <c r="F107" t="inlineStr"/>
+      <c r="G107" t="inlineStr"/>
       <c r="H107" t="inlineStr"/>
       <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/ueV1odVEdtxrmE3m7</t>
+          <t>SOUTHWEST HEALTH HOSPITAL-OUTPATIENT, PLATTEVILLE</t>
         </is>
       </c>
       <c r="K107" t="inlineStr"/>
@@ -5700,24 +5676,24 @@
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>1)</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Josie</t>
+          <t>Sarah</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>@ Store, Until Noon</t>
+          <t>@ Store, Equip</t>
         </is>
       </c>
       <c r="H108" t="inlineStr"/>
       <c r="I108" t="inlineStr"/>
       <c r="J108" t="inlineStr">
         <is>
-          <t>*IL Meet is 4:00 am at IL Office</t>
+          <t>1400 EASTSIDE RD</t>
         </is>
       </c>
       <c r="K108" t="inlineStr"/>
@@ -5743,24 +5719,25 @@
       <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr">
         <is>
-          <t>3)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>Lori</t>
+          <t>Angela</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>@ Store, Until Noon</t>
+          <t>Driver, 1/2
+Silver Van</t>
         </is>
       </c>
       <c r="H109" t="inlineStr"/>
       <c r="I109" t="inlineStr"/>
       <c r="J109" t="inlineStr">
         <is>
-          <t>*Sarah, Josie &amp; Lori - 4:45 am meet Home Depot Verona Rd</t>
+          <t>https://goo.gl/maps/ueV1odVEdtxrmE3m7</t>
         </is>
       </c>
       <c r="K109" t="inlineStr"/>
@@ -5786,19 +5763,15 @@
       <c r="D110" t="inlineStr"/>
       <c r="E110" t="inlineStr">
         <is>
-          <t>4)</t>
+          <t>3)</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Qiana</t>
-        </is>
-      </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>Camry 3 to meet</t>
-        </is>
-      </c>
+          <t>Anisha</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr"/>
       <c r="H110" t="inlineStr"/>
       <c r="I110" t="inlineStr"/>
       <c r="J110" t="inlineStr"/>
@@ -5823,9 +5796,22 @@
       <c r="B111" t="inlineStr"/>
       <c r="C111" t="inlineStr"/>
       <c r="D111" t="inlineStr"/>
-      <c r="E111" t="inlineStr"/>
-      <c r="F111" t="inlineStr"/>
-      <c r="G111" t="inlineStr"/>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>4)</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Ashley P</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>Driver, 1/2
+Silver Van</t>
+        </is>
+      </c>
       <c r="H111" t="inlineStr"/>
       <c r="I111" t="inlineStr">
         <is>
@@ -5839,7 +5825,7 @@
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>@ Store,
+          <t>Driver,
 Equip</t>
         </is>
       </c>
@@ -5863,8 +5849,16 @@
       <c r="B112" t="inlineStr"/>
       <c r="C112" t="inlineStr"/>
       <c r="D112" t="inlineStr"/>
-      <c r="E112" t="inlineStr"/>
-      <c r="F112" t="inlineStr"/>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>5)</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Elijah</t>
+        </is>
+      </c>
       <c r="G112" t="inlineStr"/>
       <c r="H112" t="inlineStr"/>
       <c r="I112" t="inlineStr">
@@ -5903,10 +5897,14 @@
       <c r="B113" t="inlineStr"/>
       <c r="C113" t="inlineStr"/>
       <c r="D113" t="inlineStr"/>
-      <c r="E113" t="inlineStr"/>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>6)</t>
+        </is>
+      </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>6:00 AM START</t>
+          <t>Eva</t>
         </is>
       </c>
       <c r="G113" t="inlineStr"/>
@@ -5942,10 +5940,14 @@
       <c r="B114" t="inlineStr"/>
       <c r="C114" t="inlineStr"/>
       <c r="D114" t="inlineStr"/>
-      <c r="E114" t="inlineStr"/>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>7)</t>
+        </is>
+      </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>Evelin</t>
         </is>
       </c>
       <c r="G114" t="inlineStr"/>
@@ -5960,11 +5962,7 @@
           <t>Josie</t>
         </is>
       </c>
-      <c r="K114" t="inlineStr">
-        <is>
-          <t>w/ Sarah</t>
-        </is>
-      </c>
+      <c r="K114" t="inlineStr"/>
       <c r="L114" t="inlineStr"/>
       <c r="M114" t="inlineStr"/>
       <c r="N114" t="inlineStr"/>
@@ -5985,10 +5983,14 @@
       <c r="B115" t="inlineStr"/>
       <c r="C115" t="inlineStr"/>
       <c r="D115" t="inlineStr"/>
-      <c r="E115" t="inlineStr"/>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>8)</t>
+        </is>
+      </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>PIERCE'S EXPRESS MARKET, BARABOO (GROC + C-STORE)</t>
+          <t>Joseph</t>
         </is>
       </c>
       <c r="G115" t="inlineStr"/>
@@ -6003,11 +6005,7 @@
           <t>Lori</t>
         </is>
       </c>
-      <c r="K115" t="inlineStr">
-        <is>
-          <t>w/ Sarah</t>
-        </is>
-      </c>
+      <c r="K115" t="inlineStr"/>
       <c r="L115" t="inlineStr"/>
       <c r="M115" t="inlineStr"/>
       <c r="N115" t="inlineStr"/>
@@ -6028,10 +6026,14 @@
       <c r="B116" t="inlineStr"/>
       <c r="C116" t="inlineStr"/>
       <c r="D116" t="inlineStr"/>
-      <c r="E116" t="inlineStr"/>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>9)</t>
+        </is>
+      </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>935 8TH ST</t>
+          <t>Justin</t>
         </is>
       </c>
       <c r="G116" t="inlineStr"/>
@@ -6072,13 +6074,22 @@
       <c r="B117" t="inlineStr"/>
       <c r="C117" t="inlineStr"/>
       <c r="D117" t="inlineStr"/>
-      <c r="E117" t="inlineStr"/>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>10)</t>
+        </is>
+      </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/GhH3B9P8DGn</t>
-        </is>
-      </c>
-      <c r="G117" t="inlineStr"/>
+          <t>Michael N</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>Driver, 1/2
+Gray Van</t>
+        </is>
+      </c>
       <c r="H117" t="inlineStr"/>
       <c r="I117" t="inlineStr"/>
       <c r="J117" t="inlineStr"/>
@@ -6103,13 +6114,22 @@
       <c r="B118" t="inlineStr"/>
       <c r="C118" t="inlineStr"/>
       <c r="D118" t="inlineStr"/>
-      <c r="E118" t="inlineStr"/>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>11)</t>
+        </is>
+      </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>*IL Meet is 4:15 am at IL Office</t>
-        </is>
-      </c>
-      <c r="G118" t="inlineStr"/>
+          <t>Nate</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>Driver, 1/2
+Gray Van</t>
+        </is>
+      </c>
       <c r="H118" t="inlineStr"/>
       <c r="I118" t="inlineStr"/>
       <c r="J118" t="inlineStr"/>
@@ -6134,8 +6154,16 @@
       <c r="B119" t="inlineStr"/>
       <c r="C119" t="inlineStr"/>
       <c r="D119" t="inlineStr"/>
-      <c r="E119" t="inlineStr"/>
-      <c r="F119" t="inlineStr"/>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>12)</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Taylor</t>
+        </is>
+      </c>
       <c r="G119" t="inlineStr"/>
       <c r="H119" t="inlineStr"/>
       <c r="I119" t="inlineStr"/>
@@ -6156,450 +6184,6 @@
       <c r="X119" t="inlineStr"/>
       <c r="Y119" t="inlineStr"/>
     </row>
-    <row r="120">
-      <c r="A120" t="inlineStr"/>
-      <c r="B120" t="inlineStr"/>
-      <c r="C120" t="inlineStr"/>
-      <c r="D120" t="inlineStr"/>
-      <c r="E120" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
-      <c r="F120" t="inlineStr">
-        <is>
-          <t>Sarah</t>
-        </is>
-      </c>
-      <c r="G120" t="inlineStr">
-        <is>
-          <t>@ Store, Equip</t>
-        </is>
-      </c>
-      <c r="H120" t="inlineStr"/>
-      <c r="I120" t="inlineStr"/>
-      <c r="J120" t="inlineStr"/>
-      <c r="K120" t="inlineStr"/>
-      <c r="L120" t="inlineStr"/>
-      <c r="M120" t="inlineStr"/>
-      <c r="N120" t="inlineStr"/>
-      <c r="O120" t="inlineStr"/>
-      <c r="P120" t="inlineStr"/>
-      <c r="Q120" t="inlineStr"/>
-      <c r="R120" t="inlineStr"/>
-      <c r="S120" t="inlineStr"/>
-      <c r="T120" t="inlineStr"/>
-      <c r="U120" t="inlineStr"/>
-      <c r="V120" t="inlineStr"/>
-      <c r="W120" t="inlineStr"/>
-      <c r="X120" t="inlineStr"/>
-      <c r="Y120" t="inlineStr"/>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr"/>
-      <c r="B121" t="inlineStr"/>
-      <c r="C121" t="inlineStr"/>
-      <c r="D121" t="inlineStr"/>
-      <c r="E121" t="inlineStr">
-        <is>
-          <t>2)</t>
-        </is>
-      </c>
-      <c r="F121" t="inlineStr">
-        <is>
-          <t>Angela</t>
-        </is>
-      </c>
-      <c r="G121" t="inlineStr">
-        <is>
-          <t>Driver, 1/2
-Silver Van</t>
-        </is>
-      </c>
-      <c r="H121" t="inlineStr"/>
-      <c r="I121" t="inlineStr"/>
-      <c r="J121" t="inlineStr"/>
-      <c r="K121" t="inlineStr"/>
-      <c r="L121" t="inlineStr"/>
-      <c r="M121" t="inlineStr"/>
-      <c r="N121" t="inlineStr"/>
-      <c r="O121" t="inlineStr"/>
-      <c r="P121" t="inlineStr"/>
-      <c r="Q121" t="inlineStr"/>
-      <c r="R121" t="inlineStr"/>
-      <c r="S121" t="inlineStr"/>
-      <c r="T121" t="inlineStr"/>
-      <c r="U121" t="inlineStr"/>
-      <c r="V121" t="inlineStr"/>
-      <c r="W121" t="inlineStr"/>
-      <c r="X121" t="inlineStr"/>
-      <c r="Y121" t="inlineStr"/>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr"/>
-      <c r="B122" t="inlineStr"/>
-      <c r="C122" t="inlineStr"/>
-      <c r="D122" t="inlineStr"/>
-      <c r="E122" t="inlineStr">
-        <is>
-          <t>3)</t>
-        </is>
-      </c>
-      <c r="F122" t="inlineStr">
-        <is>
-          <t>Anisha</t>
-        </is>
-      </c>
-      <c r="G122" t="inlineStr"/>
-      <c r="H122" t="inlineStr"/>
-      <c r="I122" t="inlineStr"/>
-      <c r="J122" t="inlineStr"/>
-      <c r="K122" t="inlineStr"/>
-      <c r="L122" t="inlineStr"/>
-      <c r="M122" t="inlineStr"/>
-      <c r="N122" t="inlineStr"/>
-      <c r="O122" t="inlineStr"/>
-      <c r="P122" t="inlineStr"/>
-      <c r="Q122" t="inlineStr"/>
-      <c r="R122" t="inlineStr"/>
-      <c r="S122" t="inlineStr"/>
-      <c r="T122" t="inlineStr"/>
-      <c r="U122" t="inlineStr"/>
-      <c r="V122" t="inlineStr"/>
-      <c r="W122" t="inlineStr"/>
-      <c r="X122" t="inlineStr"/>
-      <c r="Y122" t="inlineStr"/>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr"/>
-      <c r="B123" t="inlineStr"/>
-      <c r="C123" t="inlineStr"/>
-      <c r="D123" t="inlineStr"/>
-      <c r="E123" t="inlineStr">
-        <is>
-          <t>4)</t>
-        </is>
-      </c>
-      <c r="F123" t="inlineStr">
-        <is>
-          <t>Ashley P</t>
-        </is>
-      </c>
-      <c r="G123" t="inlineStr">
-        <is>
-          <t>Driver, 1/2
-Silver Van</t>
-        </is>
-      </c>
-      <c r="H123" t="inlineStr"/>
-      <c r="I123" t="inlineStr"/>
-      <c r="J123" t="inlineStr"/>
-      <c r="K123" t="inlineStr"/>
-      <c r="L123" t="inlineStr"/>
-      <c r="M123" t="inlineStr"/>
-      <c r="N123" t="inlineStr"/>
-      <c r="O123" t="inlineStr"/>
-      <c r="P123" t="inlineStr"/>
-      <c r="Q123" t="inlineStr"/>
-      <c r="R123" t="inlineStr"/>
-      <c r="S123" t="inlineStr"/>
-      <c r="T123" t="inlineStr"/>
-      <c r="U123" t="inlineStr"/>
-      <c r="V123" t="inlineStr"/>
-      <c r="W123" t="inlineStr"/>
-      <c r="X123" t="inlineStr"/>
-      <c r="Y123" t="inlineStr"/>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr"/>
-      <c r="B124" t="inlineStr"/>
-      <c r="C124" t="inlineStr"/>
-      <c r="D124" t="inlineStr"/>
-      <c r="E124" t="inlineStr">
-        <is>
-          <t>5)</t>
-        </is>
-      </c>
-      <c r="F124" t="inlineStr">
-        <is>
-          <t>Elijah</t>
-        </is>
-      </c>
-      <c r="G124" t="inlineStr"/>
-      <c r="H124" t="inlineStr"/>
-      <c r="I124" t="inlineStr"/>
-      <c r="J124" t="inlineStr"/>
-      <c r="K124" t="inlineStr"/>
-      <c r="L124" t="inlineStr"/>
-      <c r="M124" t="inlineStr"/>
-      <c r="N124" t="inlineStr"/>
-      <c r="O124" t="inlineStr"/>
-      <c r="P124" t="inlineStr"/>
-      <c r="Q124" t="inlineStr"/>
-      <c r="R124" t="inlineStr"/>
-      <c r="S124" t="inlineStr"/>
-      <c r="T124" t="inlineStr"/>
-      <c r="U124" t="inlineStr"/>
-      <c r="V124" t="inlineStr"/>
-      <c r="W124" t="inlineStr"/>
-      <c r="X124" t="inlineStr"/>
-      <c r="Y124" t="inlineStr"/>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr"/>
-      <c r="B125" t="inlineStr"/>
-      <c r="C125" t="inlineStr"/>
-      <c r="D125" t="inlineStr"/>
-      <c r="E125" t="inlineStr">
-        <is>
-          <t>6)</t>
-        </is>
-      </c>
-      <c r="F125" t="inlineStr">
-        <is>
-          <t>Eva</t>
-        </is>
-      </c>
-      <c r="G125" t="inlineStr"/>
-      <c r="H125" t="inlineStr"/>
-      <c r="I125" t="inlineStr"/>
-      <c r="J125" t="inlineStr"/>
-      <c r="K125" t="inlineStr"/>
-      <c r="L125" t="inlineStr"/>
-      <c r="M125" t="inlineStr"/>
-      <c r="N125" t="inlineStr"/>
-      <c r="O125" t="inlineStr"/>
-      <c r="P125" t="inlineStr"/>
-      <c r="Q125" t="inlineStr"/>
-      <c r="R125" t="inlineStr"/>
-      <c r="S125" t="inlineStr"/>
-      <c r="T125" t="inlineStr"/>
-      <c r="U125" t="inlineStr"/>
-      <c r="V125" t="inlineStr"/>
-      <c r="W125" t="inlineStr"/>
-      <c r="X125" t="inlineStr"/>
-      <c r="Y125" t="inlineStr"/>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr"/>
-      <c r="B126" t="inlineStr"/>
-      <c r="C126" t="inlineStr"/>
-      <c r="D126" t="inlineStr"/>
-      <c r="E126" t="inlineStr">
-        <is>
-          <t>7)</t>
-        </is>
-      </c>
-      <c r="F126" t="inlineStr">
-        <is>
-          <t>Evelin</t>
-        </is>
-      </c>
-      <c r="G126" t="inlineStr"/>
-      <c r="H126" t="inlineStr"/>
-      <c r="I126" t="inlineStr"/>
-      <c r="J126" t="inlineStr"/>
-      <c r="K126" t="inlineStr"/>
-      <c r="L126" t="inlineStr"/>
-      <c r="M126" t="inlineStr"/>
-      <c r="N126" t="inlineStr"/>
-      <c r="O126" t="inlineStr"/>
-      <c r="P126" t="inlineStr"/>
-      <c r="Q126" t="inlineStr"/>
-      <c r="R126" t="inlineStr"/>
-      <c r="S126" t="inlineStr"/>
-      <c r="T126" t="inlineStr"/>
-      <c r="U126" t="inlineStr"/>
-      <c r="V126" t="inlineStr"/>
-      <c r="W126" t="inlineStr"/>
-      <c r="X126" t="inlineStr"/>
-      <c r="Y126" t="inlineStr"/>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr"/>
-      <c r="B127" t="inlineStr"/>
-      <c r="C127" t="inlineStr"/>
-      <c r="D127" t="inlineStr"/>
-      <c r="E127" t="inlineStr">
-        <is>
-          <t>8)</t>
-        </is>
-      </c>
-      <c r="F127" t="inlineStr">
-        <is>
-          <t>Joseph</t>
-        </is>
-      </c>
-      <c r="G127" t="inlineStr"/>
-      <c r="H127" t="inlineStr"/>
-      <c r="I127" t="inlineStr"/>
-      <c r="J127" t="inlineStr"/>
-      <c r="K127" t="inlineStr"/>
-      <c r="L127" t="inlineStr"/>
-      <c r="M127" t="inlineStr"/>
-      <c r="N127" t="inlineStr"/>
-      <c r="O127" t="inlineStr"/>
-      <c r="P127" t="inlineStr"/>
-      <c r="Q127" t="inlineStr"/>
-      <c r="R127" t="inlineStr"/>
-      <c r="S127" t="inlineStr"/>
-      <c r="T127" t="inlineStr"/>
-      <c r="U127" t="inlineStr"/>
-      <c r="V127" t="inlineStr"/>
-      <c r="W127" t="inlineStr"/>
-      <c r="X127" t="inlineStr"/>
-      <c r="Y127" t="inlineStr"/>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr"/>
-      <c r="B128" t="inlineStr"/>
-      <c r="C128" t="inlineStr"/>
-      <c r="D128" t="inlineStr"/>
-      <c r="E128" t="inlineStr">
-        <is>
-          <t>9)</t>
-        </is>
-      </c>
-      <c r="F128" t="inlineStr">
-        <is>
-          <t>Justin</t>
-        </is>
-      </c>
-      <c r="G128" t="inlineStr"/>
-      <c r="H128" t="inlineStr"/>
-      <c r="I128" t="inlineStr"/>
-      <c r="J128" t="inlineStr"/>
-      <c r="K128" t="inlineStr"/>
-      <c r="L128" t="inlineStr"/>
-      <c r="M128" t="inlineStr"/>
-      <c r="N128" t="inlineStr"/>
-      <c r="O128" t="inlineStr"/>
-      <c r="P128" t="inlineStr"/>
-      <c r="Q128" t="inlineStr"/>
-      <c r="R128" t="inlineStr"/>
-      <c r="S128" t="inlineStr"/>
-      <c r="T128" t="inlineStr"/>
-      <c r="U128" t="inlineStr"/>
-      <c r="V128" t="inlineStr"/>
-      <c r="W128" t="inlineStr"/>
-      <c r="X128" t="inlineStr"/>
-      <c r="Y128" t="inlineStr"/>
-    </row>
-    <row r="129">
-      <c r="A129" t="inlineStr"/>
-      <c r="B129" t="inlineStr"/>
-      <c r="C129" t="inlineStr"/>
-      <c r="D129" t="inlineStr"/>
-      <c r="E129" t="inlineStr">
-        <is>
-          <t>10)</t>
-        </is>
-      </c>
-      <c r="F129" t="inlineStr">
-        <is>
-          <t>Michael N</t>
-        </is>
-      </c>
-      <c r="G129" t="inlineStr">
-        <is>
-          <t>Driver, 1/2
-Gray Van</t>
-        </is>
-      </c>
-      <c r="H129" t="inlineStr"/>
-      <c r="I129" t="inlineStr"/>
-      <c r="J129" t="inlineStr"/>
-      <c r="K129" t="inlineStr"/>
-      <c r="L129" t="inlineStr"/>
-      <c r="M129" t="inlineStr"/>
-      <c r="N129" t="inlineStr"/>
-      <c r="O129" t="inlineStr"/>
-      <c r="P129" t="inlineStr"/>
-      <c r="Q129" t="inlineStr"/>
-      <c r="R129" t="inlineStr"/>
-      <c r="S129" t="inlineStr"/>
-      <c r="T129" t="inlineStr"/>
-      <c r="U129" t="inlineStr"/>
-      <c r="V129" t="inlineStr"/>
-      <c r="W129" t="inlineStr"/>
-      <c r="X129" t="inlineStr"/>
-      <c r="Y129" t="inlineStr"/>
-    </row>
-    <row r="130">
-      <c r="A130" t="inlineStr"/>
-      <c r="B130" t="inlineStr"/>
-      <c r="C130" t="inlineStr"/>
-      <c r="D130" t="inlineStr"/>
-      <c r="E130" t="inlineStr">
-        <is>
-          <t>11)</t>
-        </is>
-      </c>
-      <c r="F130" t="inlineStr">
-        <is>
-          <t>Nate</t>
-        </is>
-      </c>
-      <c r="G130" t="inlineStr">
-        <is>
-          <t>Driver, 1/2
-Gray Van</t>
-        </is>
-      </c>
-      <c r="H130" t="inlineStr"/>
-      <c r="I130" t="inlineStr"/>
-      <c r="J130" t="inlineStr"/>
-      <c r="K130" t="inlineStr"/>
-      <c r="L130" t="inlineStr"/>
-      <c r="M130" t="inlineStr"/>
-      <c r="N130" t="inlineStr"/>
-      <c r="O130" t="inlineStr"/>
-      <c r="P130" t="inlineStr"/>
-      <c r="Q130" t="inlineStr"/>
-      <c r="R130" t="inlineStr"/>
-      <c r="S130" t="inlineStr"/>
-      <c r="T130" t="inlineStr"/>
-      <c r="U130" t="inlineStr"/>
-      <c r="V130" t="inlineStr"/>
-      <c r="W130" t="inlineStr"/>
-      <c r="X130" t="inlineStr"/>
-      <c r="Y130" t="inlineStr"/>
-    </row>
-    <row r="131">
-      <c r="A131" t="inlineStr"/>
-      <c r="B131" t="inlineStr"/>
-      <c r="C131" t="inlineStr"/>
-      <c r="D131" t="inlineStr"/>
-      <c r="E131" t="inlineStr">
-        <is>
-          <t>12)</t>
-        </is>
-      </c>
-      <c r="F131" t="inlineStr">
-        <is>
-          <t>Taylor</t>
-        </is>
-      </c>
-      <c r="G131" t="inlineStr"/>
-      <c r="H131" t="inlineStr"/>
-      <c r="I131" t="inlineStr"/>
-      <c r="J131" t="inlineStr"/>
-      <c r="K131" t="inlineStr"/>
-      <c r="L131" t="inlineStr"/>
-      <c r="M131" t="inlineStr"/>
-      <c r="N131" t="inlineStr"/>
-      <c r="O131" t="inlineStr"/>
-      <c r="P131" t="inlineStr"/>
-      <c r="Q131" t="inlineStr"/>
-      <c r="R131" t="inlineStr"/>
-      <c r="S131" t="inlineStr"/>
-      <c r="T131" t="inlineStr"/>
-      <c r="U131" t="inlineStr"/>
-      <c r="V131" t="inlineStr"/>
-      <c r="W131" t="inlineStr"/>
-      <c r="X131" t="inlineStr"/>
-      <c r="Y131" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
save pw as string
</commit_message>
<xml_diff>
--- a/Copy of 06-23-24 to 06-29-24 Full Shedule.xlsx
+++ b/Copy of 06-23-24 to 06-29-24 Full Shedule.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y119"/>
+  <dimension ref="A1:Y116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5318,11 +5318,20 @@
       <c r="C98" t="inlineStr"/>
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr"/>
-      <c r="F98" t="inlineStr"/>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>IL: 4:15 AM MEET AT OFFICE</t>
+        </is>
+      </c>
       <c r="G98" t="inlineStr"/>
       <c r="H98" t="inlineStr"/>
       <c r="I98" t="inlineStr"/>
-      <c r="J98" t="inlineStr"/>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>IL: 4:00 AM MEET AT OFFICE
+MD: 4:45 MEET HOME DEPOT VERONA RD</t>
+        </is>
+      </c>
       <c r="K98" t="inlineStr"/>
       <c r="L98" t="inlineStr"/>
       <c r="M98" t="inlineStr"/>
@@ -5358,14 +5367,17 @@
       <c r="C99" t="inlineStr"/>
       <c r="D99" t="inlineStr"/>
       <c r="E99" t="inlineStr"/>
-      <c r="F99" t="inlineStr"/>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>6:00 AM START</t>
+        </is>
+      </c>
       <c r="G99" t="inlineStr"/>
       <c r="H99" t="inlineStr"/>
       <c r="I99" t="inlineStr"/>
       <c r="J99" t="inlineStr">
         <is>
-          <t>IL: 4:00 AM MEET AT OFFICE
-MD: 4:45 MEET HOME DEPOT VERONA RD</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="K99" t="inlineStr"/>
@@ -5403,13 +5415,17 @@
       <c r="C100" t="inlineStr"/>
       <c r="D100" t="inlineStr"/>
       <c r="E100" t="inlineStr"/>
-      <c r="F100" t="inlineStr"/>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>DC5-FINANCIAL</t>
+        </is>
+      </c>
       <c r="G100" t="inlineStr"/>
       <c r="H100" t="inlineStr"/>
       <c r="I100" t="inlineStr"/>
       <c r="J100" t="inlineStr">
         <is>
-          <t>6:00 AM START</t>
+          <t>DC5-ITEM LEVEL</t>
         </is>
       </c>
       <c r="K100" t="inlineStr"/>
@@ -5436,7 +5452,7 @@
       <c r="E101" t="inlineStr"/>
       <c r="F101" t="inlineStr">
         <is>
-          <t>IL: 4:15 AM MEET AT OFFICE</t>
+          <t>PIERCE'S EXPRESS MARKET, BARABOO (GROC + C-STORE)</t>
         </is>
       </c>
       <c r="G101" t="inlineStr"/>
@@ -5444,7 +5460,7 @@
       <c r="I101" t="inlineStr"/>
       <c r="J101" t="inlineStr">
         <is>
-          <t>DC5-ITEM LEVEL</t>
+          <t>SOUTHWEST HEALTH HOSPITAL-INPATIENT, PLATTEVILLE</t>
         </is>
       </c>
       <c r="K101" t="inlineStr"/>
@@ -5471,7 +5487,7 @@
       <c r="E102" t="inlineStr"/>
       <c r="F102" t="inlineStr">
         <is>
-          <t>6:00 AM START</t>
+          <t>935 8TH ST</t>
         </is>
       </c>
       <c r="G102" t="inlineStr"/>
@@ -5479,7 +5495,7 @@
       <c r="I102" t="inlineStr"/>
       <c r="J102" t="inlineStr">
         <is>
-          <t>SOUTHWEST HEALTH HOSPITAL-INPATIENT, PLATTEVILLE</t>
+          <t>1400 EASTSIDE RD</t>
         </is>
       </c>
       <c r="K102" t="inlineStr"/>
@@ -5506,7 +5522,7 @@
       <c r="E103" t="inlineStr"/>
       <c r="F103" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>https://goo.gl/maps/GhH3B9P8DGn</t>
         </is>
       </c>
       <c r="G103" t="inlineStr"/>
@@ -5514,7 +5530,7 @@
       <c r="I103" t="inlineStr"/>
       <c r="J103" t="inlineStr">
         <is>
-          <t>1400 EASTSIDE RD</t>
+          <t>https://goo.gl/maps/tENERhYm35H2</t>
         </is>
       </c>
       <c r="K103" t="inlineStr"/>
@@ -5539,17 +5555,13 @@
       <c r="C104" t="inlineStr"/>
       <c r="D104" t="inlineStr"/>
       <c r="E104" t="inlineStr"/>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>PIERCE'S EXPRESS MARKET, BARABOO (GROC + C-STORE)</t>
-        </is>
-      </c>
+      <c r="F104" t="inlineStr"/>
       <c r="G104" t="inlineStr"/>
       <c r="H104" t="inlineStr"/>
       <c r="I104" t="inlineStr"/>
       <c r="J104" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/tENERhYm35H2</t>
+          <t>TO FOLLOW</t>
         </is>
       </c>
       <c r="K104" t="inlineStr"/>
@@ -5573,18 +5585,26 @@
       <c r="B105" t="inlineStr"/>
       <c r="C105" t="inlineStr"/>
       <c r="D105" t="inlineStr"/>
-      <c r="E105" t="inlineStr"/>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>935 8TH ST</t>
-        </is>
-      </c>
-      <c r="G105" t="inlineStr"/>
+          <t>Sarah</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>@ Store, Equip</t>
+        </is>
+      </c>
       <c r="H105" t="inlineStr"/>
       <c r="I105" t="inlineStr"/>
       <c r="J105" t="inlineStr">
         <is>
-          <t>TO FOLLOW</t>
+          <t>DC5-ITEM LEVEL</t>
         </is>
       </c>
       <c r="K105" t="inlineStr"/>
@@ -5608,18 +5628,27 @@
       <c r="B106" t="inlineStr"/>
       <c r="C106" t="inlineStr"/>
       <c r="D106" t="inlineStr"/>
-      <c r="E106" t="inlineStr"/>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/GhH3B9P8DGn</t>
-        </is>
-      </c>
-      <c r="G106" t="inlineStr"/>
+          <t>Angela</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>Driver, 1/2
+Silver Van</t>
+        </is>
+      </c>
       <c r="H106" t="inlineStr"/>
       <c r="I106" t="inlineStr"/>
       <c r="J106" t="inlineStr">
         <is>
-          <t>DC5-ITEM LEVEL</t>
+          <t>SOUTHWEST HEALTH HOSPITAL-OUTPATIENT, PLATTEVILLE</t>
         </is>
       </c>
       <c r="K106" t="inlineStr"/>
@@ -5643,14 +5672,22 @@
       <c r="B107" t="inlineStr"/>
       <c r="C107" t="inlineStr"/>
       <c r="D107" t="inlineStr"/>
-      <c r="E107" t="inlineStr"/>
-      <c r="F107" t="inlineStr"/>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>3)</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Anisha</t>
+        </is>
+      </c>
       <c r="G107" t="inlineStr"/>
       <c r="H107" t="inlineStr"/>
       <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr">
         <is>
-          <t>SOUTHWEST HEALTH HOSPITAL-OUTPATIENT, PLATTEVILLE</t>
+          <t>1400 EASTSIDE RD</t>
         </is>
       </c>
       <c r="K107" t="inlineStr"/>
@@ -5676,24 +5713,25 @@
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr">
         <is>
-          <t>1)</t>
+          <t>4)</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Sarah</t>
+          <t>Ashley P</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>@ Store, Equip</t>
+          <t>Driver, 1/2
+Silver Van</t>
         </is>
       </c>
       <c r="H108" t="inlineStr"/>
       <c r="I108" t="inlineStr"/>
       <c r="J108" t="inlineStr">
         <is>
-          <t>1400 EASTSIDE RD</t>
+          <t>https://goo.gl/maps/ueV1odVEdtxrmE3m7</t>
         </is>
       </c>
       <c r="K108" t="inlineStr"/>
@@ -5719,27 +5757,18 @@
       <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>5)</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>Angela</t>
-        </is>
-      </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>Driver, 1/2
-Silver Van</t>
-        </is>
-      </c>
+          <t>Elijah</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr"/>
       <c r="H109" t="inlineStr"/>
       <c r="I109" t="inlineStr"/>
-      <c r="J109" t="inlineStr">
-        <is>
-          <t>https://goo.gl/maps/ueV1odVEdtxrmE3m7</t>
-        </is>
-      </c>
+      <c r="J109" t="inlineStr"/>
       <c r="K109" t="inlineStr"/>
       <c r="L109" t="inlineStr"/>
       <c r="M109" t="inlineStr"/>
@@ -5763,19 +5792,32 @@
       <c r="D110" t="inlineStr"/>
       <c r="E110" t="inlineStr">
         <is>
-          <t>3)</t>
+          <t>6)</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Anisha</t>
+          <t>Eva</t>
         </is>
       </c>
       <c r="G110" t="inlineStr"/>
       <c r="H110" t="inlineStr"/>
-      <c r="I110" t="inlineStr"/>
-      <c r="J110" t="inlineStr"/>
-      <c r="K110" t="inlineStr"/>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>Sarah</t>
+        </is>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>Driver,
+Equip</t>
+        </is>
+      </c>
       <c r="L110" t="inlineStr"/>
       <c r="M110" t="inlineStr"/>
       <c r="N110" t="inlineStr"/>
@@ -5798,35 +5840,30 @@
       <c r="D111" t="inlineStr"/>
       <c r="E111" t="inlineStr">
         <is>
-          <t>4)</t>
+          <t>7)</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
+          <t>Evelin</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr"/>
+      <c r="H111" t="inlineStr"/>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
           <t>Ashley P</t>
         </is>
       </c>
-      <c r="G111" t="inlineStr">
+      <c r="K111" t="inlineStr">
         <is>
           <t>Driver, 1/2
 Silver Van</t>
-        </is>
-      </c>
-      <c r="H111" t="inlineStr"/>
-      <c r="I111" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
-      <c r="J111" t="inlineStr">
-        <is>
-          <t>Sarah</t>
-        </is>
-      </c>
-      <c r="K111" t="inlineStr">
-        <is>
-          <t>Driver,
-Equip</t>
         </is>
       </c>
       <c r="L111" t="inlineStr"/>
@@ -5851,32 +5888,27 @@
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="inlineStr">
         <is>
-          <t>5)</t>
+          <t>8)</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Elijah</t>
+          <t>Joseph</t>
         </is>
       </c>
       <c r="G112" t="inlineStr"/>
       <c r="H112" t="inlineStr"/>
       <c r="I112" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>3)</t>
         </is>
       </c>
       <c r="J112" t="inlineStr">
         <is>
-          <t>Ashley P</t>
-        </is>
-      </c>
-      <c r="K112" t="inlineStr">
-        <is>
-          <t>Driver, 1/2
-Silver Van</t>
-        </is>
-      </c>
+          <t>Eva</t>
+        </is>
+      </c>
+      <c r="K112" t="inlineStr"/>
       <c r="L112" t="inlineStr"/>
       <c r="M112" t="inlineStr"/>
       <c r="N112" t="inlineStr"/>
@@ -5899,24 +5931,24 @@
       <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr">
         <is>
-          <t>6)</t>
+          <t>9)</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>Eva</t>
+          <t>Justin</t>
         </is>
       </c>
       <c r="G113" t="inlineStr"/>
       <c r="H113" t="inlineStr"/>
       <c r="I113" t="inlineStr">
         <is>
-          <t>3)</t>
+          <t>4)</t>
         </is>
       </c>
       <c r="J113" t="inlineStr">
         <is>
-          <t>Eva</t>
+          <t>Josie</t>
         </is>
       </c>
       <c r="K113" t="inlineStr"/>
@@ -5942,24 +5974,29 @@
       <c r="D114" t="inlineStr"/>
       <c r="E114" t="inlineStr">
         <is>
-          <t>7)</t>
+          <t>10)</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>Evelin</t>
-        </is>
-      </c>
-      <c r="G114" t="inlineStr"/>
+          <t>Michael N</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>Driver, 1/2
+Gray Van</t>
+        </is>
+      </c>
       <c r="H114" t="inlineStr"/>
       <c r="I114" t="inlineStr">
         <is>
-          <t>4)</t>
+          <t>5)</t>
         </is>
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>Josie</t>
+          <t>Lori</t>
         </is>
       </c>
       <c r="K114" t="inlineStr"/>
@@ -5985,27 +6022,37 @@
       <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr">
         <is>
-          <t>8)</t>
+          <t>11)</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>Joseph</t>
-        </is>
-      </c>
-      <c r="G115" t="inlineStr"/>
+          <t>Nate</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>Driver, 1/2
+Gray Van</t>
+        </is>
+      </c>
       <c r="H115" t="inlineStr"/>
       <c r="I115" t="inlineStr">
         <is>
-          <t>5)</t>
+          <t>6)</t>
         </is>
       </c>
       <c r="J115" t="inlineStr">
         <is>
-          <t>Lori</t>
-        </is>
-      </c>
-      <c r="K115" t="inlineStr"/>
+          <t>Michael N</t>
+        </is>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>Driver, 1/2
+Silver Van</t>
+        </is>
+      </c>
       <c r="L115" t="inlineStr"/>
       <c r="M115" t="inlineStr"/>
       <c r="N115" t="inlineStr"/>
@@ -6028,32 +6075,19 @@
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr">
         <is>
-          <t>9)</t>
+          <t>12)</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>Justin</t>
+          <t>Taylor</t>
         </is>
       </c>
       <c r="G116" t="inlineStr"/>
       <c r="H116" t="inlineStr"/>
-      <c r="I116" t="inlineStr">
-        <is>
-          <t>6)</t>
-        </is>
-      </c>
-      <c r="J116" t="inlineStr">
-        <is>
-          <t>Michael N</t>
-        </is>
-      </c>
-      <c r="K116" t="inlineStr">
-        <is>
-          <t>Driver, 1/2
-Silver Van</t>
-        </is>
-      </c>
+      <c r="I116" t="inlineStr"/>
+      <c r="J116" t="inlineStr"/>
+      <c r="K116" t="inlineStr"/>
       <c r="L116" t="inlineStr"/>
       <c r="M116" t="inlineStr"/>
       <c r="N116" t="inlineStr"/>
@@ -6069,121 +6103,6 @@
       <c r="X116" t="inlineStr"/>
       <c r="Y116" t="inlineStr"/>
     </row>
-    <row r="117">
-      <c r="A117" t="inlineStr"/>
-      <c r="B117" t="inlineStr"/>
-      <c r="C117" t="inlineStr"/>
-      <c r="D117" t="inlineStr"/>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>10)</t>
-        </is>
-      </c>
-      <c r="F117" t="inlineStr">
-        <is>
-          <t>Michael N</t>
-        </is>
-      </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>Driver, 1/2
-Gray Van</t>
-        </is>
-      </c>
-      <c r="H117" t="inlineStr"/>
-      <c r="I117" t="inlineStr"/>
-      <c r="J117" t="inlineStr"/>
-      <c r="K117" t="inlineStr"/>
-      <c r="L117" t="inlineStr"/>
-      <c r="M117" t="inlineStr"/>
-      <c r="N117" t="inlineStr"/>
-      <c r="O117" t="inlineStr"/>
-      <c r="P117" t="inlineStr"/>
-      <c r="Q117" t="inlineStr"/>
-      <c r="R117" t="inlineStr"/>
-      <c r="S117" t="inlineStr"/>
-      <c r="T117" t="inlineStr"/>
-      <c r="U117" t="inlineStr"/>
-      <c r="V117" t="inlineStr"/>
-      <c r="W117" t="inlineStr"/>
-      <c r="X117" t="inlineStr"/>
-      <c r="Y117" t="inlineStr"/>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr"/>
-      <c r="B118" t="inlineStr"/>
-      <c r="C118" t="inlineStr"/>
-      <c r="D118" t="inlineStr"/>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t>11)</t>
-        </is>
-      </c>
-      <c r="F118" t="inlineStr">
-        <is>
-          <t>Nate</t>
-        </is>
-      </c>
-      <c r="G118" t="inlineStr">
-        <is>
-          <t>Driver, 1/2
-Gray Van</t>
-        </is>
-      </c>
-      <c r="H118" t="inlineStr"/>
-      <c r="I118" t="inlineStr"/>
-      <c r="J118" t="inlineStr"/>
-      <c r="K118" t="inlineStr"/>
-      <c r="L118" t="inlineStr"/>
-      <c r="M118" t="inlineStr"/>
-      <c r="N118" t="inlineStr"/>
-      <c r="O118" t="inlineStr"/>
-      <c r="P118" t="inlineStr"/>
-      <c r="Q118" t="inlineStr"/>
-      <c r="R118" t="inlineStr"/>
-      <c r="S118" t="inlineStr"/>
-      <c r="T118" t="inlineStr"/>
-      <c r="U118" t="inlineStr"/>
-      <c r="V118" t="inlineStr"/>
-      <c r="W118" t="inlineStr"/>
-      <c r="X118" t="inlineStr"/>
-      <c r="Y118" t="inlineStr"/>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr"/>
-      <c r="B119" t="inlineStr"/>
-      <c r="C119" t="inlineStr"/>
-      <c r="D119" t="inlineStr"/>
-      <c r="E119" t="inlineStr">
-        <is>
-          <t>12)</t>
-        </is>
-      </c>
-      <c r="F119" t="inlineStr">
-        <is>
-          <t>Taylor</t>
-        </is>
-      </c>
-      <c r="G119" t="inlineStr"/>
-      <c r="H119" t="inlineStr"/>
-      <c r="I119" t="inlineStr"/>
-      <c r="J119" t="inlineStr"/>
-      <c r="K119" t="inlineStr"/>
-      <c r="L119" t="inlineStr"/>
-      <c r="M119" t="inlineStr"/>
-      <c r="N119" t="inlineStr"/>
-      <c r="O119" t="inlineStr"/>
-      <c r="P119" t="inlineStr"/>
-      <c r="Q119" t="inlineStr"/>
-      <c r="R119" t="inlineStr"/>
-      <c r="S119" t="inlineStr"/>
-      <c r="T119" t="inlineStr"/>
-      <c r="U119" t="inlineStr"/>
-      <c r="V119" t="inlineStr"/>
-      <c r="W119" t="inlineStr"/>
-      <c r="X119" t="inlineStr"/>
-      <c r="Y119" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
search must inlcude full display name
</commit_message>
<xml_diff>
--- a/Copy of 06-23-24 to 06-29-24 Full Shedule.xlsx
+++ b/Copy of 06-23-24 to 06-29-24 Full Shedule.xlsx
@@ -909,7 +909,7 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
-          <t>5:30 am meet for Carlie/Trevor at Grafton Park n Ride</t>
+          <t>5:30 am meet for Carlie K/Trevor M at Grafton Park n Ride</t>
         </is>
       </c>
       <c r="K13" t="inlineStr"/>
@@ -949,7 +949,7 @@
       <c r="F14" t="inlineStr">
         <is>
           <t>SMALL CHANGES-RESET
-4:45 am meet for Carlie/Trevor at Grafton Park n Ride</t>
+4:45 am meet for Carlie K/Trevor M at Grafton Park n Ride</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
@@ -962,7 +962,7 @@
       <c r="N14" t="inlineStr">
         <is>
           <t xml:space="preserve">SET UP ON REG FAR RIGHT BY OFFICE
-5:15 am meet for Carlie/Trevor at Grafton Park n Ride	</t>
+5:15 am meet for Carlie K/Trevor M at Grafton Park n Ride	</t>
         </is>
       </c>
       <c r="O14" t="inlineStr"/>
@@ -970,7 +970,7 @@
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr">
         <is>
-          <t>4:45 am meet for Carlie/Trevor at Grafton Park n Ride</t>
+          <t>4:45 am meet for Carlie K/Trevor M at Grafton Park n Ride</t>
         </is>
       </c>
       <c r="S14" t="inlineStr"/>
@@ -997,7 +997,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Brianna</t>
+          <t>Brianna H</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>DJ</t>
+          <t>DJ S</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Kim G</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Aaron</t>
+          <t>Aaron M</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1077,7 +1077,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>Nate</t>
+          <t>Nate C</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>DJ</t>
+          <t>DJ S</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
@@ -1110,7 +1110,7 @@
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>Aaron</t>
+          <t>Aaron M</t>
         </is>
       </c>
       <c r="W16" t="inlineStr"/>
@@ -1129,13 +1129,13 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Carlie</t>
+          <t>Carlie K</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
           <t>@ Store
-(w/ Trevor)</t>
+(w/ Trevor M)</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
@@ -1146,13 +1146,13 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Carlie</t>
+          <t>Carlie K</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
           <t>@ Store
-(w/ Trevor)</t>
+(w/ Trevor M)</t>
         </is>
       </c>
       <c r="L17" t="inlineStr"/>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>Aaron</t>
+          <t>Aaron M</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -1179,13 +1179,13 @@
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>Carlie</t>
+          <t>Carlie K</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
         <is>
           <t>@ Store
-(w/ Trevor)</t>
+(w/ Trevor M)</t>
         </is>
       </c>
       <c r="T17" t="inlineStr"/>
@@ -1196,7 +1196,7 @@
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>Greg</t>
+          <t>Greg H</t>
         </is>
       </c>
       <c r="W17" t="inlineStr"/>
@@ -1215,7 +1215,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Curt</t>
+          <t>Curt B</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Greg</t>
+          <t>Greg H</t>
         </is>
       </c>
       <c r="K18" t="inlineStr"/>
@@ -1239,13 +1239,13 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>Carlie</t>
+          <t>Carlie K</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
           <t>@ Store
-(w/ Trevor)</t>
+(w/ Trevor M)</t>
         </is>
       </c>
       <c r="P18" t="inlineStr"/>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>Monica</t>
+          <t>Monica G</t>
         </is>
       </c>
       <c r="S18" t="inlineStr"/>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Cynthia</t>
+          <t>Cynthia M</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
@@ -1299,7 +1299,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Monica</t>
+          <t>Monica G</t>
         </is>
       </c>
       <c r="K19" t="inlineStr"/>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>Cynthia</t>
+          <t>Cynthia M</t>
         </is>
       </c>
       <c r="O19" t="inlineStr"/>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>Stephanie</t>
+          <t>Stephanie G</t>
         </is>
       </c>
       <c r="S19" t="inlineStr"/>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>Sonia</t>
+          <t>Sonia T</t>
         </is>
       </c>
       <c r="W19" t="inlineStr"/>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Greg</t>
+          <t>Greg H</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Robyn</t>
+          <t>Robyn K</t>
         </is>
       </c>
       <c r="K20" t="inlineStr"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>Greg</t>
+          <t>Greg H</t>
         </is>
       </c>
       <c r="O20" t="inlineStr"/>
@@ -1390,13 +1390,13 @@
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Trevor M</t>
         </is>
       </c>
       <c r="S20" t="inlineStr">
         <is>
           <t>@ Store
-(w/ Carlie)</t>
+(w/ Carlie K)</t>
         </is>
       </c>
       <c r="T20" t="inlineStr"/>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Robyn</t>
+          <t>Robyn K</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
@@ -1443,7 +1443,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Sonia</t>
+          <t>Sonia T</t>
         </is>
       </c>
       <c r="K21" t="inlineStr"/>
@@ -1455,7 +1455,7 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>Mai</t>
+          <t>Mai M</t>
         </is>
       </c>
       <c r="O21" t="inlineStr"/>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>Evelin</t>
+          <t>Evelin A</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
@@ -1495,7 +1495,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Sonia</t>
+          <t>Sonia T</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Stephanie</t>
+          <t>Stephanie G</t>
         </is>
       </c>
       <c r="K22" t="inlineStr"/>
@@ -1519,7 +1519,7 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>Monica</t>
+          <t>Monica G</t>
         </is>
       </c>
       <c r="O22" t="inlineStr"/>
@@ -1535,7 +1535,7 @@
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>Qiana</t>
+          <t>Qiana B</t>
         </is>
       </c>
       <c r="W22" t="inlineStr"/>
@@ -1554,13 +1554,13 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Trevor M</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
           <t>@ Store
-(w/ Carlie)</t>
+(w/ Carlie K)</t>
         </is>
       </c>
       <c r="H23" t="inlineStr"/>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Sue M</t>
         </is>
       </c>
       <c r="K23" t="inlineStr"/>
@@ -1583,7 +1583,7 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Paul T</t>
         </is>
       </c>
       <c r="O23" t="inlineStr"/>
@@ -1618,13 +1618,13 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Trevor M</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
           <t>@ Store
-(w/ Carlie)</t>
+(w/ Carlie K)</t>
         </is>
       </c>
       <c r="L24" t="inlineStr"/>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>Sonia</t>
+          <t>Sonia T</t>
         </is>
       </c>
       <c r="O24" t="inlineStr"/>
@@ -1674,7 +1674,7 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>Stephanie</t>
+          <t>Stephanie G</t>
         </is>
       </c>
       <c r="O25" t="inlineStr"/>
@@ -1721,13 +1721,13 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>Trevor</t>
+          <t>Trevor M</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
           <t>@ Store
-(w/ Carlie)</t>
+(w/ Carlie K)</t>
         </is>
       </c>
       <c r="P26" t="inlineStr"/>
@@ -1777,7 +1777,7 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>Angela</t>
+          <t>Angela B</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
@@ -1834,7 +1834,7 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>Anisha</t>
+          <t>Anisha V</t>
         </is>
       </c>
       <c r="O28" t="inlineStr"/>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>Brianna</t>
+          <t>Brianna H</t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
@@ -1932,7 +1932,7 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>Evelin</t>
+          <t>Evelin A</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
@@ -1949,7 +1949,7 @@
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>Brianna</t>
+          <t>Brianna H</t>
         </is>
       </c>
       <c r="S30" t="inlineStr">
@@ -1996,7 +1996,7 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>Joseph</t>
+          <t>Joseph S</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
@@ -2008,7 +2008,7 @@
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>Casey</t>
+          <t>Casey V</t>
         </is>
       </c>
       <c r="S31" t="inlineStr"/>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>Justin</t>
+          <t>Justin L</t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
@@ -2059,7 +2059,7 @@
       </c>
       <c r="R32" t="inlineStr">
         <is>
-          <t>Lashaun</t>
+          <t>Lashaun C</t>
         </is>
       </c>
       <c r="S32" t="inlineStr">
@@ -2076,7 +2076,7 @@
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>Nate</t>
+          <t>Nate C</t>
         </is>
       </c>
       <c r="W32" t="inlineStr">
@@ -2132,7 +2132,7 @@
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>Lori</t>
+          <t>Lori N</t>
         </is>
       </c>
       <c r="S33" t="inlineStr"/>
@@ -2144,7 +2144,7 @@
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Kim G</t>
         </is>
       </c>
       <c r="W33" t="inlineStr">
@@ -2180,7 +2180,7 @@
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>Qiana</t>
+          <t>Qiana B</t>
         </is>
       </c>
       <c r="O34" t="inlineStr">
@@ -2202,7 +2202,7 @@
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>Lori</t>
+          <t>Lori N</t>
         </is>
       </c>
       <c r="W34" t="inlineStr"/>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Kim G</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -2246,7 +2246,7 @@
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>Taylor</t>
+          <t>Taylor G</t>
         </is>
       </c>
       <c r="O35" t="inlineStr"/>
@@ -2281,7 +2281,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Cynthia</t>
+          <t>Cynthia M</t>
         </is>
       </c>
       <c r="K36" t="inlineStr"/>
@@ -2320,7 +2320,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Mai</t>
+          <t>Mai M</t>
         </is>
       </c>
       <c r="K37" t="inlineStr"/>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Ian</t>
+          <t>Ian K</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -2411,7 +2411,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Paul T</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="R43" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Kim G</t>
         </is>
       </c>
       <c r="S43" t="inlineStr">
@@ -2671,7 +2671,7 @@
       </c>
       <c r="R44" t="inlineStr">
         <is>
-          <t>Cynthia</t>
+          <t>Cynthia M</t>
         </is>
       </c>
       <c r="S44" t="inlineStr"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>Lashaun</t>
+          <t>Lashaun C</t>
         </is>
       </c>
       <c r="W44" t="inlineStr">
@@ -2731,7 +2731,7 @@
       </c>
       <c r="R45" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Paul T</t>
         </is>
       </c>
       <c r="S45" t="inlineStr"/>
@@ -2743,7 +2743,7 @@
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t>Carlie</t>
+          <t>Carlie K</t>
         </is>
       </c>
       <c r="W45" t="inlineStr">
@@ -2790,7 +2790,7 @@
       </c>
       <c r="R46" t="inlineStr">
         <is>
-          <t>Sonia</t>
+          <t>Sonia T</t>
         </is>
       </c>
       <c r="S46" t="inlineStr"/>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="V46" t="inlineStr">
         <is>
-          <t>Casey</t>
+          <t>Casey V</t>
         </is>
       </c>
       <c r="W46" t="inlineStr"/>
@@ -2849,7 +2849,7 @@
       </c>
       <c r="V47" t="inlineStr">
         <is>
-          <t>Stephanie</t>
+          <t>Stephanie G</t>
         </is>
       </c>
       <c r="W47" t="inlineStr"/>
@@ -3048,7 +3048,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Ian</t>
+          <t>Ian K</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -3100,7 +3100,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Paul T</t>
         </is>
       </c>
       <c r="K53" t="inlineStr"/>
@@ -3112,7 +3112,7 @@
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>Katherine</t>
+          <t>Katherine G</t>
         </is>
       </c>
       <c r="O53" t="inlineStr">
@@ -3163,7 +3163,7 @@
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>Ian</t>
+          <t>Ian K</t>
         </is>
       </c>
       <c r="O54" t="inlineStr"/>
@@ -3261,7 +3261,7 @@
       </c>
       <c r="V56" t="inlineStr">
         <is>
-          <t>Katherine</t>
+          <t>Katherine G</t>
         </is>
       </c>
       <c r="W56" t="inlineStr">
@@ -3316,7 +3316,7 @@
       </c>
       <c r="V57" t="inlineStr">
         <is>
-          <t>Cynthia</t>
+          <t>Cynthia M</t>
         </is>
       </c>
       <c r="W57" t="inlineStr"/>
@@ -3363,7 +3363,7 @@
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t>Mai</t>
+          <t>Mai M</t>
         </is>
       </c>
       <c r="W58" t="inlineStr"/>
@@ -3382,7 +3382,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Katherine</t>
+          <t>Katherine G</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -3422,7 +3422,7 @@
       </c>
       <c r="V59" t="inlineStr">
         <is>
-          <t>Monica</t>
+          <t>Monica G</t>
         </is>
       </c>
       <c r="W59" t="inlineStr"/>
@@ -3441,7 +3441,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Sue M</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="R61" t="inlineStr">
         <is>
-          <t>Katherine</t>
+          <t>Katherine G</t>
         </is>
       </c>
       <c r="S61" t="inlineStr">
@@ -3556,7 +3556,7 @@
       </c>
       <c r="R62" t="inlineStr">
         <is>
-          <t>Ian</t>
+          <t>Ian K</t>
         </is>
       </c>
       <c r="S62" t="inlineStr">
@@ -3703,7 +3703,7 @@
       <c r="U65" t="inlineStr"/>
       <c r="V65" t="inlineStr">
         <is>
-          <t>ROTE OIL #14 TREVOR (CITGO)</t>
+          <t>ROTE OIL #14 Trevor M (CITGO)</t>
         </is>
       </c>
       <c r="W65" t="inlineStr"/>
@@ -3938,7 +3938,7 @@
       <c r="U70" t="inlineStr"/>
       <c r="V70" t="inlineStr">
         <is>
-          <t>ROTE OIL #13 TREVOR (BP)</t>
+          <t>ROTE OIL #13 Trevor M (BP)</t>
         </is>
       </c>
       <c r="W70" t="inlineStr"/>
@@ -4024,7 +4024,7 @@
       </c>
       <c r="R72" t="inlineStr">
         <is>
-          <t>Nate</t>
+          <t>Nate C</t>
         </is>
       </c>
       <c r="S72" t="inlineStr">
@@ -4075,7 +4075,7 @@
       </c>
       <c r="R73" t="inlineStr">
         <is>
-          <t>Curt</t>
+          <t>Curt B</t>
         </is>
       </c>
       <c r="S73" t="inlineStr"/>
@@ -4110,7 +4110,7 @@
       </c>
       <c r="N74" t="inlineStr">
         <is>
-          <t>Sarah</t>
+          <t>Sarah H</t>
         </is>
       </c>
       <c r="O74" t="inlineStr">
@@ -4139,7 +4139,7 @@
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>Ian</t>
+          <t>Ian K</t>
         </is>
       </c>
       <c r="W74" t="inlineStr">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>DJ</t>
+          <t>DJ S</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -4205,7 +4205,7 @@
       </c>
       <c r="R75" t="inlineStr">
         <is>
-          <t>Robyn</t>
+          <t>Robyn K</t>
         </is>
       </c>
       <c r="S75" t="inlineStr"/>
@@ -4217,7 +4217,7 @@
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Paul T</t>
         </is>
       </c>
       <c r="W75" t="inlineStr"/>
@@ -4236,7 +4236,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Mai</t>
+          <t>Mai M</t>
         </is>
       </c>
       <c r="G76" t="inlineStr"/>
@@ -4252,7 +4252,7 @@
       </c>
       <c r="N76" t="inlineStr">
         <is>
-          <t>Eva</t>
+          <t>Eva G</t>
         </is>
       </c>
       <c r="O76" t="inlineStr"/>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="R76" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Sue M</t>
         </is>
       </c>
       <c r="S76" t="inlineStr">
@@ -4296,7 +4296,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>Katherine</t>
+          <t>Katherine G</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -4312,7 +4312,7 @@
       </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>Lori</t>
+          <t>Lori N</t>
         </is>
       </c>
       <c r="O77" t="inlineStr">
@@ -4328,7 +4328,7 @@
       </c>
       <c r="R77" t="inlineStr">
         <is>
-          <t>Evelin</t>
+          <t>Evelin A</t>
         </is>
       </c>
       <c r="S77" t="inlineStr">
@@ -4364,7 +4364,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Casey</t>
+          <t>Casey V</t>
         </is>
       </c>
       <c r="K78" t="inlineStr"/>
@@ -4380,7 +4380,7 @@
       </c>
       <c r="R78" t="inlineStr">
         <is>
-          <t>Jeri</t>
+          <t>Jeri H</t>
         </is>
       </c>
       <c r="S78" t="inlineStr">
@@ -4407,7 +4407,7 @@
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr">
         <is>
-          <t>IL: 4:40 MEET AT JANESVILLE PARK N RIDE</t>
+          <t>IL: 4:40 AM MEET AT JANESVILLE PARK N RIDE</t>
         </is>
       </c>
       <c r="G79" t="inlineStr"/>
@@ -4419,7 +4419,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Lashaun</t>
+          <t>Lashaun C</t>
         </is>
       </c>
       <c r="K79" t="inlineStr"/>
@@ -4435,7 +4435,7 @@
       </c>
       <c r="R79" t="inlineStr">
         <is>
-          <t>Justin</t>
+          <t>Justin L</t>
         </is>
       </c>
       <c r="S79" t="inlineStr">
@@ -4530,7 +4530,7 @@
       <c r="M81" t="inlineStr"/>
       <c r="N81" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Kim G</t>
         </is>
       </c>
       <c r="O81" t="inlineStr"/>
@@ -4542,7 +4542,7 @@
       </c>
       <c r="R81" t="inlineStr">
         <is>
-          <t>Taylor</t>
+          <t>Taylor G</t>
         </is>
       </c>
       <c r="S81" t="inlineStr"/>
@@ -4581,7 +4581,7 @@
       <c r="M82" t="inlineStr"/>
       <c r="N82" t="inlineStr">
         <is>
-          <t>Lashaun</t>
+          <t>Lashaun C</t>
         </is>
       </c>
       <c r="O82" t="inlineStr"/>
@@ -4866,7 +4866,7 @@
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>Nate</t>
+          <t>Nate C</t>
         </is>
       </c>
       <c r="K89" t="inlineStr">
@@ -4896,7 +4896,7 @@
       </c>
       <c r="V89" t="inlineStr">
         <is>
-          <t>Sarah</t>
+          <t>Sarah H</t>
         </is>
       </c>
       <c r="W89" t="inlineStr">
@@ -4928,7 +4928,7 @@
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>Angela</t>
+          <t>Angela B</t>
         </is>
       </c>
       <c r="K90" t="inlineStr"/>
@@ -4948,7 +4948,7 @@
       </c>
       <c r="V90" t="inlineStr">
         <is>
-          <t>Brianna</t>
+          <t>Brianna H</t>
         </is>
       </c>
       <c r="W90" t="inlineStr">
@@ -4975,7 +4975,7 @@
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>Anisha</t>
+          <t>Anisha V</t>
         </is>
       </c>
       <c r="K91" t="inlineStr"/>
@@ -4991,7 +4991,7 @@
       </c>
       <c r="R91" t="inlineStr">
         <is>
-          <t>Sarah</t>
+          <t>Sarah H</t>
         </is>
       </c>
       <c r="S91" t="inlineStr">
@@ -5018,7 +5018,7 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Brianna</t>
+          <t>Brianna H</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
@@ -5035,7 +5035,7 @@
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>Elijah</t>
+          <t>Elijah E</t>
         </is>
       </c>
       <c r="K92" t="inlineStr"/>
@@ -5051,7 +5051,7 @@
       </c>
       <c r="R92" t="inlineStr">
         <is>
-          <t>Angela</t>
+          <t>Angela B</t>
         </is>
       </c>
       <c r="S92" t="inlineStr">
@@ -5079,7 +5079,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Josie</t>
+          <t>Josie N</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
@@ -5095,7 +5095,7 @@
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>Evelin</t>
+          <t>Evelin A</t>
         </is>
       </c>
       <c r="K93" t="inlineStr">
@@ -5116,7 +5116,7 @@
       </c>
       <c r="R93" t="inlineStr">
         <is>
-          <t>Anisha</t>
+          <t>Anisha V</t>
         </is>
       </c>
       <c r="S93" t="inlineStr"/>
@@ -5139,7 +5139,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Lori</t>
+          <t>Lori N</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
@@ -5155,7 +5155,7 @@
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>Joseph</t>
+          <t>Joseph S</t>
         </is>
       </c>
       <c r="K94" t="inlineStr"/>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Qiana</t>
+          <t>Qiana B</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
@@ -5215,7 +5215,7 @@
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>Taylor</t>
+          <t>Taylor G</t>
         </is>
       </c>
       <c r="K95" t="inlineStr"/>
@@ -5231,7 +5231,7 @@
       </c>
       <c r="R95" t="inlineStr">
         <is>
-          <t>Elijah</t>
+          <t>Elijah E</t>
         </is>
       </c>
       <c r="S95" t="inlineStr"/>
@@ -5266,7 +5266,7 @@
       </c>
       <c r="R96" t="inlineStr">
         <is>
-          <t>Eva</t>
+          <t>Eva G</t>
         </is>
       </c>
       <c r="S96" t="inlineStr"/>
@@ -5301,7 +5301,7 @@
       </c>
       <c r="R97" t="inlineStr">
         <is>
-          <t>Joseph</t>
+          <t>Joseph S</t>
         </is>
       </c>
       <c r="S97" t="inlineStr"/>
@@ -5393,7 +5393,7 @@
       </c>
       <c r="R99" t="inlineStr">
         <is>
-          <t>Qiana</t>
+          <t>Qiana B</t>
         </is>
       </c>
       <c r="S99" t="inlineStr">
@@ -5592,7 +5592,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Sarah</t>
+          <t>Sarah H</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
@@ -5635,7 +5635,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Angela</t>
+          <t>Angela B</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
@@ -5679,7 +5679,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Anisha</t>
+          <t>Anisha V</t>
         </is>
       </c>
       <c r="G107" t="inlineStr"/>
@@ -5762,7 +5762,7 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>Elijah</t>
+          <t>Elijah E</t>
         </is>
       </c>
       <c r="G109" t="inlineStr"/>
@@ -5797,7 +5797,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Eva</t>
+          <t>Eva G</t>
         </is>
       </c>
       <c r="G110" t="inlineStr"/>
@@ -5809,7 +5809,7 @@
       </c>
       <c r="J110" t="inlineStr">
         <is>
-          <t>Sarah</t>
+          <t>Sarah H</t>
         </is>
       </c>
       <c r="K110" t="inlineStr">
@@ -5845,7 +5845,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Evelin</t>
+          <t>Evelin A</t>
         </is>
       </c>
       <c r="G111" t="inlineStr"/>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Joseph</t>
+          <t>Joseph S</t>
         </is>
       </c>
       <c r="G112" t="inlineStr"/>
@@ -5905,7 +5905,7 @@
       </c>
       <c r="J112" t="inlineStr">
         <is>
-          <t>Eva</t>
+          <t>Eva G</t>
         </is>
       </c>
       <c r="K112" t="inlineStr"/>
@@ -5936,7 +5936,7 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>Justin</t>
+          <t>Justin L</t>
         </is>
       </c>
       <c r="G113" t="inlineStr"/>
@@ -5948,7 +5948,7 @@
       </c>
       <c r="J113" t="inlineStr">
         <is>
-          <t>Josie</t>
+          <t>Josie N</t>
         </is>
       </c>
       <c r="K113" t="inlineStr"/>
@@ -5996,7 +5996,7 @@
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>Lori</t>
+          <t>Lori N</t>
         </is>
       </c>
       <c r="K114" t="inlineStr"/>
@@ -6027,7 +6027,7 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>Nate</t>
+          <t>Nate C</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
@@ -6080,7 +6080,7 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>Taylor</t>
+          <t>Taylor G</t>
         </is>
       </c>
       <c r="G116" t="inlineStr"/>

</xml_diff>

<commit_message>
full meet times complete
</commit_message>
<xml_diff>
--- a/Copy of 06-23-24 to 06-29-24 Full Shedule.xlsx
+++ b/Copy of 06-23-24 to 06-29-24 Full Shedule.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y129"/>
+  <dimension ref="A1:Y160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4530,7 +4530,7 @@
       <c r="M81" t="inlineStr"/>
       <c r="N81" t="inlineStr">
         <is>
-          <t>Office</t>
+          <t>FV: 6:00 AM MEET BALLARD</t>
         </is>
       </c>
       <c r="O81" t="inlineStr"/>
@@ -4581,7 +4581,7 @@
       <c r="M82" t="inlineStr"/>
       <c r="N82" t="inlineStr">
         <is>
-          <t>Kim G</t>
+          <t>6:30 AM START</t>
         </is>
       </c>
       <c r="O82" t="inlineStr"/>
@@ -4624,7 +4624,7 @@
       <c r="M83" t="inlineStr"/>
       <c r="N83" t="inlineStr">
         <is>
-          <t>Lashaun C</t>
+          <t>MODAS</t>
         </is>
       </c>
       <c r="O83" t="inlineStr"/>
@@ -4665,7 +4665,11 @@
       <c r="K84" t="inlineStr"/>
       <c r="L84" t="inlineStr"/>
       <c r="M84" t="inlineStr"/>
-      <c r="N84" t="inlineStr"/>
+      <c r="N84" t="inlineStr">
+        <is>
+          <t>ONEIDA #2020 ONE STOP WESTWIND, GREEN BAY</t>
+        </is>
+      </c>
       <c r="O84" t="inlineStr"/>
       <c r="P84" t="inlineStr"/>
       <c r="Q84" t="inlineStr"/>
@@ -4708,7 +4712,11 @@
       <c r="K85" t="inlineStr"/>
       <c r="L85" t="inlineStr"/>
       <c r="M85" t="inlineStr"/>
-      <c r="N85" t="inlineStr"/>
+      <c r="N85" t="inlineStr">
+        <is>
+          <t>2370 WEST MASON ST</t>
+        </is>
+      </c>
       <c r="O85" t="inlineStr"/>
       <c r="P85" t="inlineStr"/>
       <c r="Q85" t="inlineStr"/>
@@ -4751,7 +4759,11 @@
       <c r="K86" t="inlineStr"/>
       <c r="L86" t="inlineStr"/>
       <c r="M86" t="inlineStr"/>
-      <c r="N86" t="inlineStr"/>
+      <c r="N86" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/eA3BF5KhAAp</t>
+        </is>
+      </c>
       <c r="O86" t="inlineStr"/>
       <c r="P86" t="inlineStr"/>
       <c r="Q86" t="inlineStr"/>
@@ -4794,7 +4806,11 @@
       <c r="K87" t="inlineStr"/>
       <c r="L87" t="inlineStr"/>
       <c r="M87" t="inlineStr"/>
-      <c r="N87" t="inlineStr"/>
+      <c r="N87" t="inlineStr">
+        <is>
+          <t>TO FOLLOW</t>
+        </is>
+      </c>
       <c r="O87" t="inlineStr"/>
       <c r="P87" t="inlineStr"/>
       <c r="Q87" t="inlineStr"/>
@@ -4833,7 +4849,11 @@
       <c r="K88" t="inlineStr"/>
       <c r="L88" t="inlineStr"/>
       <c r="M88" t="inlineStr"/>
-      <c r="N88" t="inlineStr"/>
+      <c r="N88" t="inlineStr">
+        <is>
+          <t>MODAS</t>
+        </is>
+      </c>
       <c r="O88" t="inlineStr"/>
       <c r="P88" t="inlineStr"/>
       <c r="Q88" t="inlineStr"/>
@@ -4882,7 +4902,11 @@
       </c>
       <c r="L89" t="inlineStr"/>
       <c r="M89" t="inlineStr"/>
-      <c r="N89" t="inlineStr"/>
+      <c r="N89" t="inlineStr">
+        <is>
+          <t>ONEIDA #2024 TRAVEL CENTER, PULASKI</t>
+        </is>
+      </c>
       <c r="O89" t="inlineStr"/>
       <c r="P89" t="inlineStr"/>
       <c r="Q89" t="inlineStr"/>
@@ -4938,7 +4962,11 @@
       <c r="K90" t="inlineStr"/>
       <c r="L90" t="inlineStr"/>
       <c r="M90" t="inlineStr"/>
-      <c r="N90" t="inlineStr"/>
+      <c r="N90" t="inlineStr">
+        <is>
+          <t>5939 OLD 29 DRIVE</t>
+        </is>
+      </c>
       <c r="O90" t="inlineStr"/>
       <c r="P90" t="inlineStr"/>
       <c r="Q90" t="inlineStr"/>
@@ -4985,7 +5013,11 @@
       <c r="K91" t="inlineStr"/>
       <c r="L91" t="inlineStr"/>
       <c r="M91" t="inlineStr"/>
-      <c r="N91" t="inlineStr"/>
+      <c r="N91" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/P7gcbpqmHRw</t>
+        </is>
+      </c>
       <c r="O91" t="inlineStr"/>
       <c r="P91" t="inlineStr"/>
       <c r="Q91" t="inlineStr">
@@ -5045,7 +5077,11 @@
       <c r="K92" t="inlineStr"/>
       <c r="L92" t="inlineStr"/>
       <c r="M92" t="inlineStr"/>
-      <c r="N92" t="inlineStr"/>
+      <c r="N92" t="inlineStr">
+        <is>
+          <t>FULL STORE</t>
+        </is>
+      </c>
       <c r="O92" t="inlineStr"/>
       <c r="P92" t="inlineStr"/>
       <c r="Q92" t="inlineStr">
@@ -5109,9 +5145,21 @@
         </is>
       </c>
       <c r="L93" t="inlineStr"/>
-      <c r="M93" t="inlineStr"/>
-      <c r="N93" t="inlineStr"/>
-      <c r="O93" t="inlineStr"/>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="N93" t="inlineStr">
+        <is>
+          <t>Jerry S</t>
+        </is>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>Driver</t>
+        </is>
+      </c>
       <c r="P93" t="inlineStr"/>
       <c r="Q93" t="inlineStr">
         <is>
@@ -5126,7 +5174,11 @@
       <c r="S93" t="inlineStr"/>
       <c r="T93" t="inlineStr"/>
       <c r="U93" t="inlineStr"/>
-      <c r="V93" t="inlineStr"/>
+      <c r="V93" t="inlineStr">
+        <is>
+          <t>FV: 5:15 MEET BALLARD</t>
+        </is>
+      </c>
       <c r="W93" t="inlineStr"/>
       <c r="X93" t="inlineStr"/>
       <c r="Y93" t="inlineStr"/>
@@ -5164,8 +5216,16 @@
       </c>
       <c r="K94" t="inlineStr"/>
       <c r="L94" t="inlineStr"/>
-      <c r="M94" t="inlineStr"/>
-      <c r="N94" t="inlineStr"/>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="N94" t="inlineStr">
+        <is>
+          <t>Annette P</t>
+        </is>
+      </c>
       <c r="O94" t="inlineStr"/>
       <c r="P94" t="inlineStr"/>
       <c r="Q94" t="inlineStr">
@@ -5186,7 +5246,11 @@
       </c>
       <c r="T94" t="inlineStr"/>
       <c r="U94" t="inlineStr"/>
-      <c r="V94" t="inlineStr"/>
+      <c r="V94" t="inlineStr">
+        <is>
+          <t>7:00 AM START</t>
+        </is>
+      </c>
       <c r="W94" t="inlineStr"/>
       <c r="X94" t="inlineStr"/>
       <c r="Y94" t="inlineStr"/>
@@ -5224,9 +5288,21 @@
       </c>
       <c r="K95" t="inlineStr"/>
       <c r="L95" t="inlineStr"/>
-      <c r="M95" t="inlineStr"/>
-      <c r="N95" t="inlineStr"/>
-      <c r="O95" t="inlineStr"/>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>3)</t>
+        </is>
+      </c>
+      <c r="N95" t="inlineStr">
+        <is>
+          <t>Katie R</t>
+        </is>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>work w/ Serena E</t>
+        </is>
+      </c>
       <c r="P95" t="inlineStr"/>
       <c r="Q95" t="inlineStr">
         <is>
@@ -5241,7 +5317,11 @@
       <c r="S95" t="inlineStr"/>
       <c r="T95" t="inlineStr"/>
       <c r="U95" t="inlineStr"/>
-      <c r="V95" t="inlineStr"/>
+      <c r="V95" t="inlineStr">
+        <is>
+          <t>DC5-FINANCIAL</t>
+        </is>
+      </c>
       <c r="W95" t="inlineStr"/>
       <c r="X95" t="inlineStr"/>
       <c r="Y95" t="inlineStr"/>
@@ -5259,9 +5339,21 @@
       <c r="J96" t="inlineStr"/>
       <c r="K96" t="inlineStr"/>
       <c r="L96" t="inlineStr"/>
-      <c r="M96" t="inlineStr"/>
-      <c r="N96" t="inlineStr"/>
-      <c r="O96" t="inlineStr"/>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>4)</t>
+        </is>
+      </c>
+      <c r="N96" t="inlineStr">
+        <is>
+          <t>Michelle C</t>
+        </is>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
       <c r="P96" t="inlineStr"/>
       <c r="Q96" t="inlineStr">
         <is>
@@ -5276,7 +5368,11 @@
       <c r="S96" t="inlineStr"/>
       <c r="T96" t="inlineStr"/>
       <c r="U96" t="inlineStr"/>
-      <c r="V96" t="inlineStr"/>
+      <c r="V96" t="inlineStr">
+        <is>
+          <t>WESTFIELD SUPERVALU</t>
+        </is>
+      </c>
       <c r="W96" t="inlineStr"/>
       <c r="X96" t="inlineStr"/>
       <c r="Y96" t="inlineStr"/>
@@ -5294,9 +5390,21 @@
       <c r="J97" t="inlineStr"/>
       <c r="K97" t="inlineStr"/>
       <c r="L97" t="inlineStr"/>
-      <c r="M97" t="inlineStr"/>
-      <c r="N97" t="inlineStr"/>
-      <c r="O97" t="inlineStr"/>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>5)</t>
+        </is>
+      </c>
+      <c r="N97" t="inlineStr">
+        <is>
+          <t>Serena E</t>
+        </is>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>1st Oneidas, work w/ Katie R</t>
+        </is>
+      </c>
       <c r="P97" t="inlineStr"/>
       <c r="Q97" t="inlineStr">
         <is>
@@ -5311,7 +5419,11 @@
       <c r="S97" t="inlineStr"/>
       <c r="T97" t="inlineStr"/>
       <c r="U97" t="inlineStr"/>
-      <c r="V97" t="inlineStr"/>
+      <c r="V97" t="inlineStr">
+        <is>
+          <t>519 S MAIN ST</t>
+        </is>
+      </c>
       <c r="W97" t="inlineStr"/>
       <c r="X97" t="inlineStr"/>
       <c r="Y97" t="inlineStr"/>
@@ -5360,7 +5472,11 @@
       </c>
       <c r="T98" t="inlineStr"/>
       <c r="U98" t="inlineStr"/>
-      <c r="V98" t="inlineStr"/>
+      <c r="V98" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/xUAXuNCLdR72</t>
+        </is>
+      </c>
       <c r="W98" t="inlineStr"/>
       <c r="X98" t="inlineStr"/>
       <c r="Y98" t="inlineStr"/>
@@ -5435,16 +5551,32 @@
       <c r="K100" t="inlineStr"/>
       <c r="L100" t="inlineStr"/>
       <c r="M100" t="inlineStr"/>
-      <c r="N100" t="inlineStr"/>
+      <c r="N100" t="inlineStr">
+        <is>
+          <t>FV: 4:45 AM MEET BALLARD</t>
+        </is>
+      </c>
       <c r="O100" t="inlineStr"/>
       <c r="P100" t="inlineStr"/>
       <c r="Q100" t="inlineStr"/>
       <c r="R100" t="inlineStr"/>
       <c r="S100" t="inlineStr"/>
       <c r="T100" t="inlineStr"/>
-      <c r="U100" t="inlineStr"/>
-      <c r="V100" t="inlineStr"/>
-      <c r="W100" t="inlineStr"/>
+      <c r="U100" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="V100" t="inlineStr">
+        <is>
+          <t>Jerry S</t>
+        </is>
+      </c>
+      <c r="W100" t="inlineStr">
+        <is>
+          <t>Driver, Equip</t>
+        </is>
+      </c>
       <c r="X100" t="inlineStr"/>
       <c r="Y100" t="inlineStr"/>
     </row>
@@ -5470,15 +5602,27 @@
       <c r="K101" t="inlineStr"/>
       <c r="L101" t="inlineStr"/>
       <c r="M101" t="inlineStr"/>
-      <c r="N101" t="inlineStr"/>
+      <c r="N101" t="inlineStr">
+        <is>
+          <t>6:00 AM START</t>
+        </is>
+      </c>
       <c r="O101" t="inlineStr"/>
       <c r="P101" t="inlineStr"/>
       <c r="Q101" t="inlineStr"/>
       <c r="R101" t="inlineStr"/>
       <c r="S101" t="inlineStr"/>
       <c r="T101" t="inlineStr"/>
-      <c r="U101" t="inlineStr"/>
-      <c r="V101" t="inlineStr"/>
+      <c r="U101" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="V101" t="inlineStr">
+        <is>
+          <t>Heather V</t>
+        </is>
+      </c>
       <c r="W101" t="inlineStr"/>
       <c r="X101" t="inlineStr"/>
       <c r="Y101" t="inlineStr"/>
@@ -5505,16 +5649,36 @@
       <c r="K102" t="inlineStr"/>
       <c r="L102" t="inlineStr"/>
       <c r="M102" t="inlineStr"/>
-      <c r="N102" t="inlineStr"/>
+      <c r="N102" t="inlineStr">
+        <is>
+          <t>DC5-FINANCIAL</t>
+        </is>
+      </c>
       <c r="O102" t="inlineStr"/>
       <c r="P102" t="inlineStr"/>
       <c r="Q102" t="inlineStr"/>
-      <c r="R102" t="inlineStr"/>
+      <c r="R102" t="inlineStr">
+        <is>
+          <t>FV: 6:00 AM MEET BALLARD</t>
+        </is>
+      </c>
       <c r="S102" t="inlineStr"/>
       <c r="T102" t="inlineStr"/>
-      <c r="U102" t="inlineStr"/>
-      <c r="V102" t="inlineStr"/>
-      <c r="W102" t="inlineStr"/>
+      <c r="U102" t="inlineStr">
+        <is>
+          <t>3)</t>
+        </is>
+      </c>
+      <c r="V102" t="inlineStr">
+        <is>
+          <t>Jeremiah F</t>
+        </is>
+      </c>
+      <c r="W102" t="inlineStr">
+        <is>
+          <t>Driver</t>
+        </is>
+      </c>
       <c r="X102" t="inlineStr"/>
       <c r="Y102" t="inlineStr"/>
     </row>
@@ -5540,15 +5704,31 @@
       <c r="K103" t="inlineStr"/>
       <c r="L103" t="inlineStr"/>
       <c r="M103" t="inlineStr"/>
-      <c r="N103" t="inlineStr"/>
+      <c r="N103" t="inlineStr">
+        <is>
+          <t>HOWARDS PANTRY, HOWARDS GROVE</t>
+        </is>
+      </c>
       <c r="O103" t="inlineStr"/>
       <c r="P103" t="inlineStr"/>
       <c r="Q103" t="inlineStr"/>
-      <c r="R103" t="inlineStr"/>
+      <c r="R103" t="inlineStr">
+        <is>
+          <t>6:30 AM START</t>
+        </is>
+      </c>
       <c r="S103" t="inlineStr"/>
       <c r="T103" t="inlineStr"/>
-      <c r="U103" t="inlineStr"/>
-      <c r="V103" t="inlineStr"/>
+      <c r="U103" t="inlineStr">
+        <is>
+          <t>4)</t>
+        </is>
+      </c>
+      <c r="V103" t="inlineStr">
+        <is>
+          <t>Kirsten E</t>
+        </is>
+      </c>
       <c r="W103" t="inlineStr"/>
       <c r="X103" t="inlineStr"/>
       <c r="Y103" t="inlineStr"/>
@@ -5571,15 +5751,31 @@
       <c r="K104" t="inlineStr"/>
       <c r="L104" t="inlineStr"/>
       <c r="M104" t="inlineStr"/>
-      <c r="N104" t="inlineStr"/>
+      <c r="N104" t="inlineStr">
+        <is>
+          <t>536 MADISON AVE</t>
+        </is>
+      </c>
       <c r="O104" t="inlineStr"/>
       <c r="P104" t="inlineStr"/>
       <c r="Q104" t="inlineStr"/>
-      <c r="R104" t="inlineStr"/>
+      <c r="R104" t="inlineStr">
+        <is>
+          <t>MODAS</t>
+        </is>
+      </c>
       <c r="S104" t="inlineStr"/>
       <c r="T104" t="inlineStr"/>
-      <c r="U104" t="inlineStr"/>
-      <c r="V104" t="inlineStr"/>
+      <c r="U104" t="inlineStr">
+        <is>
+          <t>5)</t>
+        </is>
+      </c>
+      <c r="V104" t="inlineStr">
+        <is>
+          <t>Marcia L</t>
+        </is>
+      </c>
       <c r="W104" t="inlineStr"/>
       <c r="X104" t="inlineStr"/>
       <c r="Y104" t="inlineStr"/>
@@ -5614,15 +5810,31 @@
       <c r="K105" t="inlineStr"/>
       <c r="L105" t="inlineStr"/>
       <c r="M105" t="inlineStr"/>
-      <c r="N105" t="inlineStr"/>
+      <c r="N105" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/3y3VSQssTmuh2dpo8</t>
+        </is>
+      </c>
       <c r="O105" t="inlineStr"/>
       <c r="P105" t="inlineStr"/>
       <c r="Q105" t="inlineStr"/>
-      <c r="R105" t="inlineStr"/>
+      <c r="R105" t="inlineStr">
+        <is>
+          <t>ONEIDA #2027 FOUR PATHS, GREEN BAY</t>
+        </is>
+      </c>
       <c r="S105" t="inlineStr"/>
       <c r="T105" t="inlineStr"/>
-      <c r="U105" t="inlineStr"/>
-      <c r="V105" t="inlineStr"/>
+      <c r="U105" t="inlineStr">
+        <is>
+          <t>6)</t>
+        </is>
+      </c>
+      <c r="V105" t="inlineStr">
+        <is>
+          <t>Serena E</t>
+        </is>
+      </c>
       <c r="W105" t="inlineStr"/>
       <c r="X105" t="inlineStr"/>
       <c r="Y105" t="inlineStr"/>
@@ -5658,11 +5870,19 @@
       <c r="K106" t="inlineStr"/>
       <c r="L106" t="inlineStr"/>
       <c r="M106" t="inlineStr"/>
-      <c r="N106" t="inlineStr"/>
+      <c r="N106" t="inlineStr">
+        <is>
+          <t>TO FOLLOW</t>
+        </is>
+      </c>
       <c r="O106" t="inlineStr"/>
       <c r="P106" t="inlineStr"/>
       <c r="Q106" t="inlineStr"/>
-      <c r="R106" t="inlineStr"/>
+      <c r="R106" t="inlineStr">
+        <is>
+          <t>2597 WEST MASON ST</t>
+        </is>
+      </c>
       <c r="S106" t="inlineStr"/>
       <c r="T106" t="inlineStr"/>
       <c r="U106" t="inlineStr"/>
@@ -5697,11 +5917,19 @@
       <c r="K107" t="inlineStr"/>
       <c r="L107" t="inlineStr"/>
       <c r="M107" t="inlineStr"/>
-      <c r="N107" t="inlineStr"/>
+      <c r="N107" t="inlineStr">
+        <is>
+          <t>DC5-FINANCIAL</t>
+        </is>
+      </c>
       <c r="O107" t="inlineStr"/>
       <c r="P107" t="inlineStr"/>
       <c r="Q107" t="inlineStr"/>
-      <c r="R107" t="inlineStr"/>
+      <c r="R107" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/Ejz3LxP1Y8S2</t>
+        </is>
+      </c>
       <c r="S107" t="inlineStr"/>
       <c r="T107" t="inlineStr"/>
       <c r="U107" t="inlineStr"/>
@@ -5741,15 +5969,27 @@
       <c r="K108" t="inlineStr"/>
       <c r="L108" t="inlineStr"/>
       <c r="M108" t="inlineStr"/>
-      <c r="N108" t="inlineStr"/>
+      <c r="N108" t="inlineStr">
+        <is>
+          <t>PETRO CENTER 2, HOWARDS GROVE</t>
+        </is>
+      </c>
       <c r="O108" t="inlineStr"/>
       <c r="P108" t="inlineStr"/>
       <c r="Q108" t="inlineStr"/>
-      <c r="R108" t="inlineStr"/>
+      <c r="R108" t="inlineStr">
+        <is>
+          <t>TO FOLLOW</t>
+        </is>
+      </c>
       <c r="S108" t="inlineStr"/>
       <c r="T108" t="inlineStr"/>
       <c r="U108" t="inlineStr"/>
-      <c r="V108" t="inlineStr"/>
+      <c r="V108" t="inlineStr">
+        <is>
+          <t>8:00 AM START</t>
+        </is>
+      </c>
       <c r="W108" t="inlineStr"/>
       <c r="X108" t="inlineStr"/>
       <c r="Y108" t="inlineStr"/>
@@ -5776,15 +6016,27 @@
       <c r="K109" t="inlineStr"/>
       <c r="L109" t="inlineStr"/>
       <c r="M109" t="inlineStr"/>
-      <c r="N109" t="inlineStr"/>
+      <c r="N109" t="inlineStr">
+        <is>
+          <t>220 N WISCONSIN DR</t>
+        </is>
+      </c>
       <c r="O109" t="inlineStr"/>
       <c r="P109" t="inlineStr"/>
       <c r="Q109" t="inlineStr"/>
-      <c r="R109" t="inlineStr"/>
+      <c r="R109" t="inlineStr">
+        <is>
+          <t>MODAS</t>
+        </is>
+      </c>
       <c r="S109" t="inlineStr"/>
       <c r="T109" t="inlineStr"/>
       <c r="U109" t="inlineStr"/>
-      <c r="V109" t="inlineStr"/>
+      <c r="V109" t="inlineStr">
+        <is>
+          <t>EXCEL FINANCIAL</t>
+        </is>
+      </c>
       <c r="W109" t="inlineStr"/>
       <c r="X109" t="inlineStr"/>
       <c r="Y109" t="inlineStr"/>
@@ -5824,15 +6076,27 @@
       </c>
       <c r="L110" t="inlineStr"/>
       <c r="M110" t="inlineStr"/>
-      <c r="N110" t="inlineStr"/>
+      <c r="N110" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/8Yb9mTahQpte986L6</t>
+        </is>
+      </c>
       <c r="O110" t="inlineStr"/>
       <c r="P110" t="inlineStr"/>
       <c r="Q110" t="inlineStr"/>
-      <c r="R110" t="inlineStr"/>
+      <c r="R110" t="inlineStr">
+        <is>
+          <t>ONEIDA #2032 SMOKE SHOP ISBELL, GREEN BAY</t>
+        </is>
+      </c>
       <c r="S110" t="inlineStr"/>
       <c r="T110" t="inlineStr"/>
       <c r="U110" t="inlineStr"/>
-      <c r="V110" t="inlineStr"/>
+      <c r="V110" t="inlineStr">
+        <is>
+          <t>SWETZ COUNTRY CORNER MART, BLENKER</t>
+        </is>
+      </c>
       <c r="W110" t="inlineStr"/>
       <c r="X110" t="inlineStr"/>
       <c r="Y110" t="inlineStr"/>
@@ -5871,16 +6135,29 @@
         </is>
       </c>
       <c r="L111" t="inlineStr"/>
-      <c r="M111" t="inlineStr"/>
+      <c r="M111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Switching to DC5 Financial
+*SALE INVENTORIES        </t>
+        </is>
+      </c>
       <c r="N111" t="inlineStr"/>
       <c r="O111" t="inlineStr"/>
       <c r="P111" t="inlineStr"/>
       <c r="Q111" t="inlineStr"/>
-      <c r="R111" t="inlineStr"/>
+      <c r="R111" t="inlineStr">
+        <is>
+          <t>2514 WEST MASON ST</t>
+        </is>
+      </c>
       <c r="S111" t="inlineStr"/>
       <c r="T111" t="inlineStr"/>
       <c r="U111" t="inlineStr"/>
-      <c r="V111" t="inlineStr"/>
+      <c r="V111" t="inlineStr">
+        <is>
+          <t>3912 US HWY 10</t>
+        </is>
+      </c>
       <c r="W111" t="inlineStr"/>
       <c r="X111" t="inlineStr"/>
       <c r="Y111" t="inlineStr"/>
@@ -5919,11 +6196,19 @@
       <c r="O112" t="inlineStr"/>
       <c r="P112" t="inlineStr"/>
       <c r="Q112" t="inlineStr"/>
-      <c r="R112" t="inlineStr"/>
+      <c r="R112" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/hEygq2DoHmr</t>
+        </is>
+      </c>
       <c r="S112" t="inlineStr"/>
       <c r="T112" t="inlineStr"/>
       <c r="U112" t="inlineStr"/>
-      <c r="V112" t="inlineStr"/>
+      <c r="V112" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/1dMLKgeWQnr</t>
+        </is>
+      </c>
       <c r="W112" t="inlineStr"/>
       <c r="X112" t="inlineStr"/>
       <c r="Y112" t="inlineStr"/>
@@ -5957,16 +6242,36 @@
       </c>
       <c r="K113" t="inlineStr"/>
       <c r="L113" t="inlineStr"/>
-      <c r="M113" t="inlineStr"/>
-      <c r="N113" t="inlineStr"/>
-      <c r="O113" t="inlineStr"/>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="N113" t="inlineStr">
+        <is>
+          <t>Jeremiah F</t>
+        </is>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>Driver</t>
+        </is>
+      </c>
       <c r="P113" t="inlineStr"/>
       <c r="Q113" t="inlineStr"/>
-      <c r="R113" t="inlineStr"/>
+      <c r="R113" t="inlineStr">
+        <is>
+          <t>TO FOLLOW</t>
+        </is>
+      </c>
       <c r="S113" t="inlineStr"/>
       <c r="T113" t="inlineStr"/>
       <c r="U113" t="inlineStr"/>
-      <c r="V113" t="inlineStr"/>
+      <c r="V113" t="inlineStr">
+        <is>
+          <t>TO FOLLOW</t>
+        </is>
+      </c>
       <c r="W113" t="inlineStr"/>
       <c r="X113" t="inlineStr"/>
       <c r="Y113" t="inlineStr"/>
@@ -6005,16 +6310,32 @@
       </c>
       <c r="K114" t="inlineStr"/>
       <c r="L114" t="inlineStr"/>
-      <c r="M114" t="inlineStr"/>
-      <c r="N114" t="inlineStr"/>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="N114" t="inlineStr">
+        <is>
+          <t>Louisa F</t>
+        </is>
+      </c>
       <c r="O114" t="inlineStr"/>
       <c r="P114" t="inlineStr"/>
       <c r="Q114" t="inlineStr"/>
-      <c r="R114" t="inlineStr"/>
+      <c r="R114" t="inlineStr">
+        <is>
+          <t>MODAS</t>
+        </is>
+      </c>
       <c r="S114" t="inlineStr"/>
       <c r="T114" t="inlineStr"/>
       <c r="U114" t="inlineStr"/>
-      <c r="V114" t="inlineStr"/>
+      <c r="V114" t="inlineStr">
+        <is>
+          <t>EXCEL FINANCIAL</t>
+        </is>
+      </c>
       <c r="W114" t="inlineStr"/>
       <c r="X114" t="inlineStr"/>
       <c r="Y114" t="inlineStr"/>
@@ -6058,16 +6379,32 @@
         </is>
       </c>
       <c r="L115" t="inlineStr"/>
-      <c r="M115" t="inlineStr"/>
-      <c r="N115" t="inlineStr"/>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>3)</t>
+        </is>
+      </c>
+      <c r="N115" t="inlineStr">
+        <is>
+          <t>Marcia L</t>
+        </is>
+      </c>
       <c r="O115" t="inlineStr"/>
       <c r="P115" t="inlineStr"/>
       <c r="Q115" t="inlineStr"/>
-      <c r="R115" t="inlineStr"/>
+      <c r="R115" t="inlineStr">
+        <is>
+          <t>ONEIDA #2030 SMOKE SHOP CASINO, GREEN BAY</t>
+        </is>
+      </c>
       <c r="S115" t="inlineStr"/>
       <c r="T115" t="inlineStr"/>
       <c r="U115" t="inlineStr"/>
-      <c r="V115" t="inlineStr"/>
+      <c r="V115" t="inlineStr">
+        <is>
+          <t>SWETZ ROADSIDE CONVENIENCE, STEVENS POINT</t>
+        </is>
+      </c>
       <c r="W115" t="inlineStr"/>
       <c r="X115" t="inlineStr"/>
       <c r="Y115" t="inlineStr"/>
@@ -6098,11 +6435,19 @@
       <c r="O116" t="inlineStr"/>
       <c r="P116" t="inlineStr"/>
       <c r="Q116" t="inlineStr"/>
-      <c r="R116" t="inlineStr"/>
+      <c r="R116" t="inlineStr">
+        <is>
+          <t>2020 AIRPORT DR</t>
+        </is>
+      </c>
       <c r="S116" t="inlineStr"/>
       <c r="T116" t="inlineStr"/>
       <c r="U116" t="inlineStr"/>
-      <c r="V116" t="inlineStr"/>
+      <c r="V116" t="inlineStr">
+        <is>
+          <t>2133 DIVISION ST</t>
+        </is>
+      </c>
       <c r="W116" t="inlineStr"/>
       <c r="X116" t="inlineStr"/>
       <c r="Y116" t="inlineStr"/>
@@ -6125,11 +6470,19 @@
       <c r="O117" t="inlineStr"/>
       <c r="P117" t="inlineStr"/>
       <c r="Q117" t="inlineStr"/>
-      <c r="R117" t="inlineStr"/>
+      <c r="R117" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/4XjrBGvHYgS2</t>
+        </is>
+      </c>
       <c r="S117" t="inlineStr"/>
       <c r="T117" t="inlineStr"/>
       <c r="U117" t="inlineStr"/>
-      <c r="V117" t="inlineStr"/>
+      <c r="V117" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/rCaFFDRAv7T2</t>
+        </is>
+      </c>
       <c r="W117" t="inlineStr"/>
       <c r="X117" t="inlineStr"/>
       <c r="Y117" t="inlineStr"/>
@@ -6144,15 +6497,27 @@
       <c r="G118" t="inlineStr"/>
       <c r="H118" t="inlineStr"/>
       <c r="I118" t="inlineStr"/>
-      <c r="J118" t="inlineStr"/>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t>FV: 6:00 AM MEET BALLARD</t>
+        </is>
+      </c>
       <c r="K118" t="inlineStr"/>
       <c r="L118" t="inlineStr"/>
       <c r="M118" t="inlineStr"/>
-      <c r="N118" t="inlineStr"/>
+      <c r="N118" t="inlineStr">
+        <is>
+          <t>Office</t>
+        </is>
+      </c>
       <c r="O118" t="inlineStr"/>
       <c r="P118" t="inlineStr"/>
       <c r="Q118" t="inlineStr"/>
-      <c r="R118" t="inlineStr"/>
+      <c r="R118" t="inlineStr">
+        <is>
+          <t>TO FOLLOW</t>
+        </is>
+      </c>
       <c r="S118" t="inlineStr"/>
       <c r="T118" t="inlineStr"/>
       <c r="U118" t="inlineStr"/>
@@ -6175,20 +6540,44 @@
       <c r="G119" t="inlineStr"/>
       <c r="H119" t="inlineStr"/>
       <c r="I119" t="inlineStr"/>
-      <c r="J119" t="inlineStr"/>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t>6:30 AM START</t>
+        </is>
+      </c>
       <c r="K119" t="inlineStr"/>
       <c r="L119" t="inlineStr"/>
       <c r="M119" t="inlineStr"/>
-      <c r="N119" t="inlineStr"/>
+      <c r="N119" t="inlineStr">
+        <is>
+          <t>Kim G</t>
+        </is>
+      </c>
       <c r="O119" t="inlineStr"/>
       <c r="P119" t="inlineStr"/>
       <c r="Q119" t="inlineStr"/>
-      <c r="R119" t="inlineStr"/>
+      <c r="R119" t="inlineStr">
+        <is>
+          <t>MODAS</t>
+        </is>
+      </c>
       <c r="S119" t="inlineStr"/>
       <c r="T119" t="inlineStr"/>
-      <c r="U119" t="inlineStr"/>
-      <c r="V119" t="inlineStr"/>
-      <c r="W119" t="inlineStr"/>
+      <c r="U119" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="V119" t="inlineStr">
+        <is>
+          <t>Michelle C</t>
+        </is>
+      </c>
+      <c r="W119" t="inlineStr">
+        <is>
+          <t>@ Store, Equip</t>
+        </is>
+      </c>
       <c r="X119" t="inlineStr"/>
       <c r="Y119" t="inlineStr"/>
     </row>
@@ -6206,20 +6595,44 @@
       <c r="G120" t="inlineStr"/>
       <c r="H120" t="inlineStr"/>
       <c r="I120" t="inlineStr"/>
-      <c r="J120" t="inlineStr"/>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t>MODAS</t>
+        </is>
+      </c>
       <c r="K120" t="inlineStr"/>
       <c r="L120" t="inlineStr"/>
       <c r="M120" t="inlineStr"/>
-      <c r="N120" t="inlineStr"/>
+      <c r="N120" t="inlineStr">
+        <is>
+          <t>Lashaun C</t>
+        </is>
+      </c>
       <c r="O120" t="inlineStr"/>
       <c r="P120" t="inlineStr"/>
       <c r="Q120" t="inlineStr"/>
-      <c r="R120" t="inlineStr"/>
+      <c r="R120" t="inlineStr">
+        <is>
+          <t>ONEIDA #2031 SMOKE SHOP BINGO, GREEN BAY</t>
+        </is>
+      </c>
       <c r="S120" t="inlineStr"/>
       <c r="T120" t="inlineStr"/>
-      <c r="U120" t="inlineStr"/>
-      <c r="V120" t="inlineStr"/>
-      <c r="W120" t="inlineStr"/>
+      <c r="U120" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="V120" t="inlineStr">
+        <is>
+          <t>Jacqui R</t>
+        </is>
+      </c>
+      <c r="W120" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
       <c r="X120" t="inlineStr"/>
       <c r="Y120" t="inlineStr"/>
     </row>
@@ -6237,7 +6650,11 @@
       <c r="G121" t="inlineStr"/>
       <c r="H121" t="inlineStr"/>
       <c r="I121" t="inlineStr"/>
-      <c r="J121" t="inlineStr"/>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t>ONEIDA #2022 ONE STOP E &amp; EE, DEPERE</t>
+        </is>
+      </c>
       <c r="K121" t="inlineStr"/>
       <c r="L121" t="inlineStr"/>
       <c r="M121" t="inlineStr"/>
@@ -6245,7 +6662,11 @@
       <c r="O121" t="inlineStr"/>
       <c r="P121" t="inlineStr"/>
       <c r="Q121" t="inlineStr"/>
-      <c r="R121" t="inlineStr"/>
+      <c r="R121" t="inlineStr">
+        <is>
+          <t>2020 AIRPORT DR</t>
+        </is>
+      </c>
       <c r="S121" t="inlineStr"/>
       <c r="T121" t="inlineStr"/>
       <c r="U121" t="inlineStr"/>
@@ -6268,7 +6689,11 @@
       <c r="G122" t="inlineStr"/>
       <c r="H122" t="inlineStr"/>
       <c r="I122" t="inlineStr"/>
-      <c r="J122" t="inlineStr"/>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>790 COUNTY RD EE</t>
+        </is>
+      </c>
       <c r="K122" t="inlineStr"/>
       <c r="L122" t="inlineStr"/>
       <c r="M122" t="inlineStr"/>
@@ -6276,7 +6701,11 @@
       <c r="O122" t="inlineStr"/>
       <c r="P122" t="inlineStr"/>
       <c r="Q122" t="inlineStr"/>
-      <c r="R122" t="inlineStr"/>
+      <c r="R122" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/4XjrBGvHYgS2</t>
+        </is>
+      </c>
       <c r="S122" t="inlineStr"/>
       <c r="T122" t="inlineStr"/>
       <c r="U122" t="inlineStr"/>
@@ -6299,7 +6728,11 @@
       <c r="G123" t="inlineStr"/>
       <c r="H123" t="inlineStr"/>
       <c r="I123" t="inlineStr"/>
-      <c r="J123" t="inlineStr"/>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/VLR8RdvzGgF2</t>
+        </is>
+      </c>
       <c r="K123" t="inlineStr"/>
       <c r="L123" t="inlineStr"/>
       <c r="M123" t="inlineStr"/>
@@ -6307,7 +6740,11 @@
       <c r="O123" t="inlineStr"/>
       <c r="P123" t="inlineStr"/>
       <c r="Q123" t="inlineStr"/>
-      <c r="R123" t="inlineStr"/>
+      <c r="R123" t="inlineStr">
+        <is>
+          <t>FULL STORE</t>
+        </is>
+      </c>
       <c r="S123" t="inlineStr"/>
       <c r="T123" t="inlineStr"/>
       <c r="U123" t="inlineStr"/>
@@ -6330,16 +6767,32 @@
       <c r="G124" t="inlineStr"/>
       <c r="H124" t="inlineStr"/>
       <c r="I124" t="inlineStr"/>
-      <c r="J124" t="inlineStr"/>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>TO FOLLOW</t>
+        </is>
+      </c>
       <c r="K124" t="inlineStr"/>
       <c r="L124" t="inlineStr"/>
       <c r="M124" t="inlineStr"/>
       <c r="N124" t="inlineStr"/>
       <c r="O124" t="inlineStr"/>
       <c r="P124" t="inlineStr"/>
-      <c r="Q124" t="inlineStr"/>
-      <c r="R124" t="inlineStr"/>
-      <c r="S124" t="inlineStr"/>
+      <c r="Q124" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="R124" t="inlineStr">
+        <is>
+          <t>Jerry S</t>
+        </is>
+      </c>
+      <c r="S124" t="inlineStr">
+        <is>
+          <t>Driver, Equip</t>
+        </is>
+      </c>
       <c r="T124" t="inlineStr"/>
       <c r="U124" t="inlineStr"/>
       <c r="V124" t="inlineStr"/>
@@ -6357,16 +6810,32 @@
       <c r="G125" t="inlineStr"/>
       <c r="H125" t="inlineStr"/>
       <c r="I125" t="inlineStr"/>
-      <c r="J125" t="inlineStr"/>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t>MODAS</t>
+        </is>
+      </c>
       <c r="K125" t="inlineStr"/>
       <c r="L125" t="inlineStr"/>
       <c r="M125" t="inlineStr"/>
       <c r="N125" t="inlineStr"/>
       <c r="O125" t="inlineStr"/>
       <c r="P125" t="inlineStr"/>
-      <c r="Q125" t="inlineStr"/>
-      <c r="R125" t="inlineStr"/>
-      <c r="S125" t="inlineStr"/>
+      <c r="Q125" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="R125" t="inlineStr">
+        <is>
+          <t>David B</t>
+        </is>
+      </c>
+      <c r="S125" t="inlineStr">
+        <is>
+          <t>2nd Oneidas, work w/ Katie R</t>
+        </is>
+      </c>
       <c r="T125" t="inlineStr"/>
       <c r="U125" t="inlineStr"/>
       <c r="V125" t="inlineStr"/>
@@ -6386,7 +6855,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Lashaun</t>
+          <t>Lashaun C</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
@@ -6397,16 +6866,32 @@
       </c>
       <c r="H126" t="inlineStr"/>
       <c r="I126" t="inlineStr"/>
-      <c r="J126" t="inlineStr"/>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>ONEIDA #2021 ONE STOP 54, ONEIDA</t>
+        </is>
+      </c>
       <c r="K126" t="inlineStr"/>
       <c r="L126" t="inlineStr"/>
       <c r="M126" t="inlineStr"/>
       <c r="N126" t="inlineStr"/>
       <c r="O126" t="inlineStr"/>
       <c r="P126" t="inlineStr"/>
-      <c r="Q126" t="inlineStr"/>
-      <c r="R126" t="inlineStr"/>
-      <c r="S126" t="inlineStr"/>
+      <c r="Q126" t="inlineStr">
+        <is>
+          <t>3)</t>
+        </is>
+      </c>
+      <c r="R126" t="inlineStr">
+        <is>
+          <t>Katie R</t>
+        </is>
+      </c>
+      <c r="S126" t="inlineStr">
+        <is>
+          <t>Driver, work w/ David B</t>
+        </is>
+      </c>
       <c r="T126" t="inlineStr"/>
       <c r="U126" t="inlineStr"/>
       <c r="V126" t="inlineStr"/>
@@ -6426,21 +6911,33 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>Casey</t>
+          <t>Casey V</t>
         </is>
       </c>
       <c r="G127" t="inlineStr"/>
       <c r="H127" t="inlineStr"/>
       <c r="I127" t="inlineStr"/>
-      <c r="J127" t="inlineStr"/>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>W180 HWY 54</t>
+        </is>
+      </c>
       <c r="K127" t="inlineStr"/>
       <c r="L127" t="inlineStr"/>
       <c r="M127" t="inlineStr"/>
       <c r="N127" t="inlineStr"/>
       <c r="O127" t="inlineStr"/>
       <c r="P127" t="inlineStr"/>
-      <c r="Q127" t="inlineStr"/>
-      <c r="R127" t="inlineStr"/>
+      <c r="Q127" t="inlineStr">
+        <is>
+          <t>4)</t>
+        </is>
+      </c>
+      <c r="R127" t="inlineStr">
+        <is>
+          <t>Kirsten E</t>
+        </is>
+      </c>
       <c r="S127" t="inlineStr"/>
       <c r="T127" t="inlineStr"/>
       <c r="U127" t="inlineStr"/>
@@ -6467,15 +6964,27 @@
       <c r="G128" t="inlineStr"/>
       <c r="H128" t="inlineStr"/>
       <c r="I128" t="inlineStr"/>
-      <c r="J128" t="inlineStr"/>
+      <c r="J128" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/kMzccLLaPd22</t>
+        </is>
+      </c>
       <c r="K128" t="inlineStr"/>
       <c r="L128" t="inlineStr"/>
       <c r="M128" t="inlineStr"/>
       <c r="N128" t="inlineStr"/>
       <c r="O128" t="inlineStr"/>
       <c r="P128" t="inlineStr"/>
-      <c r="Q128" t="inlineStr"/>
-      <c r="R128" t="inlineStr"/>
+      <c r="Q128" t="inlineStr">
+        <is>
+          <t>5)</t>
+        </is>
+      </c>
+      <c r="R128" t="inlineStr">
+        <is>
+          <t>Marcia L</t>
+        </is>
+      </c>
       <c r="S128" t="inlineStr"/>
       <c r="T128" t="inlineStr"/>
       <c r="U128" t="inlineStr"/>
@@ -6496,13 +7005,17 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>Stephanie</t>
+          <t>Stephanie G</t>
         </is>
       </c>
       <c r="G129" t="inlineStr"/>
       <c r="H129" t="inlineStr"/>
       <c r="I129" t="inlineStr"/>
-      <c r="J129" t="inlineStr"/>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t>FULL STORE</t>
+        </is>
+      </c>
       <c r="K129" t="inlineStr"/>
       <c r="L129" t="inlineStr"/>
       <c r="M129" t="inlineStr"/>
@@ -6519,6 +7032,1203 @@
       <c r="X129" t="inlineStr"/>
       <c r="Y129" t="inlineStr"/>
     </row>
+    <row r="130">
+      <c r="A130" t="inlineStr"/>
+      <c r="B130" t="inlineStr"/>
+      <c r="C130" t="inlineStr"/>
+      <c r="D130" t="inlineStr"/>
+      <c r="E130" t="inlineStr"/>
+      <c r="F130" t="inlineStr"/>
+      <c r="G130" t="inlineStr"/>
+      <c r="H130" t="inlineStr"/>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="J130" t="inlineStr">
+        <is>
+          <t>Jerry S</t>
+        </is>
+      </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>Driver</t>
+        </is>
+      </c>
+      <c r="L130" t="inlineStr"/>
+      <c r="M130" t="inlineStr"/>
+      <c r="N130" t="inlineStr"/>
+      <c r="O130" t="inlineStr"/>
+      <c r="P130" t="inlineStr"/>
+      <c r="Q130" t="inlineStr"/>
+      <c r="R130" t="inlineStr"/>
+      <c r="S130" t="inlineStr"/>
+      <c r="T130" t="inlineStr"/>
+      <c r="U130" t="inlineStr"/>
+      <c r="V130" t="inlineStr"/>
+      <c r="W130" t="inlineStr"/>
+      <c r="X130" t="inlineStr"/>
+      <c r="Y130" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr"/>
+      <c r="B131" t="inlineStr"/>
+      <c r="C131" t="inlineStr"/>
+      <c r="D131" t="inlineStr"/>
+      <c r="E131" t="inlineStr"/>
+      <c r="F131" t="inlineStr"/>
+      <c r="G131" t="inlineStr"/>
+      <c r="H131" t="inlineStr"/>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>David B</t>
+        </is>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>1st Oneidas, work w/ Katie R</t>
+        </is>
+      </c>
+      <c r="L131" t="inlineStr"/>
+      <c r="M131" t="inlineStr"/>
+      <c r="N131" t="inlineStr"/>
+      <c r="O131" t="inlineStr"/>
+      <c r="P131" t="inlineStr"/>
+      <c r="Q131" t="inlineStr"/>
+      <c r="R131" t="inlineStr">
+        <is>
+          <t>FV: 5:15 MEET BALLARD</t>
+        </is>
+      </c>
+      <c r="S131" t="inlineStr"/>
+      <c r="T131" t="inlineStr"/>
+      <c r="U131" t="inlineStr"/>
+      <c r="V131" t="inlineStr"/>
+      <c r="W131" t="inlineStr"/>
+      <c r="X131" t="inlineStr"/>
+      <c r="Y131" t="inlineStr"/>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr"/>
+      <c r="B132" t="inlineStr"/>
+      <c r="C132" t="inlineStr"/>
+      <c r="D132" t="inlineStr"/>
+      <c r="E132" t="inlineStr"/>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>FV: 6:00 AM MEET BALLARD</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr"/>
+      <c r="H132" t="inlineStr"/>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>3)</t>
+        </is>
+      </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>Heather V</t>
+        </is>
+      </c>
+      <c r="K132" t="inlineStr"/>
+      <c r="L132" t="inlineStr"/>
+      <c r="M132" t="inlineStr"/>
+      <c r="N132" t="inlineStr"/>
+      <c r="O132" t="inlineStr"/>
+      <c r="P132" t="inlineStr"/>
+      <c r="Q132" t="inlineStr"/>
+      <c r="R132" t="inlineStr">
+        <is>
+          <t>7:00 AM START</t>
+        </is>
+      </c>
+      <c r="S132" t="inlineStr"/>
+      <c r="T132" t="inlineStr"/>
+      <c r="U132" t="inlineStr"/>
+      <c r="V132" t="inlineStr"/>
+      <c r="W132" t="inlineStr"/>
+      <c r="X132" t="inlineStr"/>
+      <c r="Y132" t="inlineStr"/>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr"/>
+      <c r="B133" t="inlineStr"/>
+      <c r="C133" t="inlineStr"/>
+      <c r="D133" t="inlineStr"/>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>6:30 AM START</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr"/>
+      <c r="H133" t="inlineStr"/>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>4)</t>
+        </is>
+      </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>Katie R</t>
+        </is>
+      </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>Driver, work w/ David B</t>
+        </is>
+      </c>
+      <c r="L133" t="inlineStr"/>
+      <c r="M133" t="inlineStr"/>
+      <c r="N133" t="inlineStr"/>
+      <c r="O133" t="inlineStr"/>
+      <c r="P133" t="inlineStr"/>
+      <c r="Q133" t="inlineStr"/>
+      <c r="R133" t="inlineStr">
+        <is>
+          <t>MODAS / WINTAKES</t>
+        </is>
+      </c>
+      <c r="S133" t="inlineStr"/>
+      <c r="T133" t="inlineStr"/>
+      <c r="U133" t="inlineStr"/>
+      <c r="V133" t="inlineStr"/>
+      <c r="W133" t="inlineStr"/>
+      <c r="X133" t="inlineStr"/>
+      <c r="Y133" t="inlineStr"/>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr"/>
+      <c r="B134" t="inlineStr"/>
+      <c r="C134" t="inlineStr"/>
+      <c r="D134" t="inlineStr"/>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>MODAS</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr"/>
+      <c r="H134" t="inlineStr"/>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>5)</t>
+        </is>
+      </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t>Marcia L</t>
+        </is>
+      </c>
+      <c r="K134" t="inlineStr"/>
+      <c r="L134" t="inlineStr"/>
+      <c r="M134" t="inlineStr"/>
+      <c r="N134" t="inlineStr"/>
+      <c r="O134" t="inlineStr"/>
+      <c r="P134" t="inlineStr"/>
+      <c r="Q134" t="inlineStr"/>
+      <c r="R134" t="inlineStr">
+        <is>
+          <t>SCHIERL #81, AUBURNDALE</t>
+        </is>
+      </c>
+      <c r="S134" t="inlineStr"/>
+      <c r="T134" t="inlineStr"/>
+      <c r="U134" t="inlineStr"/>
+      <c r="V134" t="inlineStr"/>
+      <c r="W134" t="inlineStr"/>
+      <c r="X134" t="inlineStr"/>
+      <c r="Y134" t="inlineStr"/>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr"/>
+      <c r="B135" t="inlineStr"/>
+      <c r="C135" t="inlineStr"/>
+      <c r="D135" t="inlineStr"/>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>ONEIDA #2026 ONE STOP LARSEN, GREEN BAY</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr"/>
+      <c r="H135" t="inlineStr"/>
+      <c r="I135" t="inlineStr"/>
+      <c r="J135" t="inlineStr"/>
+      <c r="K135" t="inlineStr"/>
+      <c r="L135" t="inlineStr"/>
+      <c r="M135" t="inlineStr"/>
+      <c r="N135" t="inlineStr"/>
+      <c r="O135" t="inlineStr"/>
+      <c r="P135" t="inlineStr"/>
+      <c r="Q135" t="inlineStr"/>
+      <c r="R135" t="inlineStr">
+        <is>
+          <t>6018 MAIN ST</t>
+        </is>
+      </c>
+      <c r="S135" t="inlineStr"/>
+      <c r="T135" t="inlineStr"/>
+      <c r="U135" t="inlineStr"/>
+      <c r="V135" t="inlineStr"/>
+      <c r="W135" t="inlineStr"/>
+      <c r="X135" t="inlineStr"/>
+      <c r="Y135" t="inlineStr"/>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr"/>
+      <c r="B136" t="inlineStr"/>
+      <c r="C136" t="inlineStr"/>
+      <c r="D136" t="inlineStr"/>
+      <c r="E136" t="inlineStr"/>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>501 PACKERLAND DR</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr"/>
+      <c r="H136" t="inlineStr"/>
+      <c r="I136" t="inlineStr"/>
+      <c r="J136" t="inlineStr"/>
+      <c r="K136" t="inlineStr"/>
+      <c r="L136" t="inlineStr"/>
+      <c r="M136" t="inlineStr"/>
+      <c r="N136" t="inlineStr"/>
+      <c r="O136" t="inlineStr"/>
+      <c r="P136" t="inlineStr"/>
+      <c r="Q136" t="inlineStr"/>
+      <c r="R136" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/qr31xSMhPtRtRAvB7</t>
+        </is>
+      </c>
+      <c r="S136" t="inlineStr"/>
+      <c r="T136" t="inlineStr"/>
+      <c r="U136" t="inlineStr"/>
+      <c r="V136" t="inlineStr"/>
+      <c r="W136" t="inlineStr"/>
+      <c r="X136" t="inlineStr"/>
+      <c r="Y136" t="inlineStr"/>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr"/>
+      <c r="B137" t="inlineStr"/>
+      <c r="C137" t="inlineStr"/>
+      <c r="D137" t="inlineStr"/>
+      <c r="E137" t="inlineStr"/>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/gjFs8S2qgY22</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr"/>
+      <c r="H137" t="inlineStr"/>
+      <c r="I137" t="inlineStr"/>
+      <c r="J137" t="inlineStr">
+        <is>
+          <t>FV: 6:45 AM MEET BALLARD</t>
+        </is>
+      </c>
+      <c r="K137" t="inlineStr"/>
+      <c r="L137" t="inlineStr"/>
+      <c r="M137" t="inlineStr"/>
+      <c r="N137" t="inlineStr"/>
+      <c r="O137" t="inlineStr"/>
+      <c r="P137" t="inlineStr"/>
+      <c r="Q137" t="inlineStr"/>
+      <c r="R137" t="inlineStr"/>
+      <c r="S137" t="inlineStr"/>
+      <c r="T137" t="inlineStr"/>
+      <c r="U137" t="inlineStr"/>
+      <c r="V137" t="inlineStr"/>
+      <c r="W137" t="inlineStr"/>
+      <c r="X137" t="inlineStr"/>
+      <c r="Y137" t="inlineStr"/>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr"/>
+      <c r="B138" t="inlineStr"/>
+      <c r="C138" t="inlineStr"/>
+      <c r="D138" t="inlineStr"/>
+      <c r="E138" t="inlineStr"/>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>TO FOLLOW</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr"/>
+      <c r="H138" t="inlineStr"/>
+      <c r="I138" t="inlineStr"/>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>8:00 AM START</t>
+        </is>
+      </c>
+      <c r="K138" t="inlineStr"/>
+      <c r="L138" t="inlineStr"/>
+      <c r="M138" t="inlineStr"/>
+      <c r="N138" t="inlineStr"/>
+      <c r="O138" t="inlineStr"/>
+      <c r="P138" t="inlineStr"/>
+      <c r="Q138" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="R138" t="inlineStr">
+        <is>
+          <t>Jeremiah F</t>
+        </is>
+      </c>
+      <c r="S138" t="inlineStr">
+        <is>
+          <t>Driver</t>
+        </is>
+      </c>
+      <c r="T138" t="inlineStr"/>
+      <c r="U138" t="inlineStr"/>
+      <c r="V138" t="inlineStr"/>
+      <c r="W138" t="inlineStr"/>
+      <c r="X138" t="inlineStr"/>
+      <c r="Y138" t="inlineStr"/>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr"/>
+      <c r="B139" t="inlineStr"/>
+      <c r="C139" t="inlineStr"/>
+      <c r="D139" t="inlineStr"/>
+      <c r="E139" t="inlineStr"/>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>MODAS</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr"/>
+      <c r="H139" t="inlineStr"/>
+      <c r="I139" t="inlineStr"/>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>EXCEL FINANCIAL</t>
+        </is>
+      </c>
+      <c r="K139" t="inlineStr"/>
+      <c r="L139" t="inlineStr"/>
+      <c r="M139" t="inlineStr"/>
+      <c r="N139" t="inlineStr"/>
+      <c r="O139" t="inlineStr"/>
+      <c r="P139" t="inlineStr"/>
+      <c r="Q139" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="R139" t="inlineStr">
+        <is>
+          <t>Annette P</t>
+        </is>
+      </c>
+      <c r="S139" t="inlineStr"/>
+      <c r="T139" t="inlineStr"/>
+      <c r="U139" t="inlineStr"/>
+      <c r="V139" t="inlineStr"/>
+      <c r="W139" t="inlineStr"/>
+      <c r="X139" t="inlineStr"/>
+      <c r="Y139" t="inlineStr"/>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr"/>
+      <c r="B140" t="inlineStr"/>
+      <c r="C140" t="inlineStr"/>
+      <c r="D140" t="inlineStr"/>
+      <c r="E140" t="inlineStr"/>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>ONEIDA #2025 ONE STOP PACKERLAND, GREEN BAY</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr"/>
+      <c r="H140" t="inlineStr"/>
+      <c r="I140" t="inlineStr"/>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>GRESHAM TOWNMART</t>
+        </is>
+      </c>
+      <c r="K140" t="inlineStr"/>
+      <c r="L140" t="inlineStr"/>
+      <c r="M140" t="inlineStr"/>
+      <c r="N140" t="inlineStr"/>
+      <c r="O140" t="inlineStr"/>
+      <c r="P140" t="inlineStr"/>
+      <c r="Q140" t="inlineStr">
+        <is>
+          <t>3)</t>
+        </is>
+      </c>
+      <c r="R140" t="inlineStr">
+        <is>
+          <t>Jacqui R</t>
+        </is>
+      </c>
+      <c r="S140" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
+      <c r="T140" t="inlineStr"/>
+      <c r="U140" t="inlineStr"/>
+      <c r="V140" t="inlineStr"/>
+      <c r="W140" t="inlineStr"/>
+      <c r="X140" t="inlineStr"/>
+      <c r="Y140" t="inlineStr"/>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr"/>
+      <c r="B141" t="inlineStr"/>
+      <c r="C141" t="inlineStr"/>
+      <c r="D141" t="inlineStr"/>
+      <c r="E141" t="inlineStr"/>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>3120 PACKERLAND DR</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr"/>
+      <c r="H141" t="inlineStr"/>
+      <c r="I141" t="inlineStr"/>
+      <c r="J141" t="inlineStr">
+        <is>
+          <t>1129 MAIN STREET</t>
+        </is>
+      </c>
+      <c r="K141" t="inlineStr"/>
+      <c r="L141" t="inlineStr"/>
+      <c r="M141" t="inlineStr"/>
+      <c r="N141" t="inlineStr"/>
+      <c r="O141" t="inlineStr"/>
+      <c r="P141" t="inlineStr"/>
+      <c r="Q141" t="inlineStr">
+        <is>
+          <t>4)</t>
+        </is>
+      </c>
+      <c r="R141" t="inlineStr">
+        <is>
+          <t>Michelle C</t>
+        </is>
+      </c>
+      <c r="S141" t="inlineStr">
+        <is>
+          <t>@ Store, work w/ Serena E</t>
+        </is>
+      </c>
+      <c r="T141" t="inlineStr"/>
+      <c r="U141" t="inlineStr"/>
+      <c r="V141" t="inlineStr"/>
+      <c r="W141" t="inlineStr"/>
+      <c r="X141" t="inlineStr"/>
+      <c r="Y141" t="inlineStr"/>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr"/>
+      <c r="B142" t="inlineStr"/>
+      <c r="C142" t="inlineStr"/>
+      <c r="D142" t="inlineStr"/>
+      <c r="E142" t="inlineStr"/>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/ZGaeiY3ZxBS2</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr"/>
+      <c r="H142" t="inlineStr"/>
+      <c r="I142" t="inlineStr"/>
+      <c r="J142" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/Kk6fx4yLi322</t>
+        </is>
+      </c>
+      <c r="K142" t="inlineStr"/>
+      <c r="L142" t="inlineStr"/>
+      <c r="M142" t="inlineStr"/>
+      <c r="N142" t="inlineStr"/>
+      <c r="O142" t="inlineStr"/>
+      <c r="P142" t="inlineStr"/>
+      <c r="Q142" t="inlineStr">
+        <is>
+          <t>5)</t>
+        </is>
+      </c>
+      <c r="R142" t="inlineStr">
+        <is>
+          <t>Serena E</t>
+        </is>
+      </c>
+      <c r="S142" t="inlineStr">
+        <is>
+          <t>3rd Schierl scan, work w/ Michelle C</t>
+        </is>
+      </c>
+      <c r="T142" t="inlineStr"/>
+      <c r="U142" t="inlineStr"/>
+      <c r="V142" t="inlineStr"/>
+      <c r="W142" t="inlineStr"/>
+      <c r="X142" t="inlineStr"/>
+      <c r="Y142" t="inlineStr"/>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr"/>
+      <c r="B143" t="inlineStr"/>
+      <c r="C143" t="inlineStr"/>
+      <c r="D143" t="inlineStr"/>
+      <c r="E143" t="inlineStr"/>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>FULL STORE</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr"/>
+      <c r="H143" t="inlineStr"/>
+      <c r="I143" t="inlineStr"/>
+      <c r="J143" t="inlineStr"/>
+      <c r="K143" t="inlineStr"/>
+      <c r="L143" t="inlineStr"/>
+      <c r="M143" t="inlineStr"/>
+      <c r="N143" t="inlineStr"/>
+      <c r="O143" t="inlineStr"/>
+      <c r="P143" t="inlineStr"/>
+      <c r="Q143" t="inlineStr"/>
+      <c r="R143" t="inlineStr"/>
+      <c r="S143" t="inlineStr"/>
+      <c r="T143" t="inlineStr"/>
+      <c r="U143" t="inlineStr"/>
+      <c r="V143" t="inlineStr"/>
+      <c r="W143" t="inlineStr"/>
+      <c r="X143" t="inlineStr"/>
+      <c r="Y143" t="inlineStr"/>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr"/>
+      <c r="B144" t="inlineStr"/>
+      <c r="C144" t="inlineStr"/>
+      <c r="D144" t="inlineStr"/>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Jerry S</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>Driver</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr"/>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>Jeremiah F</t>
+        </is>
+      </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>Driver, Equip</t>
+        </is>
+      </c>
+      <c r="L144" t="inlineStr"/>
+      <c r="M144" t="inlineStr"/>
+      <c r="N144" t="inlineStr"/>
+      <c r="O144" t="inlineStr"/>
+      <c r="P144" t="inlineStr"/>
+      <c r="Q144" t="inlineStr"/>
+      <c r="R144" t="inlineStr"/>
+      <c r="S144" t="inlineStr"/>
+      <c r="T144" t="inlineStr"/>
+      <c r="U144" t="inlineStr"/>
+      <c r="V144" t="inlineStr"/>
+      <c r="W144" t="inlineStr"/>
+      <c r="X144" t="inlineStr"/>
+      <c r="Y144" t="inlineStr"/>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr"/>
+      <c r="B145" t="inlineStr"/>
+      <c r="C145" t="inlineStr"/>
+      <c r="D145" t="inlineStr"/>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Katie R</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr"/>
+      <c r="H145" t="inlineStr"/>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>Kirsten E</t>
+        </is>
+      </c>
+      <c r="K145" t="inlineStr"/>
+      <c r="L145" t="inlineStr"/>
+      <c r="M145" t="inlineStr"/>
+      <c r="N145" t="inlineStr"/>
+      <c r="O145" t="inlineStr"/>
+      <c r="P145" t="inlineStr"/>
+      <c r="Q145" t="inlineStr"/>
+      <c r="R145" t="inlineStr"/>
+      <c r="S145" t="inlineStr"/>
+      <c r="T145" t="inlineStr"/>
+      <c r="U145" t="inlineStr"/>
+      <c r="V145" t="inlineStr"/>
+      <c r="W145" t="inlineStr"/>
+      <c r="X145" t="inlineStr"/>
+      <c r="Y145" t="inlineStr"/>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr"/>
+      <c r="B146" t="inlineStr"/>
+      <c r="C146" t="inlineStr"/>
+      <c r="D146" t="inlineStr"/>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>3)</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Kirsten E</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr"/>
+      <c r="H146" t="inlineStr"/>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>3)</t>
+        </is>
+      </c>
+      <c r="J146" t="inlineStr">
+        <is>
+          <t>Michelle C</t>
+        </is>
+      </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>@ Store, Until 11:30</t>
+        </is>
+      </c>
+      <c r="L146" t="inlineStr"/>
+      <c r="M146" t="inlineStr"/>
+      <c r="N146" t="inlineStr"/>
+      <c r="O146" t="inlineStr"/>
+      <c r="P146" t="inlineStr"/>
+      <c r="Q146" t="inlineStr"/>
+      <c r="R146" t="inlineStr"/>
+      <c r="S146" t="inlineStr"/>
+      <c r="T146" t="inlineStr"/>
+      <c r="U146" t="inlineStr"/>
+      <c r="V146" t="inlineStr"/>
+      <c r="W146" t="inlineStr"/>
+      <c r="X146" t="inlineStr"/>
+      <c r="Y146" t="inlineStr"/>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr"/>
+      <c r="B147" t="inlineStr"/>
+      <c r="C147" t="inlineStr"/>
+      <c r="D147" t="inlineStr"/>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>4)</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Marcia L</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr"/>
+      <c r="H147" t="inlineStr"/>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>4)</t>
+        </is>
+      </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>Serena E</t>
+        </is>
+      </c>
+      <c r="K147" t="inlineStr"/>
+      <c r="L147" t="inlineStr"/>
+      <c r="M147" t="inlineStr"/>
+      <c r="N147" t="inlineStr"/>
+      <c r="O147" t="inlineStr"/>
+      <c r="P147" t="inlineStr"/>
+      <c r="Q147" t="inlineStr"/>
+      <c r="R147" t="inlineStr"/>
+      <c r="S147" t="inlineStr"/>
+      <c r="T147" t="inlineStr"/>
+      <c r="U147" t="inlineStr"/>
+      <c r="V147" t="inlineStr"/>
+      <c r="W147" t="inlineStr"/>
+      <c r="X147" t="inlineStr"/>
+      <c r="Y147" t="inlineStr"/>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr"/>
+      <c r="B148" t="inlineStr"/>
+      <c r="C148" t="inlineStr"/>
+      <c r="D148" t="inlineStr"/>
+      <c r="E148" t="inlineStr"/>
+      <c r="F148" t="inlineStr"/>
+      <c r="G148" t="inlineStr"/>
+      <c r="H148" t="inlineStr"/>
+      <c r="I148" t="inlineStr"/>
+      <c r="J148" t="inlineStr"/>
+      <c r="K148" t="inlineStr"/>
+      <c r="L148" t="inlineStr"/>
+      <c r="M148" t="inlineStr"/>
+      <c r="N148" t="inlineStr"/>
+      <c r="O148" t="inlineStr"/>
+      <c r="P148" t="inlineStr"/>
+      <c r="Q148" t="inlineStr"/>
+      <c r="R148" t="inlineStr"/>
+      <c r="S148" t="inlineStr"/>
+      <c r="T148" t="inlineStr"/>
+      <c r="U148" t="inlineStr"/>
+      <c r="V148" t="inlineStr"/>
+      <c r="W148" t="inlineStr"/>
+      <c r="X148" t="inlineStr"/>
+      <c r="Y148" t="inlineStr"/>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr"/>
+      <c r="B149" t="inlineStr"/>
+      <c r="C149" t="inlineStr"/>
+      <c r="D149" t="inlineStr"/>
+      <c r="E149" t="inlineStr"/>
+      <c r="F149" t="inlineStr"/>
+      <c r="G149" t="inlineStr"/>
+      <c r="H149" t="inlineStr"/>
+      <c r="I149" t="inlineStr"/>
+      <c r="J149" t="inlineStr"/>
+      <c r="K149" t="inlineStr"/>
+      <c r="L149" t="inlineStr"/>
+      <c r="M149" t="inlineStr"/>
+      <c r="N149" t="inlineStr"/>
+      <c r="O149" t="inlineStr"/>
+      <c r="P149" t="inlineStr"/>
+      <c r="Q149" t="inlineStr"/>
+      <c r="R149" t="inlineStr"/>
+      <c r="S149" t="inlineStr"/>
+      <c r="T149" t="inlineStr"/>
+      <c r="U149" t="inlineStr"/>
+      <c r="V149" t="inlineStr"/>
+      <c r="W149" t="inlineStr"/>
+      <c r="X149" t="inlineStr"/>
+      <c r="Y149" t="inlineStr"/>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr"/>
+      <c r="B150" t="inlineStr"/>
+      <c r="C150" t="inlineStr"/>
+      <c r="D150" t="inlineStr"/>
+      <c r="E150" t="inlineStr"/>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>FV: 5:15 AM MEET BALLARD</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr"/>
+      <c r="H150" t="inlineStr"/>
+      <c r="I150" t="inlineStr"/>
+      <c r="J150" t="inlineStr"/>
+      <c r="K150" t="inlineStr"/>
+      <c r="L150" t="inlineStr"/>
+      <c r="M150" t="inlineStr"/>
+      <c r="N150" t="inlineStr"/>
+      <c r="O150" t="inlineStr"/>
+      <c r="P150" t="inlineStr"/>
+      <c r="Q150" t="inlineStr"/>
+      <c r="R150" t="inlineStr"/>
+      <c r="S150" t="inlineStr"/>
+      <c r="T150" t="inlineStr"/>
+      <c r="U150" t="inlineStr"/>
+      <c r="V150" t="inlineStr"/>
+      <c r="W150" t="inlineStr"/>
+      <c r="X150" t="inlineStr"/>
+      <c r="Y150" t="inlineStr"/>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr"/>
+      <c r="B151" t="inlineStr"/>
+      <c r="C151" t="inlineStr"/>
+      <c r="D151" t="inlineStr"/>
+      <c r="E151" t="inlineStr"/>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>7:00 AM START</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr"/>
+      <c r="H151" t="inlineStr"/>
+      <c r="I151" t="inlineStr"/>
+      <c r="J151" t="inlineStr"/>
+      <c r="K151" t="inlineStr"/>
+      <c r="L151" t="inlineStr"/>
+      <c r="M151" t="inlineStr"/>
+      <c r="N151" t="inlineStr"/>
+      <c r="O151" t="inlineStr"/>
+      <c r="P151" t="inlineStr"/>
+      <c r="Q151" t="inlineStr"/>
+      <c r="R151" t="inlineStr"/>
+      <c r="S151" t="inlineStr"/>
+      <c r="T151" t="inlineStr"/>
+      <c r="U151" t="inlineStr"/>
+      <c r="V151" t="inlineStr"/>
+      <c r="W151" t="inlineStr"/>
+      <c r="X151" t="inlineStr"/>
+      <c r="Y151" t="inlineStr"/>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr"/>
+      <c r="B152" t="inlineStr"/>
+      <c r="C152" t="inlineStr"/>
+      <c r="D152" t="inlineStr"/>
+      <c r="E152" t="inlineStr"/>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>MODAS / WINTAKES</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr"/>
+      <c r="H152" t="inlineStr"/>
+      <c r="I152" t="inlineStr"/>
+      <c r="J152" t="inlineStr"/>
+      <c r="K152" t="inlineStr"/>
+      <c r="L152" t="inlineStr"/>
+      <c r="M152" t="inlineStr"/>
+      <c r="N152" t="inlineStr"/>
+      <c r="O152" t="inlineStr"/>
+      <c r="P152" t="inlineStr"/>
+      <c r="Q152" t="inlineStr"/>
+      <c r="R152" t="inlineStr"/>
+      <c r="S152" t="inlineStr"/>
+      <c r="T152" t="inlineStr"/>
+      <c r="U152" t="inlineStr"/>
+      <c r="V152" t="inlineStr"/>
+      <c r="W152" t="inlineStr"/>
+      <c r="X152" t="inlineStr"/>
+      <c r="Y152" t="inlineStr"/>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr"/>
+      <c r="B153" t="inlineStr"/>
+      <c r="C153" t="inlineStr"/>
+      <c r="D153" t="inlineStr"/>
+      <c r="E153" t="inlineStr"/>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>SCHIERL #82, MARSHFIELD-CENTRAL</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr"/>
+      <c r="H153" t="inlineStr"/>
+      <c r="I153" t="inlineStr"/>
+      <c r="J153" t="inlineStr"/>
+      <c r="K153" t="inlineStr"/>
+      <c r="L153" t="inlineStr"/>
+      <c r="M153" t="inlineStr"/>
+      <c r="N153" t="inlineStr"/>
+      <c r="O153" t="inlineStr"/>
+      <c r="P153" t="inlineStr"/>
+      <c r="Q153" t="inlineStr"/>
+      <c r="R153" t="inlineStr"/>
+      <c r="S153" t="inlineStr"/>
+      <c r="T153" t="inlineStr"/>
+      <c r="U153" t="inlineStr"/>
+      <c r="V153" t="inlineStr"/>
+      <c r="W153" t="inlineStr"/>
+      <c r="X153" t="inlineStr"/>
+      <c r="Y153" t="inlineStr"/>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr"/>
+      <c r="B154" t="inlineStr"/>
+      <c r="C154" t="inlineStr"/>
+      <c r="D154" t="inlineStr"/>
+      <c r="E154" t="inlineStr"/>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>1304 S CENTRAL AVE</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr"/>
+      <c r="H154" t="inlineStr"/>
+      <c r="I154" t="inlineStr"/>
+      <c r="J154" t="inlineStr"/>
+      <c r="K154" t="inlineStr"/>
+      <c r="L154" t="inlineStr"/>
+      <c r="M154" t="inlineStr"/>
+      <c r="N154" t="inlineStr"/>
+      <c r="O154" t="inlineStr"/>
+      <c r="P154" t="inlineStr"/>
+      <c r="Q154" t="inlineStr"/>
+      <c r="R154" t="inlineStr"/>
+      <c r="S154" t="inlineStr"/>
+      <c r="T154" t="inlineStr"/>
+      <c r="U154" t="inlineStr"/>
+      <c r="V154" t="inlineStr"/>
+      <c r="W154" t="inlineStr"/>
+      <c r="X154" t="inlineStr"/>
+      <c r="Y154" t="inlineStr"/>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr"/>
+      <c r="B155" t="inlineStr"/>
+      <c r="C155" t="inlineStr"/>
+      <c r="D155" t="inlineStr"/>
+      <c r="E155" t="inlineStr"/>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/kUJAzqFbdbsVJWbY9</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr"/>
+      <c r="H155" t="inlineStr"/>
+      <c r="I155" t="inlineStr"/>
+      <c r="J155" t="inlineStr"/>
+      <c r="K155" t="inlineStr"/>
+      <c r="L155" t="inlineStr"/>
+      <c r="M155" t="inlineStr"/>
+      <c r="N155" t="inlineStr"/>
+      <c r="O155" t="inlineStr"/>
+      <c r="P155" t="inlineStr"/>
+      <c r="Q155" t="inlineStr"/>
+      <c r="R155" t="inlineStr"/>
+      <c r="S155" t="inlineStr"/>
+      <c r="T155" t="inlineStr"/>
+      <c r="U155" t="inlineStr"/>
+      <c r="V155" t="inlineStr"/>
+      <c r="W155" t="inlineStr"/>
+      <c r="X155" t="inlineStr"/>
+      <c r="Y155" t="inlineStr"/>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr"/>
+      <c r="B156" t="inlineStr"/>
+      <c r="C156" t="inlineStr"/>
+      <c r="D156" t="inlineStr"/>
+      <c r="E156" t="inlineStr"/>
+      <c r="F156" t="inlineStr"/>
+      <c r="G156" t="inlineStr"/>
+      <c r="H156" t="inlineStr"/>
+      <c r="I156" t="inlineStr"/>
+      <c r="J156" t="inlineStr"/>
+      <c r="K156" t="inlineStr"/>
+      <c r="L156" t="inlineStr"/>
+      <c r="M156" t="inlineStr"/>
+      <c r="N156" t="inlineStr"/>
+      <c r="O156" t="inlineStr"/>
+      <c r="P156" t="inlineStr"/>
+      <c r="Q156" t="inlineStr"/>
+      <c r="R156" t="inlineStr"/>
+      <c r="S156" t="inlineStr"/>
+      <c r="T156" t="inlineStr"/>
+      <c r="U156" t="inlineStr"/>
+      <c r="V156" t="inlineStr"/>
+      <c r="W156" t="inlineStr"/>
+      <c r="X156" t="inlineStr"/>
+      <c r="Y156" t="inlineStr"/>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr"/>
+      <c r="B157" t="inlineStr"/>
+      <c r="C157" t="inlineStr"/>
+      <c r="D157" t="inlineStr"/>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>Jeremiah F</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>Driver</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr"/>
+      <c r="I157" t="inlineStr"/>
+      <c r="J157" t="inlineStr"/>
+      <c r="K157" t="inlineStr"/>
+      <c r="L157" t="inlineStr"/>
+      <c r="M157" t="inlineStr"/>
+      <c r="N157" t="inlineStr"/>
+      <c r="O157" t="inlineStr"/>
+      <c r="P157" t="inlineStr"/>
+      <c r="Q157" t="inlineStr"/>
+      <c r="R157" t="inlineStr"/>
+      <c r="S157" t="inlineStr"/>
+      <c r="T157" t="inlineStr"/>
+      <c r="U157" t="inlineStr"/>
+      <c r="V157" t="inlineStr"/>
+      <c r="W157" t="inlineStr"/>
+      <c r="X157" t="inlineStr"/>
+      <c r="Y157" t="inlineStr"/>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr"/>
+      <c r="B158" t="inlineStr"/>
+      <c r="C158" t="inlineStr"/>
+      <c r="D158" t="inlineStr"/>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Heather V</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr"/>
+      <c r="H158" t="inlineStr"/>
+      <c r="I158" t="inlineStr"/>
+      <c r="J158" t="inlineStr"/>
+      <c r="K158" t="inlineStr"/>
+      <c r="L158" t="inlineStr"/>
+      <c r="M158" t="inlineStr"/>
+      <c r="N158" t="inlineStr"/>
+      <c r="O158" t="inlineStr"/>
+      <c r="P158" t="inlineStr"/>
+      <c r="Q158" t="inlineStr"/>
+      <c r="R158" t="inlineStr"/>
+      <c r="S158" t="inlineStr"/>
+      <c r="T158" t="inlineStr"/>
+      <c r="U158" t="inlineStr"/>
+      <c r="V158" t="inlineStr"/>
+      <c r="W158" t="inlineStr"/>
+      <c r="X158" t="inlineStr"/>
+      <c r="Y158" t="inlineStr"/>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr"/>
+      <c r="B159" t="inlineStr"/>
+      <c r="C159" t="inlineStr"/>
+      <c r="D159" t="inlineStr"/>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>3)</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Michelle C</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>@ Store, work w/ Michelle C</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr"/>
+      <c r="I159" t="inlineStr"/>
+      <c r="J159" t="inlineStr"/>
+      <c r="K159" t="inlineStr"/>
+      <c r="L159" t="inlineStr"/>
+      <c r="M159" t="inlineStr"/>
+      <c r="N159" t="inlineStr"/>
+      <c r="O159" t="inlineStr"/>
+      <c r="P159" t="inlineStr"/>
+      <c r="Q159" t="inlineStr"/>
+      <c r="R159" t="inlineStr"/>
+      <c r="S159" t="inlineStr"/>
+      <c r="T159" t="inlineStr"/>
+      <c r="U159" t="inlineStr"/>
+      <c r="V159" t="inlineStr"/>
+      <c r="W159" t="inlineStr"/>
+      <c r="X159" t="inlineStr"/>
+      <c r="Y159" t="inlineStr"/>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr"/>
+      <c r="B160" t="inlineStr"/>
+      <c r="C160" t="inlineStr"/>
+      <c r="D160" t="inlineStr"/>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>4)</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Serena E</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>2nd Schierl scan, work w/ Michelle C</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr"/>
+      <c r="I160" t="inlineStr"/>
+      <c r="J160" t="inlineStr"/>
+      <c r="K160" t="inlineStr"/>
+      <c r="L160" t="inlineStr"/>
+      <c r="M160" t="inlineStr"/>
+      <c r="N160" t="inlineStr"/>
+      <c r="O160" t="inlineStr"/>
+      <c r="P160" t="inlineStr"/>
+      <c r="Q160" t="inlineStr"/>
+      <c r="R160" t="inlineStr"/>
+      <c r="S160" t="inlineStr"/>
+      <c r="T160" t="inlineStr"/>
+      <c r="U160" t="inlineStr"/>
+      <c r="V160" t="inlineStr"/>
+      <c r="W160" t="inlineStr"/>
+      <c r="X160" t="inlineStr"/>
+      <c r="Y160" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
adjust for office days
</commit_message>
<xml_diff>
--- a/Copy of 06-23-24 to 06-29-24 Full Shedule.xlsx
+++ b/Copy of 06-23-24 to 06-29-24 Full Shedule.xlsx
@@ -1021,7 +1021,7 @@
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>DJ S</t>
+          <t>DJ</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>DJ S</t>
+          <t>DJ</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
@@ -4154,7 +4154,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>DJ S</t>
+          <t>DJ</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">

</xml_diff>